<commit_message>
reactive plot back up
</commit_message>
<xml_diff>
--- a/app/data/wto_proposal_settings_master.xlsx
+++ b/app/data/wto_proposal_settings_master.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kat/GitHub/SubsidyExplorer/app/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kat/GitHub/SubsidyExplorer/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6804A9-2CBF-3F43-B9D0-2F52ECE17A1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609F0BCB-FB33-2840-83B4-E450DBB0A1A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20460" yWindow="1980" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="1" r:id="rId1"/>
     <sheet name="old" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="387">
   <si>
     <t>proposal</t>
   </si>
@@ -1359,13 +1359,145 @@
     <t>The EU is including here the concept of determination of Port state and market state. I imagine that in these cases the same assumptions from determination by coastal, flag and subsidizing members could apply. KAT ADDED.</t>
   </si>
   <si>
-    <t>KAT ADDED</t>
-  </si>
-  <si>
-    <t>other_definitions</t>
-  </si>
-  <si>
     <t>DISPUTE</t>
+  </si>
+  <si>
+    <t>iuu_sdt_ldc</t>
+  </si>
+  <si>
+    <t>iuu_sdt_what_ldc</t>
+  </si>
+  <si>
+    <t>iuu_sdt_time_delay_ldc</t>
+  </si>
+  <si>
+    <t>iuu_sdt_developing</t>
+  </si>
+  <si>
+    <t>iuu_sdt_what_developing</t>
+  </si>
+  <si>
+    <t>iuu_sdt_time_delay_developing</t>
+  </si>
+  <si>
+    <t>iuu_sdt_sve</t>
+  </si>
+  <si>
+    <t>iuu_sdt_what_sve</t>
+  </si>
+  <si>
+    <t>iuu_sdt_time_delay_sve</t>
+  </si>
+  <si>
+    <t>oa_tonnage_cutoff</t>
+  </si>
+  <si>
+    <t>oa_engine_cutoff</t>
+  </si>
+  <si>
+    <t>oa_sdt_ldc</t>
+  </si>
+  <si>
+    <t>oa_sdt_what_ldc</t>
+  </si>
+  <si>
+    <t>oa_sdt_hs_cutoff_ldc</t>
+  </si>
+  <si>
+    <t>oa_sdt_time_delay_ldc</t>
+  </si>
+  <si>
+    <t>oa_sdt_developing</t>
+  </si>
+  <si>
+    <t>oa_sdt_what_developing</t>
+  </si>
+  <si>
+    <t>oa_sdt_hs_cutoff_developing</t>
+  </si>
+  <si>
+    <t>oa_sdt_time_delay_developing</t>
+  </si>
+  <si>
+    <t>oa_sdt_sve</t>
+  </si>
+  <si>
+    <t>oa_sdt_what_sve</t>
+  </si>
+  <si>
+    <t>oa_sdt_hs_cutoff_sve</t>
+  </si>
+  <si>
+    <t>oa_sdt_time_delay_sve</t>
+  </si>
+  <si>
+    <t>overcap_tonnage_cutoff</t>
+  </si>
+  <si>
+    <t>overcap_engine_cutoff</t>
+  </si>
+  <si>
+    <t>overcap_sdt_ldc</t>
+  </si>
+  <si>
+    <t>overcap_sdt_what_ldc</t>
+  </si>
+  <si>
+    <t>overcap_sdt_hs_cutoff_ldc</t>
+  </si>
+  <si>
+    <t>overcap_sdt_time_delay_ldc</t>
+  </si>
+  <si>
+    <t>overcap_sdt_developing</t>
+  </si>
+  <si>
+    <t>overcap_sdt_what_developing</t>
+  </si>
+  <si>
+    <t>overcap_sdt_hs_cutoff_developing</t>
+  </si>
+  <si>
+    <t>overcap_sdt_time_delay_developing</t>
+  </si>
+  <si>
+    <t>overcap_sdt_sve</t>
+  </si>
+  <si>
+    <t>overcap_sdt_what_sve</t>
+  </si>
+  <si>
+    <t>overcap_sdt_hs_cutoff_sve</t>
+  </si>
+  <si>
+    <t>overcap_sdt_time_delay_sve</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>THREE</t>
+  </si>
+  <si>
+    <t>CAPTURE</t>
+  </si>
+  <si>
+    <t>PERCENT_SUBS</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>IUU1, IUU2, IUU3, IUU4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added in the dispute option. Treating this sorta as an overcapacity issue. </t>
   </si>
 </sst>
 </file>
@@ -1891,7 +2023,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1967,6 +2099,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2323,11 +2458,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BI25"/>
+  <dimension ref="A1:CH25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -2346,7 +2481,7 @@
     <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="13" customFormat="1" ht="51">
+    <row r="1" spans="1:86" s="13" customFormat="1" ht="68">
       <c r="A1" s="13" t="s">
         <v>144</v>
       </c>
@@ -2405,133 +2540,208 @@
         <v>12</v>
       </c>
       <c r="T1" s="13" t="s">
-        <v>13</v>
+        <v>341</v>
       </c>
       <c r="U1" s="13" t="s">
-        <v>14</v>
+        <v>342</v>
       </c>
       <c r="V1" s="13" t="s">
-        <v>15</v>
+        <v>343</v>
       </c>
       <c r="W1" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="X1" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="Y1" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="Z1" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="AA1" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="AB1" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="AC1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="AD1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="AE1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="AF1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AG1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="AB1" s="13" t="s">
+      <c r="AH1" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="AI1" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="AJ1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="AC1" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD1" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE1" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="AF1" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="AG1" s="13" t="s">
+      <c r="AK1" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="AL1" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="AM1" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="AN1" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="AO1" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="AP1" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="AQ1" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="AR1" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="AS1" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="AT1" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="AU1" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="AV1" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="AW1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="AH1" s="13" t="s">
+      <c r="AX1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="AI1" s="13" t="s">
+      <c r="AY1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="AJ1" s="13" t="s">
+      <c r="AZ1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AK1" s="13" t="s">
+      <c r="BA1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="AL1" s="13" t="s">
+      <c r="BB1" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="BC1" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="BD1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="AM1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AN1" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AO1" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="AP1" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="AQ1" s="13" t="s">
+      <c r="BE1" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="BF1" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="BG1" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="BH1" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="BI1" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="BJ1" s="13" t="s">
+        <v>371</v>
+      </c>
+      <c r="BK1" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="BL1" s="13" t="s">
+        <v>373</v>
+      </c>
+      <c r="BM1" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="BN1" s="13" t="s">
+        <v>375</v>
+      </c>
+      <c r="BO1" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="BP1" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="BQ1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="AR1" s="13" t="s">
+      <c r="BR1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="AS1" s="13" t="s">
+      <c r="BS1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="AT1" s="13" t="s">
+      <c r="BT1" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="AU1" s="13" t="s">
+      <c r="BU1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="AV1" s="13" t="s">
+      <c r="BV1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AW1" s="13" t="s">
+      <c r="BW1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" s="13" t="s">
+      <c r="BX1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="AY1" s="13" t="s">
+      <c r="BY1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="AZ1" s="13" t="s">
+      <c r="BZ1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="BA1" s="13" t="s">
+      <c r="CA1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="BB1" s="13" t="s">
+      <c r="CB1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="BC1" s="13" t="s">
+      <c r="CC1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="BD1" s="13" t="s">
+      <c r="CD1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="BE1" s="13" t="s">
+      <c r="CE1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="BF1" s="13" t="s">
+      <c r="CF1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="BG1" s="13" t="s">
+      <c r="CG1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="BH1" s="13" t="s">
+      <c r="CH1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="BI1" s="13" t="s">
-        <v>341</v>
-      </c>
     </row>
-    <row r="2" spans="1:61" s="13" customFormat="1" ht="282" customHeight="1">
+    <row r="2" spans="1:86" s="13" customFormat="1" ht="282" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>58</v>
       </c>
@@ -2571,8 +2781,14 @@
       <c r="M2" s="21" t="s">
         <v>313</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>379</v>
+      </c>
     </row>
-    <row r="3" spans="1:61" ht="136">
+    <row r="3" spans="1:86" ht="136">
       <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
@@ -2580,7 +2796,7 @@
         <v>89</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>340</v>
+        <v>386</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>85</v>
@@ -2612,11 +2828,17 @@
       <c r="M3" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="BI3" s="1" t="s">
-        <v>342</v>
+      <c r="AW3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="BD3" s="1" t="s">
+        <v>379</v>
       </c>
     </row>
-    <row r="4" spans="1:61" ht="170">
+    <row r="4" spans="1:86" ht="170">
       <c r="A4" s="1" t="s">
         <v>58</v>
       </c>
@@ -2654,16 +2876,19 @@
         <v>295</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>151</v>
+        <v>385</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>55</v>
+        <v>379</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>378</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>55</v>
+        <v>379</v>
       </c>
     </row>
-    <row r="5" spans="1:61" ht="119">
+    <row r="5" spans="1:86" ht="119">
       <c r="A5" s="25" t="s">
         <v>58</v>
       </c>
@@ -2707,13 +2932,16 @@
         <v>338</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>55</v>
+        <v>379</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>378</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>55</v>
+        <v>379</v>
       </c>
     </row>
-    <row r="6" spans="1:61" ht="136">
+    <row r="6" spans="1:86" ht="136">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -2763,7 +2991,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:61" ht="221">
+    <row r="7" spans="1:86" ht="221">
       <c r="A7" s="1" t="s">
         <v>58</v>
       </c>
@@ -2810,7 +3038,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:61" ht="272">
+    <row r="8" spans="1:86" ht="272">
       <c r="A8" s="1" t="s">
         <v>58</v>
       </c>
@@ -2847,38 +3075,38 @@
       <c r="M8" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="AQ8" s="1" t="s">
+      <c r="BQ8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AR8" s="1" t="s">
+      <c r="BR8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AS8" s="1" t="s">
+      <c r="BS8" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AT8" s="1" t="s">
+      <c r="BT8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AV8" s="1" t="s">
+      <c r="BV8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AW8" s="1" t="s">
+      <c r="BW8" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AZ8" s="1">
+      <c r="BZ8" s="1">
         <v>90</v>
       </c>
-      <c r="BA8" s="1" t="s">
+      <c r="CA8" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB8" s="1">
+      <c r="CB8" s="1">
         <v>50</v>
       </c>
-      <c r="BE8" s="1" t="s">
+      <c r="CE8" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:61" ht="323">
+    <row r="9" spans="1:86" ht="323">
       <c r="A9" s="1" t="s">
         <v>58</v>
       </c>
@@ -2918,26 +3146,26 @@
       <c r="M9" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="AQ9" s="1" t="s">
+      <c r="BQ9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AR9" s="1" t="s">
+      <c r="BR9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AS9" s="1" t="s">
+      <c r="BS9" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AW9" s="1" t="s">
+      <c r="BW9" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AY9" s="1">
+      <c r="BY9" s="1">
         <v>800</v>
       </c>
-      <c r="AZ9" s="1">
+      <c r="BZ9" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:61" ht="388">
+    <row r="10" spans="1:86" ht="388">
       <c r="A10" s="1" t="s">
         <v>58</v>
       </c>
@@ -2978,7 +3206,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="11" spans="1:61" ht="85">
+    <row r="11" spans="1:86" ht="85">
       <c r="A11" s="1" t="s">
         <v>55</v>
       </c>
@@ -3013,7 +3241,7 @@
       <c r="L11" s="8"/>
       <c r="M11" s="9"/>
     </row>
-    <row r="12" spans="1:61" ht="238">
+    <row r="12" spans="1:86" ht="238">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -3051,7 +3279,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="13" spans="1:61" ht="136.5" customHeight="1">
+    <row r="13" spans="1:86" ht="136.5" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
@@ -3091,20 +3319,20 @@
       <c r="M13" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="AG13" s="1" t="s">
+      <c r="AW13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AH13" s="1" t="s">
+      <c r="AX13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AJ13" s="1">
+      <c r="AZ13" s="1">
         <v>5</v>
       </c>
-      <c r="AL13" s="1" t="s">
+      <c r="BD13" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:61" ht="187">
+    <row r="14" spans="1:86" ht="187">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -3144,20 +3372,20 @@
       <c r="M14" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="AG14" s="1" t="s">
+      <c r="AW14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AH14" s="1" t="s">
+      <c r="AX14" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="AK14" s="1">
+      <c r="BA14" s="1">
         <v>24</v>
       </c>
-      <c r="AL14" s="1" t="s">
+      <c r="BD14" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:61" ht="238">
+    <row r="15" spans="1:86" ht="238">
       <c r="A15" s="1" t="s">
         <v>58</v>
       </c>
@@ -3198,7 +3426,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="16" spans="1:61" ht="238">
+    <row r="16" spans="1:86" ht="238">
       <c r="A16" s="1" t="s">
         <v>58</v>
       </c>
@@ -3238,23 +3466,35 @@
       <c r="M16" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="AG16" s="1" t="s">
+      <c r="AW16" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AH16" s="1" t="s">
+      <c r="AX16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AL16" s="1" t="s">
+      <c r="BD16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AM16" s="1" t="s">
+      <c r="BE16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AN16" s="1" t="s">
+      <c r="BF16" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="BI16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BJ16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BM16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BN16" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="17" spans="1:60" ht="136">
+    <row r="17" spans="1:86" ht="136">
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
@@ -3292,7 +3532,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="18" spans="1:60" ht="289">
+    <row r="18" spans="1:86" ht="289">
       <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
@@ -3333,7 +3573,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="19" spans="1:60" ht="136">
+    <row r="19" spans="1:86" ht="136">
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
@@ -3370,7 +3610,7 @@
       <c r="L19" s="8"/>
       <c r="M19" s="9"/>
     </row>
-    <row r="20" spans="1:60" ht="340">
+    <row r="20" spans="1:86" ht="340">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
@@ -3410,17 +3650,17 @@
       <c r="M20" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="W20" s="1" t="s">
+      <c r="AC20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="X20" s="1" t="s">
+      <c r="AD20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AB20" s="1" t="s">
+      <c r="AJ20" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:60" ht="204">
+    <row r="21" spans="1:86" ht="204">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
@@ -3460,17 +3700,17 @@
       <c r="M21" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="W21" s="1" t="s">
+      <c r="AC21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="X21" s="1" t="s">
+      <c r="AD21" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AB21" s="1" t="s">
+      <c r="AJ21" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:60" ht="204">
+    <row r="22" spans="1:86" ht="204">
       <c r="A22" s="1" t="s">
         <v>58</v>
       </c>
@@ -3510,17 +3750,17 @@
       <c r="M22" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="W22" s="1" t="s">
+      <c r="AC22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="X22" s="1" t="s">
+      <c r="AD22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AB22" s="1" t="s">
+      <c r="AJ22" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:60" ht="68">
+    <row r="23" spans="1:86" ht="68">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
@@ -3555,7 +3795,7 @@
       <c r="L23" s="8"/>
       <c r="M23" s="9"/>
     </row>
-    <row r="24" spans="1:60" ht="182.25" customHeight="1">
+    <row r="24" spans="1:86" ht="182.25" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>58</v>
       </c>
@@ -3596,7 +3836,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="25" spans="1:60" ht="51">
+    <row r="25" spans="1:86" ht="51">
       <c r="B25" s="3" t="s">
         <v>83</v>
       </c>
@@ -3610,117 +3850,177 @@
       <c r="L25" s="8"/>
       <c r="M25" s="9"/>
       <c r="O25" s="1" t="s">
-        <v>55</v>
+        <v>379</v>
       </c>
       <c r="P25" s="1">
         <v>20</v>
       </c>
-      <c r="Q25" s="1" t="s">
-        <v>57</v>
+      <c r="Q25" s="26" t="s">
+        <v>378</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>55</v>
+        <v>379</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>65</v>
+        <v>379</v>
       </c>
       <c r="V25" s="1">
-        <v>1</v>
-      </c>
-      <c r="X25" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z25" s="1">
         <v>5</v>
       </c>
-      <c r="AA25" s="1">
+      <c r="W25" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z25" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD25" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="AF25" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG25" s="1">
         <v>24</v>
       </c>
-      <c r="AB25" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE25" s="1">
+      <c r="AH25" s="1">
+        <v>100</v>
+      </c>
+      <c r="AI25" s="1">
+        <v>400</v>
+      </c>
+      <c r="AJ25" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="AK25" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="AM25" s="1">
         <v>5</v>
       </c>
-      <c r="AF25" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH25" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AJ25" s="1">
+      <c r="AN25" s="1">
         <v>5</v>
       </c>
-      <c r="AK25" s="1">
-        <v>24</v>
-      </c>
-      <c r="AL25" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AM25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AO25" s="1">
+      <c r="AO25" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="AQ25" s="1">
         <v>5</v>
       </c>
-      <c r="AP25" s="1">
-        <v>1</v>
-      </c>
-      <c r="AQ25" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AR25" s="1" t="s">
-        <v>61</v>
+      <c r="AR25" s="1">
+        <v>5</v>
       </c>
       <c r="AS25" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AT25" s="1" t="s">
-        <v>72</v>
+        <v>379</v>
       </c>
       <c r="AU25" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="AV25" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AW25" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AX25" s="1">
         <v>5</v>
       </c>
-      <c r="AY25" s="1">
-        <v>800</v>
+      <c r="AV25" s="1">
+        <v>5</v>
+      </c>
+      <c r="AX25" s="1" t="s">
+        <v>378</v>
       </c>
       <c r="AZ25" s="1">
         <v>5</v>
       </c>
-      <c r="BA25" s="1" t="s">
-        <v>75</v>
+      <c r="BA25" s="1">
+        <v>24</v>
       </c>
       <c r="BB25" s="1">
+        <v>100</v>
+      </c>
+      <c r="BC25" s="1">
+        <v>400</v>
+      </c>
+      <c r="BD25" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="BE25" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="BG25" s="1">
         <v>5</v>
       </c>
-      <c r="BC25" s="1">
+      <c r="BH25" s="1">
+        <v>5</v>
+      </c>
+      <c r="BI25" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="BK25" s="1">
+        <v>5</v>
+      </c>
+      <c r="BL25" s="1">
+        <v>5</v>
+      </c>
+      <c r="BM25" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="BO25" s="1">
+        <v>5</v>
+      </c>
+      <c r="BP25" s="1">
+        <v>5</v>
+      </c>
+      <c r="BQ25" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="BR25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BS25" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="BT25" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="BU25" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="BV25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BW25" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="BX25" s="1">
+        <v>5</v>
+      </c>
+      <c r="BY25" s="1">
         <v>800</v>
       </c>
-      <c r="BD25" s="1">
+      <c r="BZ25" s="1">
         <v>5</v>
       </c>
-      <c r="BE25" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="BF25" s="1">
+      <c r="CA25" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="CB25" s="1">
         <v>5</v>
       </c>
-      <c r="BG25" s="1">
+      <c r="CC25" s="1">
         <v>800</v>
       </c>
-      <c r="BH25" s="1">
+      <c r="CD25" s="1">
+        <v>5</v>
+      </c>
+      <c r="CE25" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="CF25" s="1">
+        <v>5</v>
+      </c>
+      <c r="CG25" s="1">
+        <v>800</v>
+      </c>
+      <c r="CH25" s="1">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
two part reactive container up
</commit_message>
<xml_diff>
--- a/app/data/wto_proposal_settings_master.xlsx
+++ b/app/data/wto_proposal_settings_master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kat/GitHub/SubsidyExplorer/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609F0BCB-FB33-2840-83B4-E450DBB0A1A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216DED76-F5DA-6843-A47C-B18A99D15E3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="391">
   <si>
     <t>proposal</t>
   </si>
@@ -462,9 +462,6 @@
   </si>
   <si>
     <t>notes</t>
-  </si>
-  <si>
-    <t>iuu1, iuu2</t>
   </si>
   <si>
     <t>Draft text on IUU fisheries subsidies</t>
@@ -1157,31 +1154,6 @@
     <t>TN/RL/GEN/200/Rev1</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Scope: 1) Exclusion of territorial waters for all members. Is not possible to make the distinction between territorial water's and the remainder of an EEZ in the tool's dataset, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>the assumtion is that is applied to all EEZ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. On IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, and coastal Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal Member. The possible effects is a conservative interpretation of this text. 3) No proportionality or the duration of prohibition is considered. On Overfished: 1) There is uncertainty  regarding the status of many fish stocks. 2) To model the proposal we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 0.8) in the RAM Legacy stock assessment database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy stock assessment database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. OFOC: 1) Prohibition of subsidies to large scale and in the high seas. General Transition period: 1) for implementation to LDC and developing countries</t>
-    </r>
-  </si>
-  <si>
     <t>LDC new proposal includes 3 pillars of prohibiion (IUU, Overfished and OFOC) and S&amp;DT. We might need to consider a new section or include it in Other. I don't think we would like to separate or divide the proposal as we would like to see the effect of the proposal as a whole.</t>
   </si>
   <si>
@@ -1498,6 +1470,46 @@
   </si>
   <si>
     <t xml:space="preserve">Added in the dispute option. Treating this sorta as an overcapacity issue. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Scope: 1) Exclusion of territorial waters for all members. Is not possible to make the distinction between territorial water's and the remainder of an EEZ in the tool's dataset, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the assumtion is that is applied to all EEZ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. On IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, and coastal Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal Member. The possible effects is a conservative interpretation of this text. 3) No proportionality or the duration of prohibition is considered. On Overfished: 1) There is uncertainty  regarding the status of many fish stocks. 2) To model the proposal we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy stock assessment database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy stock assessment database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. OFOC: 1) Prohibition of subsidies to large scale and in the high seas. General Transition period: 1) for implementation to LDC and developing countries</t>
+    </r>
+  </si>
+  <si>
+    <t>OA2</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>TIME, ALL</t>
   </si>
 </sst>
 </file>
@@ -2460,9 +2472,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CH25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -2495,7 +2507,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>1</v>
@@ -2504,7 +2516,7 @@
         <v>130</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>2</v>
@@ -2519,7 +2531,7 @@
         <v>5</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="N1" s="13" t="s">
         <v>7</v>
@@ -2540,31 +2552,31 @@
         <v>12</v>
       </c>
       <c r="T1" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="V1" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="W1" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="X1" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="Y1" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="Z1" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="AA1" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="AB1" s="13" t="s">
         <v>347</v>
-      </c>
-      <c r="AA1" s="13" t="s">
-        <v>348</v>
-      </c>
-      <c r="AB1" s="13" t="s">
-        <v>349</v>
       </c>
       <c r="AC1" s="13" t="s">
         <v>16</v>
@@ -2582,49 +2594,49 @@
         <v>20</v>
       </c>
       <c r="AH1" s="13" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AI1" s="13" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="AJ1" s="13" t="s">
         <v>21</v>
       </c>
       <c r="AK1" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="AL1" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="AM1" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="AL1" s="13" t="s">
+      <c r="AN1" s="13" t="s">
         <v>353</v>
       </c>
-      <c r="AM1" s="13" t="s">
+      <c r="AO1" s="13" t="s">
         <v>354</v>
       </c>
-      <c r="AN1" s="13" t="s">
+      <c r="AP1" s="13" t="s">
         <v>355</v>
       </c>
-      <c r="AO1" s="13" t="s">
+      <c r="AQ1" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="AP1" s="13" t="s">
+      <c r="AR1" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="AQ1" s="13" t="s">
+      <c r="AS1" s="13" t="s">
         <v>358</v>
       </c>
-      <c r="AR1" s="13" t="s">
+      <c r="AT1" s="13" t="s">
         <v>359</v>
       </c>
-      <c r="AS1" s="13" t="s">
+      <c r="AU1" s="13" t="s">
         <v>360</v>
       </c>
-      <c r="AT1" s="13" t="s">
+      <c r="AV1" s="13" t="s">
         <v>361</v>
-      </c>
-      <c r="AU1" s="13" t="s">
-        <v>362</v>
-      </c>
-      <c r="AV1" s="13" t="s">
-        <v>363</v>
       </c>
       <c r="AW1" s="13" t="s">
         <v>26</v>
@@ -2642,49 +2654,49 @@
         <v>30</v>
       </c>
       <c r="BB1" s="13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="BC1" s="13" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="BD1" s="13" t="s">
         <v>31</v>
       </c>
       <c r="BE1" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="BF1" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="BG1" s="13" t="s">
         <v>366</v>
       </c>
-      <c r="BF1" s="13" t="s">
+      <c r="BH1" s="13" t="s">
         <v>367</v>
       </c>
-      <c r="BG1" s="13" t="s">
+      <c r="BI1" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="BH1" s="13" t="s">
+      <c r="BJ1" s="13" t="s">
         <v>369</v>
       </c>
-      <c r="BI1" s="13" t="s">
+      <c r="BK1" s="13" t="s">
         <v>370</v>
       </c>
-      <c r="BJ1" s="13" t="s">
+      <c r="BL1" s="13" t="s">
         <v>371</v>
       </c>
-      <c r="BK1" s="13" t="s">
+      <c r="BM1" s="13" t="s">
         <v>372</v>
       </c>
-      <c r="BL1" s="13" t="s">
+      <c r="BN1" s="13" t="s">
         <v>373</v>
       </c>
-      <c r="BM1" s="13" t="s">
+      <c r="BO1" s="13" t="s">
         <v>374</v>
       </c>
-      <c r="BN1" s="13" t="s">
+      <c r="BP1" s="13" t="s">
         <v>375</v>
-      </c>
-      <c r="BO1" s="13" t="s">
-        <v>376</v>
-      </c>
-      <c r="BP1" s="13" t="s">
-        <v>377</v>
       </c>
       <c r="BQ1" s="13" t="s">
         <v>36</v>
@@ -2749,43 +2761,115 @@
         <v>89</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D2" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>305</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>306</v>
       </c>
       <c r="G2" s="18">
         <v>43896</v>
       </c>
       <c r="H2" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="K2" s="19" t="s">
         <v>309</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="L2" s="20" t="s">
         <v>310</v>
       </c>
-      <c r="L2" s="20" t="s">
-        <v>311</v>
-      </c>
       <c r="M2" s="21" t="s">
-        <v>313</v>
+        <v>385</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>379</v>
+        <v>377</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="AC2" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="AD2" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="AJ2" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="AK2" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="AL2" s="13" t="s">
+        <v>388</v>
+      </c>
+      <c r="AN2" s="13">
+        <v>5</v>
+      </c>
+      <c r="AO2" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="AP2" s="13" t="s">
+        <v>388</v>
+      </c>
+      <c r="AR2" s="13">
+        <v>3</v>
+      </c>
+      <c r="AS2" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AX2" s="13" t="s">
+        <v>389</v>
+      </c>
+      <c r="AZ2" s="13">
+        <v>5</v>
+      </c>
+      <c r="BA2" s="13">
+        <v>24</v>
+      </c>
+      <c r="BD2" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="BE2" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="BF2" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="BH2" s="13">
+        <v>5</v>
+      </c>
+      <c r="BI2" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="BJ2" s="13" t="s">
+        <v>388</v>
+      </c>
+      <c r="BL2" s="13">
+        <v>3</v>
+      </c>
+      <c r="BM2" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="BQ2" s="13" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="3" spans="1:86" ht="136">
@@ -2796,7 +2880,7 @@
         <v>89</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>85</v>
@@ -2811,7 +2895,7 @@
         <v>43759</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>86</v>
@@ -2820,22 +2904,22 @@
         <v>87</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>55</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="AW3" s="1" t="s">
         <v>61</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="BD3" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="4" spans="1:86" ht="170">
@@ -2858,7 +2942,7 @@
         <v>43801</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>92</v>
@@ -2867,25 +2951,25 @@
         <v>93</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>55</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5" spans="1:86" ht="119">
@@ -2896,7 +2980,7 @@
         <v>90</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>94</v>
@@ -2911,7 +2995,7 @@
         <v>43718</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>95</v>
@@ -2920,25 +3004,25 @@
         <v>96</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L5" s="24" t="s">
         <v>55</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="6" spans="1:86" ht="136">
@@ -2949,10 +3033,10 @@
         <v>90</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>55</v>
@@ -2964,7 +3048,7 @@
         <v>43865</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>145</v>
@@ -2973,22 +3057,46 @@
         <v>117</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="L6" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="L6" s="8" t="s">
-        <v>260</v>
-      </c>
       <c r="M6" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>147</v>
+        <v>383</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>55</v>
+        <v>377</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>376</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>55</v>
+        <v>387</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="V6" s="1">
+        <v>5</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="7" spans="1:86" ht="221">
@@ -3005,31 +3113,31 @@
         <v>55</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G7" s="2">
         <v>43628</v>
       </c>
       <c r="H7" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="L7" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>55</v>
@@ -3058,7 +3166,7 @@
         <v>43657</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>70</v>
@@ -3067,13 +3175,13 @@
         <v>129</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M8" s="9" t="s">
         <v>152</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>153</v>
       </c>
       <c r="BQ8" s="1" t="s">
         <v>58</v>
@@ -3114,7 +3222,7 @@
         <v>99</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>77</v>
@@ -3129,7 +3237,7 @@
         <v>43620</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>78</v>
@@ -3138,13 +3246,13 @@
         <v>79</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>55</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="BQ9" s="1" t="s">
         <v>58</v>
@@ -3173,7 +3281,7 @@
         <v>99</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>100</v>
@@ -3188,22 +3296,22 @@
         <v>43545</v>
       </c>
       <c r="H10" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>280</v>
-      </c>
       <c r="M10" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:86" ht="85">
@@ -3214,7 +3322,7 @@
         <v>99</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>101</v>
@@ -3230,13 +3338,13 @@
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="K11" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L11" s="8"/>
       <c r="M11" s="9"/>
@@ -3249,34 +3357,34 @@
         <v>99</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G12" s="2">
         <v>43843</v>
       </c>
       <c r="H12" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="K12" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="K12" s="6" t="s">
-        <v>293</v>
-      </c>
       <c r="L12" s="7" t="s">
         <v>55</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:86" ht="136.5" customHeight="1">
@@ -3287,7 +3395,7 @@
         <v>99</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>103</v>
@@ -3302,7 +3410,7 @@
         <v>43643</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>104</v>
@@ -3311,13 +3419,13 @@
         <v>105</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L13" s="10" t="s">
         <v>55</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AW13" s="1" t="s">
         <v>61</v>
@@ -3329,7 +3437,7 @@
         <v>5</v>
       </c>
       <c r="BD13" s="1" t="s">
-        <v>55</v>
+        <v>377</v>
       </c>
     </row>
     <row r="14" spans="1:86" ht="187">
@@ -3340,7 +3448,7 @@
         <v>99</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>107</v>
@@ -3355,7 +3463,7 @@
         <v>43684</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>113</v>
@@ -3364,25 +3472,25 @@
         <v>114</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L14" s="10" t="s">
         <v>55</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AW14" s="1" t="s">
         <v>61</v>
       </c>
       <c r="AX14" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="BA14" s="1">
         <v>24</v>
       </c>
       <c r="BD14" s="1" t="s">
-        <v>55</v>
+        <v>377</v>
       </c>
     </row>
     <row r="15" spans="1:86" ht="238">
@@ -3393,7 +3501,7 @@
         <v>99</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>109</v>
@@ -3408,7 +3516,7 @@
         <v>43573</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>111</v>
@@ -3417,13 +3525,13 @@
         <v>112</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L15" s="7" t="s">
         <v>55</v>
       </c>
       <c r="M15" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="16" spans="1:86" ht="238">
@@ -3434,7 +3542,7 @@
         <v>99</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>115</v>
@@ -3449,7 +3557,7 @@
         <v>43648</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>116</v>
@@ -3458,13 +3566,13 @@
         <v>117</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AW16" s="1" t="s">
         <v>64</v>
@@ -3502,10 +3610,10 @@
         <v>99</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>55</v>
@@ -3517,19 +3625,19 @@
         <v>43865</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>116</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L17" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="M17" s="11" t="s">
         <v>274</v>
-      </c>
-      <c r="M17" s="11" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:86" ht="289">
@@ -3540,10 +3648,10 @@
         <v>99</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>55</v>
@@ -3555,7 +3663,7 @@
         <v>43775</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>119</v>
@@ -3564,13 +3672,13 @@
         <v>120</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="19" spans="1:86" ht="136">
@@ -3581,7 +3689,7 @@
         <v>99</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>121</v>
@@ -3596,7 +3704,7 @@
         <v>43801</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>123</v>
@@ -3605,7 +3713,7 @@
         <v>124</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L19" s="8"/>
       <c r="M19" s="9"/>
@@ -3618,7 +3726,7 @@
         <v>125</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>126</v>
@@ -3633,7 +3741,7 @@
         <v>43803</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>127</v>
@@ -3642,13 +3750,13 @@
         <v>128</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L20" s="10" t="s">
         <v>55</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AC20" s="1" t="s">
         <v>56</v>
@@ -3668,7 +3776,7 @@
         <v>125</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>131</v>
@@ -3683,7 +3791,7 @@
         <v>43648</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>132</v>
@@ -3692,13 +3800,13 @@
         <v>117</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="M21" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AC21" s="1" t="s">
         <v>56</v>
@@ -3718,7 +3826,7 @@
         <v>125</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>133</v>
@@ -3733,7 +3841,7 @@
         <v>43621</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>135</v>
@@ -3742,13 +3850,13 @@
         <v>136</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L22" s="10" t="s">
         <v>55</v>
       </c>
       <c r="M22" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AC22" s="1" t="s">
         <v>56</v>
@@ -3768,7 +3876,7 @@
         <v>137</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>138</v>
@@ -3790,7 +3898,7 @@
         <v>140</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L23" s="8"/>
       <c r="M23" s="9"/>
@@ -3803,10 +3911,10 @@
         <v>137</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>58</v>
@@ -3818,7 +3926,7 @@
         <v>43896</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>142</v>
@@ -3827,13 +3935,13 @@
         <v>143</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M24" s="9" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="25" spans="1:86" ht="51">
@@ -3850,37 +3958,37 @@
       <c r="L25" s="8"/>
       <c r="M25" s="9"/>
       <c r="O25" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="P25" s="1">
         <v>20</v>
       </c>
       <c r="Q25" s="26" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="V25" s="1">
         <v>5</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="Y25" s="1">
         <v>5</v>
       </c>
       <c r="Z25" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="AB25" s="1">
         <v>5</v>
       </c>
       <c r="AD25" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="AF25" s="1">
         <v>5</v>
@@ -3895,10 +4003,10 @@
         <v>400</v>
       </c>
       <c r="AJ25" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="AK25" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="AM25" s="1">
         <v>5</v>
@@ -3907,7 +4015,7 @@
         <v>5</v>
       </c>
       <c r="AO25" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="AQ25" s="1">
         <v>5</v>
@@ -3916,7 +4024,7 @@
         <v>5</v>
       </c>
       <c r="AS25" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="AU25" s="1">
         <v>5</v>
@@ -3925,7 +4033,7 @@
         <v>5</v>
       </c>
       <c r="AX25" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="AZ25" s="1">
         <v>5</v>
@@ -3940,10 +4048,10 @@
         <v>400</v>
       </c>
       <c r="BD25" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="BE25" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="BG25" s="1">
         <v>5</v>
@@ -3952,7 +4060,7 @@
         <v>5</v>
       </c>
       <c r="BI25" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="BK25" s="1">
         <v>5</v>
@@ -3961,7 +4069,7 @@
         <v>5</v>
       </c>
       <c r="BM25" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="BO25" s="1">
         <v>5</v>
@@ -3970,16 +4078,16 @@
         <v>5</v>
       </c>
       <c r="BQ25" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="BR25" s="1" t="s">
         <v>61</v>
       </c>
       <c r="BS25" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="BT25" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="BU25" s="1">
         <v>0.7</v>
@@ -3988,7 +4096,7 @@
         <v>84</v>
       </c>
       <c r="BW25" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="BX25" s="1">
         <v>5</v>
@@ -4000,7 +4108,7 @@
         <v>5</v>
       </c>
       <c r="CA25" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="CB25" s="1">
         <v>5</v>
@@ -4012,7 +4120,7 @@
         <v>5</v>
       </c>
       <c r="CE25" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="CF25" s="1">
         <v>5</v>
@@ -4236,13 +4344,13 @@
         <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>54</v>
@@ -4251,22 +4359,22 @@
         <v>42922</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>55</v>
@@ -4287,7 +4395,7 @@
         <v>60</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AF2" s="1" t="s">
         <v>57</v>
@@ -4310,34 +4418,34 @@
         <v>55</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="F3" s="2">
         <v>42852</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>187</v>
-      </c>
       <c r="L3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>55</v>
@@ -4372,37 +4480,37 @@
         <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="F4" s="2">
         <v>42941</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>55</v>
@@ -4437,34 +4545,34 @@
         <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="F5" s="2">
         <v>42929</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="L5" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>55</v>
@@ -4499,31 +4607,31 @@
         <v>90</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="F6" s="2">
         <v>42941</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>208</v>
-      </c>
       <c r="L6" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>55</v>
@@ -4537,37 +4645,37 @@
         <v>55</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="F7" s="2">
         <v>42930</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="L7" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>57</v>
@@ -4608,37 +4716,37 @@
         <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="F8" s="2">
         <v>42933</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>222</v>
-      </c>
       <c r="L8" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>57</v>
@@ -4656,7 +4764,7 @@
         <v>55</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AF8" s="1" t="s">
         <v>57</v>
@@ -4682,10 +4790,10 @@
         <v>90</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>66</v>
@@ -4694,22 +4802,22 @@
         <v>43040</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>229</v>
-      </c>
       <c r="L9" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>57</v>
@@ -4726,10 +4834,10 @@
         <v>89</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>67</v>
@@ -4738,25 +4846,25 @@
         <v>43055</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="AE10" s="1" t="s">
         <v>61</v>
       </c>
       <c r="AF10" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AJ10" s="1" t="s">
         <v>55</v>
@@ -4767,7 +4875,7 @@
         <v>55</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>68</v>
@@ -4782,16 +4890,16 @@
         <v>70</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="AO11" s="1" t="s">
         <v>58</v>
@@ -4829,10 +4937,10 @@
         <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>77</v>
@@ -4850,13 +4958,13 @@
         <v>79</v>
       </c>
       <c r="I12" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="AO12" s="1" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
iuu and oa back up
</commit_message>
<xml_diff>
--- a/app/data/wto_proposal_settings_master.xlsx
+++ b/app/data/wto_proposal_settings_master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kat/GitHub/SubsidyExplorer/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216DED76-F5DA-6843-A47C-B18A99D15E3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A023396-805E-A649-9593-70E454D0C665}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="390">
   <si>
     <t>proposal</t>
   </si>
@@ -471,9 +471,6 @@
   </si>
   <si>
     <t>This unofficial room document was circulated at the request of the Delegations of Argentina, Colombia, Costa Rica, Panama, Peru, Uruguay, Canada, Iceland, New Zealand, and the United States on June 12, 2019.</t>
-  </si>
-  <si>
-    <t>iuu1, iuu2, iuu3, iuu4</t>
   </si>
   <si>
     <t xml:space="preserve">This communication advocates for negotiating Member-specific subsidy caps (expressed in monetary terms). Subsidies in excess of a Member's cap would be prohibited. This cap is intended to be suplementary to any prohibitions on subsidies that support IUU, fishing beyond national jurisdiction, and subsidies for fishing that negatively affect overfished stocks. Members would also commit to maintain fisheries management and conservation measures. </t>
@@ -2472,9 +2469,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CH25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA6" sqref="AA6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -2507,7 +2504,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>1</v>
@@ -2516,7 +2513,7 @@
         <v>130</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>2</v>
@@ -2531,7 +2528,7 @@
         <v>5</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="N1" s="13" t="s">
         <v>7</v>
@@ -2552,31 +2549,31 @@
         <v>12</v>
       </c>
       <c r="T1" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="U1" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="V1" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="W1" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="X1" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="Y1" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="Z1" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="AA1" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AB1" s="13" t="s">
         <v>346</v>
-      </c>
-      <c r="AB1" s="13" t="s">
-        <v>347</v>
       </c>
       <c r="AC1" s="13" t="s">
         <v>16</v>
@@ -2594,49 +2591,49 @@
         <v>20</v>
       </c>
       <c r="AH1" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="AI1" s="13" t="s">
         <v>348</v>
-      </c>
-      <c r="AI1" s="13" t="s">
-        <v>349</v>
       </c>
       <c r="AJ1" s="13" t="s">
         <v>21</v>
       </c>
       <c r="AK1" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="AL1" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="AL1" s="13" t="s">
+      <c r="AM1" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="AM1" s="13" t="s">
+      <c r="AN1" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="AN1" s="13" t="s">
+      <c r="AO1" s="13" t="s">
         <v>353</v>
       </c>
-      <c r="AO1" s="13" t="s">
+      <c r="AP1" s="13" t="s">
         <v>354</v>
       </c>
-      <c r="AP1" s="13" t="s">
+      <c r="AQ1" s="13" t="s">
         <v>355</v>
       </c>
-      <c r="AQ1" s="13" t="s">
+      <c r="AR1" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="AR1" s="13" t="s">
+      <c r="AS1" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="AS1" s="13" t="s">
+      <c r="AT1" s="13" t="s">
         <v>358</v>
       </c>
-      <c r="AT1" s="13" t="s">
+      <c r="AU1" s="13" t="s">
         <v>359</v>
       </c>
-      <c r="AU1" s="13" t="s">
+      <c r="AV1" s="13" t="s">
         <v>360</v>
-      </c>
-      <c r="AV1" s="13" t="s">
-        <v>361</v>
       </c>
       <c r="AW1" s="13" t="s">
         <v>26</v>
@@ -2654,49 +2651,49 @@
         <v>30</v>
       </c>
       <c r="BB1" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="BC1" s="13" t="s">
         <v>362</v>
-      </c>
-      <c r="BC1" s="13" t="s">
-        <v>363</v>
       </c>
       <c r="BD1" s="13" t="s">
         <v>31</v>
       </c>
       <c r="BE1" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="BF1" s="13" t="s">
         <v>364</v>
       </c>
-      <c r="BF1" s="13" t="s">
+      <c r="BG1" s="13" t="s">
         <v>365</v>
       </c>
-      <c r="BG1" s="13" t="s">
+      <c r="BH1" s="13" t="s">
         <v>366</v>
       </c>
-      <c r="BH1" s="13" t="s">
+      <c r="BI1" s="13" t="s">
         <v>367</v>
       </c>
-      <c r="BI1" s="13" t="s">
+      <c r="BJ1" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="BJ1" s="13" t="s">
+      <c r="BK1" s="13" t="s">
         <v>369</v>
       </c>
-      <c r="BK1" s="13" t="s">
+      <c r="BL1" s="13" t="s">
         <v>370</v>
       </c>
-      <c r="BL1" s="13" t="s">
+      <c r="BM1" s="13" t="s">
         <v>371</v>
       </c>
-      <c r="BM1" s="13" t="s">
+      <c r="BN1" s="13" t="s">
         <v>372</v>
       </c>
-      <c r="BN1" s="13" t="s">
+      <c r="BO1" s="13" t="s">
         <v>373</v>
       </c>
-      <c r="BO1" s="13" t="s">
+      <c r="BP1" s="13" t="s">
         <v>374</v>
-      </c>
-      <c r="BP1" s="13" t="s">
-        <v>375</v>
       </c>
       <c r="BQ1" s="13" t="s">
         <v>36</v>
@@ -2761,82 +2758,82 @@
         <v>89</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D2" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>304</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>305</v>
       </c>
       <c r="G2" s="18">
         <v>43896</v>
       </c>
       <c r="H2" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>306</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="K2" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="L2" s="20" t="s">
         <v>309</v>
       </c>
-      <c r="L2" s="20" t="s">
-        <v>310</v>
-      </c>
       <c r="M2" s="21" t="s">
+        <v>384</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="AC2" s="13" t="s">
         <v>385</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>377</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>377</v>
-      </c>
-      <c r="AC2" s="13" t="s">
+      <c r="AD2" s="13" t="s">
+        <v>375</v>
+      </c>
+      <c r="AJ2" s="13" t="s">
         <v>386</v>
       </c>
-      <c r="AD2" s="13" t="s">
-        <v>376</v>
-      </c>
-      <c r="AJ2" s="13" t="s">
+      <c r="AK2" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="AL2" s="13" t="s">
         <v>387</v>
-      </c>
-      <c r="AK2" s="13" t="s">
-        <v>387</v>
-      </c>
-      <c r="AL2" s="13" t="s">
-        <v>388</v>
       </c>
       <c r="AN2" s="13">
         <v>5</v>
       </c>
       <c r="AO2" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="AP2" s="13" t="s">
         <v>387</v>
-      </c>
-      <c r="AP2" s="13" t="s">
-        <v>388</v>
       </c>
       <c r="AR2" s="13">
         <v>3</v>
       </c>
       <c r="AS2" s="13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AW2" s="1" t="s">
         <v>61</v>
       </c>
       <c r="AX2" s="13" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AZ2" s="13">
         <v>5</v>
@@ -2845,31 +2842,31 @@
         <v>24</v>
       </c>
       <c r="BD2" s="13" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="BE2" s="13" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="BF2" s="13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="BH2" s="13">
         <v>5</v>
       </c>
       <c r="BI2" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="BJ2" s="13" t="s">
         <v>387</v>
-      </c>
-      <c r="BJ2" s="13" t="s">
-        <v>388</v>
       </c>
       <c r="BL2" s="13">
         <v>3</v>
       </c>
       <c r="BM2" s="13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="BQ2" s="13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="3" spans="1:86" ht="136">
@@ -2880,7 +2877,7 @@
         <v>89</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>85</v>
@@ -2895,7 +2892,7 @@
         <v>43759</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>86</v>
@@ -2904,22 +2901,22 @@
         <v>87</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>55</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AW3" s="1" t="s">
         <v>61</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="BD3" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4" spans="1:86" ht="170">
@@ -2942,7 +2939,7 @@
         <v>43801</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>92</v>
@@ -2951,25 +2948,25 @@
         <v>93</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>55</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="Q4" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="5" spans="1:86" ht="119">
@@ -2980,7 +2977,7 @@
         <v>90</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>94</v>
@@ -2995,7 +2992,7 @@
         <v>43718</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>95</v>
@@ -3004,25 +3001,25 @@
         <v>96</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L5" s="24" t="s">
         <v>55</v>
       </c>
       <c r="M5" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="O5" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="Q5" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="6" spans="1:86" ht="136">
@@ -3033,10 +3030,10 @@
         <v>90</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>55</v>
@@ -3048,7 +3045,7 @@
         <v>43865</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>145</v>
@@ -3057,46 +3054,46 @@
         <v>117</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="L6" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="L6" s="8" t="s">
-        <v>259</v>
-      </c>
       <c r="M6" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="S6" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>388</v>
       </c>
       <c r="V6" s="1">
         <v>5</v>
       </c>
       <c r="W6" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="X6" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="X6" s="1" t="s">
-        <v>388</v>
       </c>
       <c r="Y6" s="1">
         <v>3</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="7" spans="1:86" ht="221">
@@ -3119,7 +3116,7 @@
         <v>43628</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>147</v>
@@ -3128,22 +3125,22 @@
         <v>149</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>55</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>150</v>
+        <v>382</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>55</v>
+        <v>376</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>55</v>
+        <v>376</v>
       </c>
     </row>
     <row r="8" spans="1:86" ht="272">
@@ -3166,7 +3163,7 @@
         <v>43657</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>70</v>
@@ -3175,13 +3172,13 @@
         <v>129</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M8" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>152</v>
       </c>
       <c r="BQ8" s="1" t="s">
         <v>58</v>
@@ -3222,7 +3219,7 @@
         <v>99</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>77</v>
@@ -3237,7 +3234,7 @@
         <v>43620</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>78</v>
@@ -3246,13 +3243,13 @@
         <v>79</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>55</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="BQ9" s="1" t="s">
         <v>58</v>
@@ -3281,7 +3278,7 @@
         <v>99</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>100</v>
@@ -3296,22 +3293,22 @@
         <v>43545</v>
       </c>
       <c r="H10" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>279</v>
-      </c>
       <c r="M10" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:86" ht="85">
@@ -3322,7 +3319,7 @@
         <v>99</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>101</v>
@@ -3338,13 +3335,13 @@
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="K11" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L11" s="8"/>
       <c r="M11" s="9"/>
@@ -3357,34 +3354,34 @@
         <v>99</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G12" s="2">
         <v>43843</v>
       </c>
       <c r="H12" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="K12" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="K12" s="6" t="s">
-        <v>292</v>
-      </c>
       <c r="L12" s="7" t="s">
         <v>55</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:86" ht="136.5" customHeight="1">
@@ -3395,7 +3392,7 @@
         <v>99</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>103</v>
@@ -3410,7 +3407,7 @@
         <v>43643</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>104</v>
@@ -3419,13 +3416,13 @@
         <v>105</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L13" s="10" t="s">
         <v>55</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AW13" s="1" t="s">
         <v>61</v>
@@ -3437,7 +3434,7 @@
         <v>5</v>
       </c>
       <c r="BD13" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="14" spans="1:86" ht="187">
@@ -3448,7 +3445,7 @@
         <v>99</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>107</v>
@@ -3463,7 +3460,7 @@
         <v>43684</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>113</v>
@@ -3472,25 +3469,25 @@
         <v>114</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L14" s="10" t="s">
         <v>55</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AW14" s="1" t="s">
         <v>61</v>
       </c>
       <c r="AX14" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="BA14" s="1">
         <v>24</v>
       </c>
       <c r="BD14" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="15" spans="1:86" ht="238">
@@ -3501,7 +3498,7 @@
         <v>99</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>109</v>
@@ -3516,7 +3513,7 @@
         <v>43573</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>111</v>
@@ -3525,13 +3522,13 @@
         <v>112</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L15" s="7" t="s">
         <v>55</v>
       </c>
       <c r="M15" s="11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:86" ht="238">
@@ -3542,7 +3539,7 @@
         <v>99</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>115</v>
@@ -3557,7 +3554,7 @@
         <v>43648</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>116</v>
@@ -3566,13 +3563,13 @@
         <v>117</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AW16" s="1" t="s">
         <v>64</v>
@@ -3610,10 +3607,10 @@
         <v>99</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>55</v>
@@ -3625,19 +3622,19 @@
         <v>43865</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>116</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L17" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="M17" s="11" t="s">
         <v>273</v>
-      </c>
-      <c r="M17" s="11" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="18" spans="1:86" ht="289">
@@ -3648,10 +3645,10 @@
         <v>99</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>55</v>
@@ -3663,7 +3660,7 @@
         <v>43775</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>119</v>
@@ -3672,13 +3669,13 @@
         <v>120</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="19" spans="1:86" ht="136">
@@ -3689,7 +3686,7 @@
         <v>99</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>121</v>
@@ -3704,7 +3701,7 @@
         <v>43801</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>123</v>
@@ -3713,7 +3710,7 @@
         <v>124</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L19" s="8"/>
       <c r="M19" s="9"/>
@@ -3726,7 +3723,7 @@
         <v>125</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>126</v>
@@ -3741,7 +3738,7 @@
         <v>43803</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>127</v>
@@ -3750,13 +3747,13 @@
         <v>128</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L20" s="10" t="s">
         <v>55</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AC20" s="1" t="s">
         <v>56</v>
@@ -3776,7 +3773,7 @@
         <v>125</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>131</v>
@@ -3791,7 +3788,7 @@
         <v>43648</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>132</v>
@@ -3800,13 +3797,13 @@
         <v>117</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M21" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AC21" s="1" t="s">
         <v>56</v>
@@ -3826,7 +3823,7 @@
         <v>125</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>133</v>
@@ -3841,7 +3838,7 @@
         <v>43621</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>135</v>
@@ -3850,13 +3847,13 @@
         <v>136</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L22" s="10" t="s">
         <v>55</v>
       </c>
       <c r="M22" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AC22" s="1" t="s">
         <v>56</v>
@@ -3876,7 +3873,7 @@
         <v>137</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>138</v>
@@ -3898,7 +3895,7 @@
         <v>140</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L23" s="8"/>
       <c r="M23" s="9"/>
@@ -3911,10 +3908,10 @@
         <v>137</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>58</v>
@@ -3926,7 +3923,7 @@
         <v>43896</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>142</v>
@@ -3935,13 +3932,13 @@
         <v>143</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L24" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="M24" s="9" t="s">
         <v>313</v>
-      </c>
-      <c r="M24" s="9" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="25" spans="1:86" ht="51">
@@ -3958,37 +3955,37 @@
       <c r="L25" s="8"/>
       <c r="M25" s="9"/>
       <c r="O25" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P25" s="1">
         <v>20</v>
       </c>
       <c r="Q25" s="26" t="s">
+        <v>375</v>
+      </c>
+      <c r="S25" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="S25" s="1" t="s">
-        <v>377</v>
-      </c>
       <c r="T25" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="V25" s="1">
         <v>5</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="Y25" s="1">
         <v>5</v>
       </c>
       <c r="Z25" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AB25" s="1">
         <v>5</v>
       </c>
       <c r="AD25" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AF25" s="1">
         <v>5</v>
@@ -4003,10 +4000,10 @@
         <v>400</v>
       </c>
       <c r="AJ25" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AK25" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AM25" s="1">
         <v>5</v>
@@ -4015,7 +4012,7 @@
         <v>5</v>
       </c>
       <c r="AO25" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AQ25" s="1">
         <v>5</v>
@@ -4024,7 +4021,7 @@
         <v>5</v>
       </c>
       <c r="AS25" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AU25" s="1">
         <v>5</v>
@@ -4033,7 +4030,7 @@
         <v>5</v>
       </c>
       <c r="AX25" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AZ25" s="1">
         <v>5</v>
@@ -4048,10 +4045,10 @@
         <v>400</v>
       </c>
       <c r="BD25" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="BE25" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="BG25" s="1">
         <v>5</v>
@@ -4060,7 +4057,7 @@
         <v>5</v>
       </c>
       <c r="BI25" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="BK25" s="1">
         <v>5</v>
@@ -4069,7 +4066,7 @@
         <v>5</v>
       </c>
       <c r="BM25" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="BO25" s="1">
         <v>5</v>
@@ -4078,16 +4075,16 @@
         <v>5</v>
       </c>
       <c r="BQ25" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="BR25" s="1" t="s">
         <v>61</v>
       </c>
       <c r="BS25" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="BT25" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="BT25" s="1" t="s">
-        <v>379</v>
       </c>
       <c r="BU25" s="1">
         <v>0.7</v>
@@ -4096,7 +4093,7 @@
         <v>84</v>
       </c>
       <c r="BW25" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="BX25" s="1">
         <v>5</v>
@@ -4108,7 +4105,7 @@
         <v>5</v>
       </c>
       <c r="CA25" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="CB25" s="1">
         <v>5</v>
@@ -4120,7 +4117,7 @@
         <v>5</v>
       </c>
       <c r="CE25" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="CF25" s="1">
         <v>5</v>
@@ -4344,13 +4341,13 @@
         <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>54</v>
@@ -4359,22 +4356,22 @@
         <v>42922</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>55</v>
@@ -4395,7 +4392,7 @@
         <v>60</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AF2" s="1" t="s">
         <v>57</v>
@@ -4418,34 +4415,34 @@
         <v>55</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="F3" s="2">
         <v>42852</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="L3" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>55</v>
@@ -4480,37 +4477,37 @@
         <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="F4" s="2">
         <v>42941</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>55</v>
@@ -4545,34 +4542,34 @@
         <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="F5" s="2">
         <v>42929</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>200</v>
-      </c>
       <c r="L5" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>55</v>
@@ -4607,31 +4604,31 @@
         <v>90</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="F6" s="2">
         <v>42941</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="L6" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>55</v>
@@ -4645,37 +4642,37 @@
         <v>55</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="F7" s="2">
         <v>42930</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>214</v>
-      </c>
       <c r="L7" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>57</v>
@@ -4716,37 +4713,37 @@
         <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="F8" s="2">
         <v>42933</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="L8" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>57</v>
@@ -4764,7 +4761,7 @@
         <v>55</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AF8" s="1" t="s">
         <v>57</v>
@@ -4790,10 +4787,10 @@
         <v>90</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>66</v>
@@ -4802,22 +4799,22 @@
         <v>43040</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>228</v>
-      </c>
       <c r="L9" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>57</v>
@@ -4834,10 +4831,10 @@
         <v>89</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>67</v>
@@ -4846,25 +4843,25 @@
         <v>43055</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="AE10" s="1" t="s">
         <v>61</v>
       </c>
       <c r="AF10" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AJ10" s="1" t="s">
         <v>55</v>
@@ -4875,7 +4872,7 @@
         <v>55</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>68</v>
@@ -4890,16 +4887,16 @@
         <v>70</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="AO11" s="1" t="s">
         <v>58</v>
@@ -4937,10 +4934,10 @@
         <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>77</v>
@@ -4958,13 +4955,13 @@
         <v>79</v>
       </c>
       <c r="I12" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="AO12" s="1" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
broke policy widget options
</commit_message>
<xml_diff>
--- a/app/data/wto_proposal_settings_master.xlsx
+++ b/app/data/wto_proposal_settings_master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kat/GitHub/SubsidyExplorer/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF30155-D08C-C342-A039-5E620F86AB6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9517B7-4F7A-8846-807E-8B77D8DA24E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="398">
   <si>
     <t>proposal</t>
   </si>
@@ -1371,9 +1371,6 @@
     <t>TIME</t>
   </si>
   <si>
-    <t>LENGTH</t>
-  </si>
-  <si>
     <t>Facilitator's Proposal - IUU</t>
   </si>
   <si>
@@ -1446,9 +1443,6 @@
     <t>DONE</t>
   </si>
   <si>
-    <t>MOSTLY DONE - LDC new proposal includes 3 pillars of prohibiion (IUU, Overfished and OFOC) and S&amp;DT. We might need to consider a new section or include it in Other. I don't think we would like to separate or divide the proposal as we would like to see the effect of the proposal as a whole.</t>
-  </si>
-  <si>
     <t xml:space="preserve">MOSTLY DONE - Time delay to be incorporated. </t>
   </si>
   <si>
@@ -1462,6 +1456,33 @@
   </si>
   <si>
     <t>ONE</t>
+  </si>
+  <si>
+    <t>kat_notes</t>
+  </si>
+  <si>
+    <t>ernesto_notes</t>
+  </si>
+  <si>
+    <t>LDC new proposal includes 3 pillars of prohibiion (IUU, Overfished and OFOC) and S&amp;DT. We might need to consider a new section or include it in Other. I don't think we would like to separate or divide the proposal as we would like to see the effect of the proposal as a whole.</t>
+  </si>
+  <si>
+    <t>summary_html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transition period missing; need to figure out what this proposal says about territorial waters. </t>
+  </si>
+  <si>
+    <t>&lt;b&gt; IUU:  &lt;/b&gt;&lt;/br&gt;  None. &lt;/br&gt; &lt;b&gt; Overfished:  &lt;/b&gt;&lt;/br&gt; None. &lt;/br&gt; &lt;b&gt; OFOC:  &lt;/b&gt;&lt;/br&gt; All capacity enhancing subsidies are prohibited to vessels fishing in disputed waters. &lt;/br&gt; &lt;b&gt; S&amp;DT:  &lt;/b&gt;&lt;/br&gt; None.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt; IUU:  &lt;/b&gt;&lt;/br&gt;  Determination made by: &lt;ul&gt;&lt;li&gt;RMFO/A lists&lt;/li&gt;&lt;li&gt;Flag Member states&lt;/li&gt;&lt;li&gt;Coastal Member states&lt;/li&gt;&lt;li&gt;Subsidizing Member states&lt;/li&gt;&lt;/ul&gt; &lt;/br&gt; &lt;b&gt; Overfished:  &lt;/b&gt;&lt;/br&gt; Overfished stock determination made by best scientific evidence available: &lt;ul&gt;&lt;li&gt; B/Bmsy &lt; 1  (RAM Legacy stock assessment database) &lt;/li&gt;&lt;/ul&gt; Subsidies to fishing in territorial waters is allowed. &lt;/br&gt; &lt;b&gt; OFOC:  &lt;/b&gt;&lt;/br&gt; All capacity enhancing subsidies are prohibited to vessels meeting any of the following characteristics: &lt;ul&gt;&lt;li&gt;fishing on the high seas&lt;/li&gt;&lt;li&gt; &gt; 24m in length&lt;/li&gt;&lt;li&gt; &gt; 100 gross tons&lt;/li&gt;&lt;/ul&gt; Subsidies to fishing in territorial waters is allowed. &lt;/br&gt; &lt;b&gt; S&amp;DT:  &lt;/b&gt;&lt;/br&gt;&lt;i&gt;LDCs  :&lt;/i&gt; Transition period of X years for all prohibitions; excluded from OFOC prohibitions. &lt;/br&gt; &lt;i&gt;Developing :&lt;/i&gt; Transition period of Y years for all prohibitions. &lt;/br&gt; &lt;i&gt;SVEs :&lt;/i&gt; None.</t>
+  </si>
+  <si>
+    <t>EX_TER</t>
+  </si>
+  <si>
+    <t>LENGTH, EX_TER</t>
   </si>
 </sst>
 </file>
@@ -1987,7 +2008,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2066,6 +2087,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2422,1758 +2449,1778 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CH25"/>
+  <dimension ref="A1:CJ25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BL1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BQ10" sqref="BQ10"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BB2" sqref="BB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="10.83203125" style="12"/>
-    <col min="3" max="3" width="32.83203125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="13" style="1" customWidth="1"/>
-    <col min="6" max="7" width="10.83203125" style="1"/>
-    <col min="8" max="8" width="15.1640625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="28" style="1" customWidth="1"/>
-    <col min="10" max="10" width="48" style="1" customWidth="1"/>
-    <col min="11" max="11" width="48.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="56.1640625" style="12" customWidth="1"/>
-    <col min="13" max="13" width="71" style="12" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="36.5" style="12" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="13" style="1" customWidth="1"/>
+    <col min="7" max="8" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="15.1640625" style="12" customWidth="1"/>
+    <col min="10" max="10" width="28" style="1" customWidth="1"/>
+    <col min="11" max="11" width="48" style="1" customWidth="1"/>
+    <col min="12" max="13" width="48.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="56.1640625" style="12" customWidth="1"/>
+    <col min="15" max="15" width="71" style="12" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:86" s="13" customFormat="1" ht="68">
+    <row r="1" spans="1:88" s="13" customFormat="1" ht="68">
       <c r="A1" s="13" t="s">
         <v>144</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>146</v>
+      <c r="C1" s="27" t="s">
+        <v>389</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>311</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="M1" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="N1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="O1" s="17" t="s">
         <v>309</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="U1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="V1" s="13" t="s">
         <v>315</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="W1" s="13" t="s">
         <v>316</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="X1" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="Y1" s="13" t="s">
         <v>318</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="Z1" s="13" t="s">
         <v>319</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="AA1" s="13" t="s">
         <v>320</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="AB1" s="13" t="s">
         <v>321</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AC1" s="13" t="s">
         <v>322</v>
       </c>
-      <c r="AB1" s="13" t="s">
+      <c r="AD1" s="13" t="s">
         <v>323</v>
       </c>
-      <c r="AC1" s="13" t="s">
+      <c r="AE1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="AD1" s="13" t="s">
+      <c r="AF1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="AE1" s="13" t="s">
+      <c r="AG1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="AF1" s="13" t="s">
+      <c r="AH1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="AG1" s="13" t="s">
+      <c r="AI1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="AH1" s="13" t="s">
+      <c r="AJ1" s="13" t="s">
         <v>324</v>
       </c>
-      <c r="AI1" s="13" t="s">
+      <c r="AK1" s="13" t="s">
         <v>325</v>
       </c>
-      <c r="AJ1" s="13" t="s">
+      <c r="AL1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="AK1" s="13" t="s">
+      <c r="AM1" s="13" t="s">
         <v>326</v>
       </c>
-      <c r="AL1" s="13" t="s">
+      <c r="AN1" s="13" t="s">
         <v>327</v>
       </c>
-      <c r="AM1" s="13" t="s">
+      <c r="AO1" s="13" t="s">
         <v>328</v>
       </c>
-      <c r="AN1" s="13" t="s">
+      <c r="AP1" s="13" t="s">
         <v>329</v>
       </c>
-      <c r="AO1" s="13" t="s">
+      <c r="AQ1" s="13" t="s">
         <v>330</v>
       </c>
-      <c r="AP1" s="13" t="s">
+      <c r="AR1" s="13" t="s">
         <v>331</v>
       </c>
-      <c r="AQ1" s="13" t="s">
+      <c r="AS1" s="13" t="s">
         <v>332</v>
       </c>
-      <c r="AR1" s="13" t="s">
+      <c r="AT1" s="13" t="s">
         <v>333</v>
       </c>
-      <c r="AS1" s="13" t="s">
+      <c r="AU1" s="13" t="s">
         <v>334</v>
       </c>
-      <c r="AT1" s="13" t="s">
+      <c r="AV1" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="AU1" s="13" t="s">
+      <c r="AW1" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="AV1" s="13" t="s">
+      <c r="AX1" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="AW1" s="13" t="s">
+      <c r="AY1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="AX1" s="13" t="s">
+      <c r="AZ1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="AY1" s="13" t="s">
+      <c r="BA1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="AZ1" s="13" t="s">
+      <c r="BB1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="BA1" s="13" t="s">
+      <c r="BC1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="BB1" s="13" t="s">
+      <c r="BD1" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="BC1" s="13" t="s">
+      <c r="BE1" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="BD1" s="13" t="s">
+      <c r="BF1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="BE1" s="13" t="s">
+      <c r="BG1" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="BF1" s="13" t="s">
+      <c r="BH1" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="BG1" s="13" t="s">
+      <c r="BI1" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="BH1" s="13" t="s">
+      <c r="BJ1" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="BI1" s="13" t="s">
+      <c r="BK1" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="BJ1" s="13" t="s">
+      <c r="BL1" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="BK1" s="13" t="s">
+      <c r="BM1" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="BL1" s="13" t="s">
+      <c r="BN1" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="BM1" s="13" t="s">
+      <c r="BO1" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="BN1" s="13" t="s">
+      <c r="BP1" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="BO1" s="13" t="s">
+      <c r="BQ1" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="BP1" s="13" t="s">
+      <c r="BR1" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="BQ1" s="13" t="s">
+      <c r="BS1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="BR1" s="13" t="s">
+      <c r="BT1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="BS1" s="13" t="s">
+      <c r="BU1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="BT1" s="13" t="s">
+      <c r="BV1" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="BU1" s="13" t="s">
+      <c r="BW1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="BV1" s="13" t="s">
+      <c r="BX1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="BW1" s="13" t="s">
+      <c r="BY1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="BX1" s="13" t="s">
+      <c r="BZ1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="BY1" s="13" t="s">
+      <c r="CA1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="BZ1" s="13" t="s">
+      <c r="CB1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="CA1" s="13" t="s">
+      <c r="CC1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="CB1" s="13" t="s">
+      <c r="CD1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="CC1" s="13" t="s">
+      <c r="CE1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="CD1" s="13" t="s">
+      <c r="CF1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="CE1" s="13" t="s">
+      <c r="CG1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="CF1" s="13" t="s">
+      <c r="CH1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="CG1" s="13" t="s">
+      <c r="CI1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="CH1" s="13" t="s">
+      <c r="CJ1" s="13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:86" s="13" customFormat="1" ht="282" customHeight="1">
+    <row r="2" spans="1:88" s="13" customFormat="1" ht="282" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>58</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>385</v>
-      </c>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="28" t="s">
+        <v>393</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>391</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>55</v>
-      </c>
       <c r="F2" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="G2" s="18">
+      <c r="H2" s="18">
         <v>43896</v>
       </c>
-      <c r="H2" s="15" t="s">
-        <v>367</v>
-      </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="J2" s="13" t="s">
         <v>290</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="K2" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="L2" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="M2" s="19" t="s">
+        <v>395</v>
+      </c>
+      <c r="N2" s="20" t="s">
         <v>293</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="O2" s="21" t="s">
         <v>360</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="O2" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="AC2" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="AD2" s="13" t="s">
-        <v>352</v>
-      </c>
-      <c r="AJ2" s="13" t="s">
+      <c r="Q2" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="U2" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="AE2" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="AF2" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="AL2" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="AK2" s="13" t="s">
+      <c r="AM2" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="AL2" s="13" t="s">
+      <c r="AN2" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="AN2" s="13">
+      <c r="AP2" s="13">
         <v>5</v>
       </c>
-      <c r="AO2" s="13" t="s">
+      <c r="AQ2" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="AP2" s="13" t="s">
+      <c r="AR2" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="AR2" s="13">
+      <c r="AT2" s="13">
         <v>3</v>
       </c>
-      <c r="AS2" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AU2" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="AY2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AX2" s="13" t="s">
-        <v>364</v>
-      </c>
-      <c r="BA2" s="13">
+      <c r="AZ2" s="13" t="s">
+        <v>397</v>
+      </c>
+      <c r="BC2" s="13">
         <v>24</v>
       </c>
-      <c r="BD2" s="13" t="s">
+      <c r="BF2" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="BE2" s="13" t="s">
+      <c r="BG2" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="BF2" s="13" t="s">
+      <c r="BH2" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="BH2" s="13">
+      <c r="BJ2" s="13">
         <v>5</v>
       </c>
-      <c r="BI2" s="13" t="s">
+      <c r="BK2" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="BJ2" s="13" t="s">
+      <c r="BL2" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="BL2" s="13">
+      <c r="BN2" s="13">
         <v>3</v>
       </c>
-      <c r="BM2" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="BQ2" s="13" t="s">
+      <c r="BO2" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="BS2" s="13" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="3" spans="1:86" ht="136">
+    <row r="3" spans="1:88" ht="136">
       <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>43759</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="L3" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="19" t="s">
+        <v>394</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="AJ3" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="AW3" s="1" t="s">
+      <c r="U3" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AY3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AX3" s="1" t="s">
+      <c r="AZ3" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="BD3" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="BQ3" s="1" t="s">
+      <c r="BF3" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BS3" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="4" spans="1:86" ht="170">
+    <row r="4" spans="1:88" ht="170">
       <c r="A4" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>384</v>
-      </c>
       <c r="D4" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>43801</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>365</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="M4" s="9" t="s">
+      <c r="N4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>353</v>
-      </c>
       <c r="Q4" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="AJ4" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="BD4" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="BQ4" s="1" t="s">
+      <c r="U4" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BF4" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BS4" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="5" spans="1:86" ht="119">
+    <row r="5" spans="1:88" ht="119">
       <c r="A5" s="25" t="s">
         <v>58</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>384</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="25" t="s">
+        <v>383</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>43718</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>366</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="L5" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" s="9" t="s">
+      <c r="N5" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>353</v>
-      </c>
       <c r="Q5" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="S5" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="AJ5" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="BD5" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="BQ5" s="1" t="s">
+      <c r="U5" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BF5" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BS5" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="6" spans="1:86" ht="136">
+    <row r="6" spans="1:88" ht="136">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>386</v>
-      </c>
       <c r="D6" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>43865</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="N6" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="O6" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>353</v>
-      </c>
       <c r="Q6" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="S6" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="U6" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="V6" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="W6" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="V6" s="1">
+      <c r="X6" s="1">
         <v>5</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="Y6" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="Z6" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="Y6" s="1">
+      <c r="AA6" s="1">
         <v>3</v>
       </c>
-      <c r="Z6" s="1" t="s">
+      <c r="AB6" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AC6" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="AB6" s="1">
+      <c r="AD6" s="1">
         <v>5</v>
       </c>
-      <c r="AJ6" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="BD6" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="BQ6" s="1" t="s">
+      <c r="AL6" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BF6" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BS6" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="7" spans="1:86" ht="221">
+    <row r="7" spans="1:88" ht="221">
       <c r="A7" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>384</v>
-      </c>
       <c r="D7" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>43628</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="L7" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="M7" s="9" t="s">
+      <c r="N7" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="O7" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="AJ7" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="BD7" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="BQ7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AL7" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BF7" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BS7" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="8" spans="1:86" ht="272">
+    <row r="8" spans="1:88" ht="272">
       <c r="A8" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>43657</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>368</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="L8" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="M8" s="9" t="s">
+      <c r="N8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="O8" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="BQ8" s="1" t="s">
+      <c r="BS8" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="BR8" s="1" t="s">
+      <c r="BT8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BS8" s="1" t="s">
+      <c r="BU8" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="BT8" s="1" t="s">
+      <c r="BV8" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="BV8" s="1" t="s">
+      <c r="BX8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BW8" s="1" t="s">
+      <c r="BY8" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="BZ8" s="1">
+      <c r="CB8" s="1">
         <v>90</v>
       </c>
-      <c r="CA8" s="1" t="s">
+      <c r="CC8" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="CB8" s="1">
+      <c r="CD8" s="1">
         <v>50</v>
       </c>
-      <c r="CE8" s="1" t="s">
+      <c r="CG8" s="1" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="9" spans="1:86" ht="323">
+    <row r="9" spans="1:88" ht="323">
       <c r="A9" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="2">
+        <v>43620</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="BS9" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="BT9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BU9" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="BY9" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G9" s="2">
-        <v>43620</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="M9" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="BQ9" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="BR9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="BS9" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="BW9" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="BY9" s="1">
+      <c r="CA9" s="1">
         <v>800</v>
       </c>
-      <c r="BZ9" s="1">
+      <c r="CB9" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:86" ht="388">
+    <row r="10" spans="1:88" ht="388">
       <c r="A10" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>43545</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="I10" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="L10" s="8" t="s">
+      <c r="N10" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="M10" s="9" t="s">
+      <c r="O10" s="9" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="11" spans="1:86" ht="85">
+    <row r="11" spans="1:88" ht="85">
       <c r="A11" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>43801</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="5"/>
+      <c r="J11" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="L11" s="8"/>
-      <c r="M11" s="9"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:86" ht="238">
+    <row r="12" spans="1:88" ht="238">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>43843</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="K12" s="6" t="s">
+      <c r="L12" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="L12" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="M12" s="11" t="s">
+      <c r="M12" s="6"/>
+      <c r="N12" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="O12" s="11" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="13" spans="1:86" ht="136.5" customHeight="1">
+    <row r="13" spans="1:88" ht="136.5" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>43643</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="I13" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="L13" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="M13" s="9" t="s">
+      <c r="N13" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="O13" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="AW13" s="1" t="s">
+      <c r="AY13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AX13" s="1" t="s">
+      <c r="AZ13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AZ13" s="1">
+      <c r="BB13" s="1">
         <v>5</v>
       </c>
-      <c r="BD13" s="1" t="s">
+      <c r="BF13" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="14" spans="1:86" ht="187">
+    <row r="14" spans="1:88" ht="187">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <v>43684</v>
       </c>
-      <c r="H14" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="L14" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="M14" s="9" t="s">
+      <c r="N14" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="O14" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="AW14" s="1" t="s">
+      <c r="AY14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AX14" s="1" t="s">
+      <c r="AZ14" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="BA14" s="1">
+      <c r="BC14" s="1">
         <v>24</v>
       </c>
-      <c r="BD14" s="1" t="s">
+      <c r="BF14" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="15" spans="1:86" ht="238">
+    <row r="15" spans="1:88" ht="238">
       <c r="A15" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>370</v>
-      </c>
       <c r="D15" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>43573</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="I15" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L15" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="M15" s="11" t="s">
+      <c r="N15" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="O15" s="11" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="1:86" ht="238">
+    <row r="16" spans="1:88" ht="238">
       <c r="A16" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>43648</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="L16" s="8" t="s">
+      <c r="N16" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="M16" s="9" t="s">
+      <c r="O16" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="AW16" s="1" t="s">
+      <c r="AY16" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AX16" s="1" t="s">
+      <c r="AZ16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BD16" s="1" t="s">
+      <c r="BF16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BE16" s="1" t="s">
+      <c r="BG16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BF16" s="1" t="s">
+      <c r="BH16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BI16" s="1" t="s">
+      <c r="BK16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BJ16" s="1" t="s">
+      <c r="BL16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BM16" s="1" t="s">
+      <c r="BO16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BN16" s="1" t="s">
+      <c r="BP16" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:86" ht="136">
+    <row r="17" spans="1:88" ht="136">
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>43865</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="L17" s="8" t="s">
+      <c r="N17" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="M17" s="11" t="s">
+      <c r="O17" s="11" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="18" spans="1:86" ht="289">
+    <row r="18" spans="1:88" ht="289">
       <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>388</v>
-      </c>
       <c r="D18" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <v>43775</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="L18" s="8" t="s">
+      <c r="N18" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="M18" s="11" t="s">
+      <c r="O18" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="S18" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="AC18" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="AD18" s="1" t="s">
+      <c r="U18" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AE18" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="AF18" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="AJ18" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="BD18" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="BQ18" s="1" t="s">
+      <c r="AL18" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BF18" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BS18" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="19" spans="1:86" ht="136">
+    <row r="19" spans="1:88" ht="136">
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="F19" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <v>43801</v>
       </c>
-      <c r="H19" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="L19" s="8"/>
-      <c r="M19" s="9"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="9"/>
     </row>
-    <row r="20" spans="1:86" ht="340">
+    <row r="20" spans="1:88" ht="340">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H20" s="2">
         <v>43803</v>
       </c>
-      <c r="H20" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="I20" s="1" t="s">
+      <c r="I20" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="L20" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="M20" s="9" t="s">
-        <v>381</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="AC20" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="AD20" s="1" t="s">
+      <c r="N20" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="O20" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AE20" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="AF20" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="AJ20" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="BQ20" s="1" t="s">
+      <c r="AL20" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BS20" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="21" spans="1:86" ht="204">
+    <row r="21" spans="1:88" ht="204">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>379</v>
-      </c>
       <c r="D21" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G21" s="2">
+      <c r="H21" s="2">
         <v>43648</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="I21" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="L21" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="M21" s="9" t="s">
-        <v>383</v>
-      </c>
-      <c r="AC21" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="AD21" s="1" t="s">
+      <c r="N21" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="O21" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="AF21" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AJ21" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="BQ21" s="1" t="s">
+      <c r="AL21" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BS21" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="22" spans="1:86" ht="204">
+    <row r="22" spans="1:88" ht="204">
       <c r="A22" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>380</v>
-      </c>
       <c r="D22" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="G22" s="2">
+      <c r="H22" s="2">
         <v>43621</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="I22" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="L22" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="M22" s="9" t="s">
+      <c r="N22" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="O22" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="S22" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="AC22" s="1" t="s">
+      <c r="U22" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AE22" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="AD22" s="1" t="s">
+      <c r="AF22" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="AJ22" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="BQ22" s="1" t="s">
+      <c r="AL22" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BS22" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="23" spans="1:86" ht="68">
+    <row r="23" spans="1:88" ht="68">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G23" s="2">
+      <c r="H23" s="2">
         <v>43802</v>
       </c>
-      <c r="H23" s="5"/>
-      <c r="I23" s="1" t="s">
+      <c r="I23" s="5"/>
+      <c r="J23" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="L23" s="8"/>
-      <c r="M23" s="9"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="9"/>
     </row>
-    <row r="24" spans="1:86" ht="182.25" customHeight="1">
+    <row r="24" spans="1:88" ht="182.25" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="F24" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <v>43896</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="I24" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="L24" s="8" t="s">
+      <c r="N24" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="M24" s="9" t="s">
+      <c r="O24" s="9" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="25" spans="1:86" ht="51">
+    <row r="25" spans="1:88" ht="51">
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H25" s="4"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="9"/>
-      <c r="O25" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="P25" s="1">
+      <c r="I25" s="4"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="9"/>
+      <c r="Q25" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="R25" s="1">
         <v>20</v>
       </c>
-      <c r="Q25" s="26" t="s">
+      <c r="S25" s="26" t="s">
         <v>352</v>
       </c>
-      <c r="S25" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="T25" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="V25" s="1">
+      <c r="U25" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="X25" s="1">
         <v>5</v>
       </c>
-      <c r="W25" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="Y25" s="1">
+      <c r="Y25" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AA25" s="1">
         <v>5</v>
       </c>
-      <c r="Z25" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="AB25" s="1">
+      <c r="AB25" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AD25" s="1">
         <v>5</v>
       </c>
-      <c r="AD25" s="1" t="s">
+      <c r="AF25" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="AF25" s="1">
+      <c r="AH25" s="1">
         <v>5</v>
       </c>
-      <c r="AG25" s="1">
+      <c r="AI25" s="1">
         <v>24</v>
       </c>
-      <c r="AH25" s="1">
+      <c r="AJ25" s="1">
         <v>100</v>
       </c>
-      <c r="AI25" s="1">
+      <c r="AK25" s="1">
         <v>400</v>
       </c>
-      <c r="AJ25" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="AK25" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="AM25" s="1">
+      <c r="AL25" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AM25" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AO25" s="1">
         <v>5</v>
       </c>
-      <c r="AN25" s="1">
+      <c r="AP25" s="1">
         <v>5</v>
       </c>
-      <c r="AO25" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="AQ25" s="1">
+      <c r="AQ25" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AS25" s="1">
         <v>5</v>
       </c>
-      <c r="AR25" s="1">
+      <c r="AT25" s="1">
         <v>5</v>
       </c>
-      <c r="AS25" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="AU25" s="1">
+      <c r="AU25" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AW25" s="1">
         <v>5</v>
       </c>
-      <c r="AV25" s="1">
+      <c r="AX25" s="1">
         <v>5</v>
       </c>
-      <c r="AX25" s="1" t="s">
+      <c r="AZ25" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="AZ25" s="1">
+      <c r="BB25" s="1">
         <v>5</v>
       </c>
-      <c r="BA25" s="1">
+      <c r="BC25" s="1">
         <v>24</v>
       </c>
-      <c r="BB25" s="1">
+      <c r="BD25" s="1">
         <v>100</v>
       </c>
-      <c r="BC25" s="1">
+      <c r="BE25" s="1">
         <v>400</v>
       </c>
-      <c r="BD25" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE25" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="BG25" s="1">
+      <c r="BF25" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BG25" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI25" s="1">
         <v>5</v>
       </c>
-      <c r="BH25" s="1">
+      <c r="BJ25" s="1">
         <v>5</v>
       </c>
-      <c r="BI25" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="BK25" s="1">
+      <c r="BK25" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BM25" s="1">
         <v>5</v>
       </c>
-      <c r="BL25" s="1">
+      <c r="BN25" s="1">
         <v>5</v>
       </c>
-      <c r="BM25" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="BO25" s="1">
+      <c r="BO25" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BQ25" s="1">
         <v>5</v>
       </c>
-      <c r="BP25" s="1">
+      <c r="BR25" s="1">
         <v>5</v>
       </c>
-      <c r="BQ25" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="BR25" s="1" t="s">
+      <c r="BS25" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BT25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BS25" s="1" t="s">
+      <c r="BU25" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="BT25" s="1" t="s">
+      <c r="BV25" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="BU25" s="1">
+      <c r="BW25" s="1">
         <v>0.7</v>
       </c>
-      <c r="BV25" s="1" t="s">
+      <c r="BX25" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="BW25" s="1" t="s">
+      <c r="BY25" s="1" t="s">
         <v>356</v>
-      </c>
-      <c r="BX25" s="1">
-        <v>5</v>
-      </c>
-      <c r="BY25" s="1">
-        <v>800</v>
       </c>
       <c r="BZ25" s="1">
         <v>5</v>
       </c>
-      <c r="CA25" s="1" t="s">
-        <v>357</v>
+      <c r="CA25" s="1">
+        <v>800</v>
       </c>
       <c r="CB25" s="1">
         <v>5</v>
       </c>
-      <c r="CC25" s="1">
-        <v>800</v>
+      <c r="CC25" s="1" t="s">
+        <v>357</v>
       </c>
       <c r="CD25" s="1">
         <v>5</v>
       </c>
-      <c r="CE25" s="1" t="s">
-        <v>358</v>
+      <c r="CE25" s="1">
+        <v>800</v>
       </c>
       <c r="CF25" s="1">
         <v>5</v>
       </c>
-      <c r="CG25" s="1">
+      <c r="CG25" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="CH25" s="1">
+        <v>5</v>
+      </c>
+      <c r="CI25" s="1">
         <v>800</v>
       </c>
-      <c r="CH25" s="1">
+      <c r="CJ25" s="1">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
allowing multiple scope options to be selectable
</commit_message>
<xml_diff>
--- a/app/data/wto_proposal_settings_master.xlsx
+++ b/app/data/wto_proposal_settings_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kat/GitHub/SubsidyExplorer/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93EA79C2-B49C-194B-A2FF-D662E23CBB6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366665C3-D760-6442-91A7-B224332DFEE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3700" yWindow="840" windowWidth="26940" windowHeight="25280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18860" yWindow="1120" windowWidth="26940" windowHeight="25280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="429">
   <si>
     <t>proposal</t>
   </si>
@@ -483,9 +483,6 @@
   </si>
   <si>
     <t xml:space="preserve">This communication advocates for placing prohibitions on a Member's subsidies contingent upon, or tied to actual or anticipated, fishing activities in areas beyond that Member's national jurisdiction. </t>
-  </si>
-  <si>
-    <t>LTE</t>
   </si>
   <si>
     <t>This communication advocates for prohibiting subsidies that reduce the operational or capital costs of fishing when one or more of the stocks in the relevant fishery or fisheries being targeted are either 1) being fished with a measure of fishing capacity that is greater than would be required to maintain the stock(s) at a level that would maintain [MSY]; 2) being fished at a rate that is contributing to a decline in the stock(s) below a level that would maintain [MSY]. If the subsidizing Member can demonstrate that it has other policies in place that effectively ensure the stocks(s) are maintained at or above a level required to maintain [MSY], a subsidy that would otherwise be prohibited by either of the above conditions shall be allowed.</t>
@@ -1441,6 +1438,21 @@
   </si>
   <si>
     <t>Subsidies for fishing in a Member's territorial waters are excluded. Prohibition of subsidies to OFOC shall not apply to LDCs. A transition period of 5 years shall be allowed for Overfished and OFOC disciplines for developing country and LDC Members.</t>
+  </si>
+  <si>
+    <t>oa_scope_select</t>
+  </si>
+  <si>
+    <t>SELECT</t>
+  </si>
+  <si>
+    <t>overcap_scope_select</t>
+  </si>
+  <si>
+    <t>LENGTH, TONNAGE, ENGINE</t>
+  </si>
+  <si>
+    <t>iuu_scope_select</t>
   </si>
 </sst>
 </file>
@@ -2424,11 +2436,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CL26"/>
+  <dimension ref="A1:CO26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -2451,7 +2463,7 @@
     <col min="18" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:90" s="11" customFormat="1" ht="68">
+    <row r="1" spans="1:93" s="11" customFormat="1" ht="68">
       <c r="A1" s="17" t="s">
         <v>141</v>
       </c>
@@ -2459,22 +2471,22 @@
         <v>88</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>1</v>
@@ -2483,7 +2495,7 @@
         <v>129</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L1" s="11" t="s">
         <v>2</v>
@@ -2495,13 +2507,13 @@
         <v>4</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="P1" s="14" t="s">
         <v>5</v>
       </c>
       <c r="Q1" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R1" s="11" t="s">
         <v>7</v>
@@ -2516,214 +2528,223 @@
         <v>10</v>
       </c>
       <c r="V1" s="11" t="s">
+        <v>428</v>
+      </c>
+      <c r="W1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="X1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="Y1" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="Z1" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="Y1" s="11" t="s">
+      <c r="AA1" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="AB1" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="AA1" s="11" t="s">
+      <c r="AC1" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="AB1" s="11" t="s">
+      <c r="AD1" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="AC1" s="11" t="s">
+      <c r="AE1" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="AD1" s="11" t="s">
+      <c r="AF1" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="AE1" s="11" t="s">
+      <c r="AG1" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="AF1" s="11" t="s">
+      <c r="AH1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ1" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="AK1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="AN1" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="AG1" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="AI1" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="AJ1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="AK1" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="AL1" s="11" t="s">
+      <c r="AO1" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="AM1" s="11" t="s">
+      <c r="AP1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AQ1" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="AN1" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO1" s="11" t="s">
+      <c r="AR1" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="AP1" s="11" t="s">
+      <c r="AS1" s="11" t="s">
         <v>278</v>
       </c>
-      <c r="AQ1" s="11" t="s">
+      <c r="AT1" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="AR1" s="11" t="s">
+      <c r="AU1" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="AS1" s="11" t="s">
+      <c r="AV1" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="AT1" s="11" t="s">
+      <c r="AW1" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="AU1" s="11" t="s">
+      <c r="AX1" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="AV1" s="11" t="s">
+      <c r="AY1" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="AW1" s="11" t="s">
+      <c r="AZ1" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="AX1" s="11" t="s">
+      <c r="BA1" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="AY1" s="11" t="s">
+      <c r="BB1" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="AZ1" s="11" t="s">
+      <c r="BC1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="BD1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="BE1" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="BF1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="BG1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="BH1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="BI1" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="BA1" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="BB1" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="BC1" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="BD1" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="BE1" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="BF1" s="11" t="s">
+      <c r="BJ1" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="BG1" s="11" t="s">
+      <c r="BK1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="BL1" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="BH1" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="BI1" s="11" t="s">
+      <c r="BM1" s="11" t="s">
         <v>291</v>
       </c>
-      <c r="BJ1" s="11" t="s">
+      <c r="BN1" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="BK1" s="11" t="s">
+      <c r="BO1" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="BL1" s="11" t="s">
+      <c r="BP1" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="BM1" s="11" t="s">
+      <c r="BQ1" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="BN1" s="11" t="s">
+      <c r="BR1" s="11" t="s">
         <v>296</v>
       </c>
-      <c r="BO1" s="11" t="s">
+      <c r="BS1" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="BP1" s="11" t="s">
+      <c r="BT1" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="BQ1" s="11" t="s">
+      <c r="BU1" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="BR1" s="11" t="s">
+      <c r="BV1" s="11" t="s">
         <v>300</v>
       </c>
-      <c r="BS1" s="11" t="s">
+      <c r="BW1" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="BT1" s="11" t="s">
-        <v>302</v>
-      </c>
-      <c r="BU1" s="11" t="s">
+      <c r="BX1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="BV1" s="11" t="s">
+      <c r="BY1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="BW1" s="11" t="s">
+      <c r="BZ1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="BX1" s="11" t="s">
+      <c r="CA1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="BY1" s="11" t="s">
+      <c r="CB1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="BZ1" s="11" t="s">
+      <c r="CC1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="CA1" s="11" t="s">
+      <c r="CD1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="CB1" s="11" t="s">
+      <c r="CE1" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="CC1" s="11" t="s">
+      <c r="CF1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="CD1" s="11" t="s">
+      <c r="CG1" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="CE1" s="11" t="s">
+      <c r="CH1" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="CF1" s="11" t="s">
+      <c r="CI1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="CG1" s="11" t="s">
+      <c r="CJ1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="CH1" s="11" t="s">
+      <c r="CK1" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="CI1" s="11" t="s">
+      <c r="CL1" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="CJ1" s="11" t="s">
+      <c r="CM1" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="CK1" s="11" t="s">
+      <c r="CN1" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="CL1" s="11" t="s">
+      <c r="CO1" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:90" s="11" customFormat="1" ht="282" customHeight="1">
+    <row r="2" spans="1:93" s="11" customFormat="1" ht="282" customHeight="1">
       <c r="A2" s="32" t="s">
         <v>58</v>
       </c>
@@ -2731,19 +2752,19 @@
         <v>98</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>58</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>99</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>55</v>
@@ -2755,7 +2776,7 @@
         <v>43545</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>147</v>
@@ -2764,14 +2785,14 @@
         <v>148</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -2846,8 +2867,11 @@
       <c r="CJ2" s="1"/>
       <c r="CK2" s="1"/>
       <c r="CL2" s="1"/>
+      <c r="CM2" s="1"/>
+      <c r="CN2" s="1"/>
+      <c r="CO2" s="1"/>
     </row>
-    <row r="3" spans="1:90" ht="238">
+    <row r="3" spans="1:93" ht="238">
       <c r="A3" s="32" t="s">
         <v>58</v>
       </c>
@@ -2855,19 +2879,19 @@
         <v>98</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>58</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>108</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>55</v>
@@ -2879,7 +2903,7 @@
         <v>43573</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>110</v>
@@ -2888,34 +2912,34 @@
         <v>111</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P3" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Q3" s="27" t="s">
-        <v>365</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AG3" s="1" t="s">
-        <v>321</v>
+        <v>364</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="AN3" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BH3" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU3" s="1" t="s">
-        <v>304</v>
+        <v>320</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BK3" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BX3" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
-    <row r="4" spans="1:90" ht="306">
+    <row r="4" spans="1:93" ht="306">
       <c r="A4" s="32" t="s">
         <v>58</v>
       </c>
@@ -2923,7 +2947,7 @@
         <v>98</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>58</v>
@@ -2942,7 +2966,7 @@
         <v>43620</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>78</v>
@@ -2951,43 +2975,43 @@
         <v>79</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="P4" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>367</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AN4" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BH4" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU4" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="BV4" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AP4" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BK4" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BX4" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="BY4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="BW4" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="CA4" s="1" t="s">
+      <c r="BZ4" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="CC4" s="1">
+      <c r="CD4" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="CF4" s="1">
         <v>600</v>
       </c>
-      <c r="CD4" s="1">
+      <c r="CG4" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:90" ht="221">
+    <row r="5" spans="1:93" ht="221">
       <c r="A5" s="32" t="s">
         <v>58</v>
       </c>
@@ -2995,19 +3019,19 @@
         <v>124</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>58</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>132</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>55</v>
@@ -3019,7 +3043,7 @@
         <v>43621</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>134</v>
@@ -3028,34 +3052,34 @@
         <v>135</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P5" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AG5" s="1" t="s">
-        <v>358</v>
+        <v>363</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="AN5" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BH5" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU5" s="1" t="s">
-        <v>304</v>
+        <v>357</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="AP5" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BK5" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BX5" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
-    <row r="6" spans="1:90" ht="221">
+    <row r="6" spans="1:93" ht="221">
       <c r="A6" s="32" t="s">
         <v>58</v>
       </c>
@@ -3063,7 +3087,7 @@
         <v>90</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>58</v>
@@ -3081,7 +3105,7 @@
         <v>43628</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>144</v>
@@ -3090,34 +3114,37 @@
         <v>146</v>
       </c>
       <c r="N6" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="P6" s="25" t="s">
         <v>343</v>
       </c>
-      <c r="P6" s="25" t="s">
-        <v>344</v>
-      </c>
       <c r="Q6" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AN6" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BH6" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU6" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AP6" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BK6" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BX6" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
-    <row r="7" spans="1:90" ht="170">
+    <row r="7" spans="1:93" ht="170">
       <c r="A7" s="32" t="s">
         <v>58</v>
       </c>
@@ -3125,13 +3152,13 @@
         <v>98</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>58</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>102</v>
@@ -3146,7 +3173,7 @@
         <v>43643</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>103</v>
@@ -3158,34 +3185,37 @@
         <v>153</v>
       </c>
       <c r="P7" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>368</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AN7" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BA7" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AP7" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BC7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BB7" s="1" t="s">
+      <c r="BD7" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="BE7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BD7" s="1">
+      <c r="BG7" s="1">
         <v>5</v>
       </c>
-      <c r="BH7" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU7" s="1" t="s">
-        <v>304</v>
+      <c r="BK7" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BX7" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:90" ht="238">
+    <row r="8" spans="1:93" ht="238">
       <c r="A8" s="32" t="s">
         <v>58</v>
       </c>
@@ -3193,19 +3223,19 @@
         <v>98</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D8" s="28" t="s">
         <v>58</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>114</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>55</v>
@@ -3217,7 +3247,7 @@
         <v>43648</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>115</v>
@@ -3226,49 +3256,49 @@
         <v>116</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>369</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AN8" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BA8" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AP8" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BC8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BB8" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="BH8" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="BI8" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="BJ8" s="1" t="s">
-        <v>303</v>
+      <c r="BD8" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="BK8" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="BL8" s="1" t="s">
+        <v>310</v>
       </c>
       <c r="BM8" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="BN8" s="1" t="s">
-        <v>336</v>
+        <v>302</v>
+      </c>
+      <c r="BP8" s="1" t="s">
+        <v>310</v>
       </c>
       <c r="BQ8" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU8" s="1" t="s">
-        <v>304</v>
+        <v>335</v>
+      </c>
+      <c r="BT8" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BX8" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
-    <row r="9" spans="1:90" ht="187">
+    <row r="9" spans="1:93" ht="187">
       <c r="A9" s="32" t="s">
         <v>58</v>
       </c>
@@ -3276,7 +3306,7 @@
         <v>124</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>58</v>
@@ -3285,7 +3315,7 @@
         <v>130</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>55</v>
@@ -3297,7 +3327,7 @@
         <v>43648</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>131</v>
@@ -3306,34 +3336,37 @@
         <v>116</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="P9" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>371</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AG9" s="1" t="s">
-        <v>358</v>
+        <v>370</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="AH9" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="AN9" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BH9" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU9" s="1" t="s">
-        <v>304</v>
+        <v>357</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="AP9" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BK9" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BX9" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
-    <row r="10" spans="1:90" ht="204">
+    <row r="10" spans="1:93" ht="204">
       <c r="A10" s="32" t="s">
         <v>58</v>
       </c>
@@ -3341,7 +3374,7 @@
         <v>98</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>58</v>
@@ -3350,7 +3383,7 @@
         <v>68</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>58</v>
@@ -3362,7 +3395,7 @@
         <v>43657</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>70</v>
@@ -3371,55 +3404,55 @@
         <v>128</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P10" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="W10" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AP10" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BK10" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BX10" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="BY10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BZ10" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="AN10" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BH10" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU10" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="BV10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BW10" s="1" t="s">
+      <c r="CA10" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="BX10" s="1" t="s">
+      <c r="CC10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="CD10" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="BZ10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="CA10" s="1" t="s">
+      <c r="CG10" s="1">
+        <v>90</v>
+      </c>
+      <c r="CH10" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="CD10" s="1">
-        <v>90</v>
-      </c>
-      <c r="CE10" s="1" t="s">
+      <c r="CI10" s="1">
+        <v>50</v>
+      </c>
+      <c r="CL10" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="CF10" s="1">
-        <v>50</v>
-      </c>
-      <c r="CI10" s="1" t="s">
-        <v>309</v>
-      </c>
     </row>
-    <row r="11" spans="1:90" ht="187">
+    <row r="11" spans="1:93" ht="187">
       <c r="A11" s="32" t="s">
         <v>58</v>
       </c>
@@ -3427,13 +3460,13 @@
         <v>98</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D11" s="28" t="s">
         <v>58</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>106</v>
@@ -3448,7 +3481,7 @@
         <v>43684</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>112</v>
@@ -3457,43 +3490,46 @@
         <v>113</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="P11" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>374</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AN11" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BA11" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AP11" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BC11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BB11" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="BE11" s="1">
+      <c r="BD11" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="BE11" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="BH11" s="1">
         <v>24</v>
       </c>
-      <c r="BF11" s="1">
+      <c r="BI11" s="1">
         <v>100</v>
       </c>
-      <c r="BG11" s="1">
+      <c r="BJ11" s="1">
         <v>130</v>
       </c>
-      <c r="BH11" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU11" s="1" t="s">
-        <v>304</v>
+      <c r="BK11" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BX11" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
-    <row r="12" spans="1:90" ht="119">
+    <row r="12" spans="1:93" ht="119">
       <c r="A12" s="33" t="s">
         <v>58</v>
       </c>
@@ -3501,7 +3537,7 @@
         <v>90</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>58</v>
@@ -3520,7 +3556,7 @@
         <v>43718</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>94</v>
@@ -3532,34 +3568,34 @@
         <v>151</v>
       </c>
       <c r="P12" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Q12" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="R12" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="R12" s="1" t="s">
-        <v>264</v>
-      </c>
       <c r="S12" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AN12" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BH12" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU12" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AP12" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BK12" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BX12" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
-    <row r="13" spans="1:90" ht="136.5" customHeight="1">
+    <row r="13" spans="1:93" ht="136.5" customHeight="1">
       <c r="A13" s="32" t="s">
         <v>58</v>
       </c>
@@ -3567,7 +3603,7 @@
         <v>89</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D13" s="28" t="s">
         <v>58</v>
@@ -3576,7 +3612,7 @@
         <v>85</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>58</v>
@@ -3588,7 +3624,7 @@
         <v>43759</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>86</v>
@@ -3597,37 +3633,40 @@
         <v>87</v>
       </c>
       <c r="N13" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="O13" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="P13" s="25" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q13" s="8" t="s">
         <v>372</v>
       </c>
-      <c r="O13" s="17" t="s">
-        <v>329</v>
-      </c>
-      <c r="P13" s="25" t="s">
-        <v>344</v>
-      </c>
-      <c r="Q13" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AN13" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BA13" s="1" t="s">
+      <c r="X13" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AP13" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BC13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BB13" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="BH13" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU13" s="1" t="s">
-        <v>304</v>
+      <c r="BD13" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="BE13" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="BK13" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BX13" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
-    <row r="14" spans="1:90" ht="289">
+    <row r="14" spans="1:93" ht="289">
       <c r="A14" s="32" t="s">
         <v>58</v>
       </c>
@@ -3635,19 +3674,19 @@
         <v>98</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>58</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>55</v>
@@ -3659,7 +3698,7 @@
         <v>43775</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>118</v>
@@ -3668,55 +3707,58 @@
         <v>119</v>
       </c>
       <c r="N14" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="P14" s="7" t="s">
         <v>376</v>
       </c>
-      <c r="P14" s="7" t="s">
+      <c r="Q14" s="27" t="s">
         <v>377</v>
       </c>
-      <c r="Q14" s="27" t="s">
-        <v>378</v>
-      </c>
-      <c r="W14" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AG14" s="1" t="s">
-        <v>321</v>
+      <c r="X14" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="AH14" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="AN14" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="AI14" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="AJ14" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="AP14" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="AQ14" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="AR14" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="AO14" s="1" t="s">
+      <c r="AT14" s="1">
+        <v>6</v>
+      </c>
+      <c r="AU14" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="AV14" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="AP14" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="AR14" s="1">
-        <v>6</v>
-      </c>
-      <c r="AS14" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="AT14" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="AV14" s="1">
+      <c r="AX14" s="1">
         <v>4</v>
       </c>
-      <c r="AW14" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BH14" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU14" s="1" t="s">
-        <v>304</v>
+      <c r="AY14" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BK14" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BX14" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
-    <row r="15" spans="1:90" ht="204">
+    <row r="15" spans="1:93" ht="204">
       <c r="A15" s="32" t="s">
         <v>58</v>
       </c>
@@ -3724,7 +3766,7 @@
         <v>90</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D15" s="28" t="s">
         <v>58</v>
@@ -3733,7 +3775,7 @@
         <v>91</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>55</v>
@@ -3745,46 +3787,46 @@
         <v>43801</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>92</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="P15" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Q15" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="W15" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AN15" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BH15" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU15" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AP15" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BK15" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BX15" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
-    <row r="16" spans="1:90" ht="85">
+    <row r="16" spans="1:93" ht="85">
       <c r="A16" s="32" t="s">
         <v>55</v>
       </c>
@@ -3795,7 +3837,7 @@
         <v>58</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>100</v>
@@ -3810,7 +3852,7 @@
         <v>43801</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>149</v>
@@ -3824,7 +3866,7 @@
       <c r="P16" s="7"/>
       <c r="Q16" s="8"/>
     </row>
-    <row r="17" spans="1:90" ht="136">
+    <row r="17" spans="1:93" ht="136">
       <c r="A17" s="32" t="s">
         <v>55</v>
       </c>
@@ -3835,7 +3877,7 @@
         <v>58</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>120</v>
@@ -3851,7 +3893,7 @@
         <v>43801</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>122</v>
@@ -3860,12 +3902,12 @@
         <v>123</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P17" s="7"/>
       <c r="Q17" s="8"/>
     </row>
-    <row r="18" spans="1:90" ht="68">
+    <row r="18" spans="1:93" ht="68">
       <c r="A18" s="32" t="s">
         <v>55</v>
       </c>
@@ -3876,7 +3918,7 @@
         <v>58</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>136</v>
@@ -3891,7 +3933,7 @@
         <v>43802</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>137</v>
@@ -3900,12 +3942,12 @@
         <v>138</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P18" s="7"/>
       <c r="Q18" s="8"/>
     </row>
-    <row r="19" spans="1:90" ht="340">
+    <row r="19" spans="1:93" ht="340">
       <c r="A19" s="32" t="s">
         <v>58</v>
       </c>
@@ -3913,13 +3955,13 @@
         <v>124</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D19" s="28" t="s">
         <v>58</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>125</v>
@@ -3934,7 +3976,7 @@
         <v>43803</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>126</v>
@@ -3943,34 +3985,34 @@
         <v>127</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="P19" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Q19" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="W19" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AG19" s="1" t="s">
-        <v>321</v>
+        <v>369</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="AH19" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="AN19" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BH19" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU19" s="1" t="s">
-        <v>304</v>
+        <v>320</v>
+      </c>
+      <c r="AI19" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="AP19" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BK19" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BX19" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
-    <row r="20" spans="1:90" ht="255">
+    <row r="20" spans="1:93" ht="255">
       <c r="A20" s="32" t="s">
         <v>58</v>
       </c>
@@ -3978,74 +4020,77 @@
         <v>98</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>58</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J20" s="2">
         <v>43843</v>
       </c>
       <c r="K20" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>249</v>
-      </c>
       <c r="M20" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="N20" s="26" t="s">
         <v>356</v>
-      </c>
-      <c r="N20" s="26" t="s">
-        <v>357</v>
       </c>
       <c r="O20" s="6"/>
       <c r="P20" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Q20" s="27" t="s">
-        <v>387</v>
-      </c>
-      <c r="W20" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AG20" s="1" t="s">
-        <v>321</v>
+        <v>386</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="AH20" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="AN20" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BA20" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="AI20" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="AP20" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BC20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BB20" s="1" t="s">
+      <c r="BD20" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="BE20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BD20" s="1">
+      <c r="BG20" s="1">
         <v>5</v>
       </c>
-      <c r="BH20" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU20" s="1" t="s">
-        <v>304</v>
+      <c r="BK20" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BX20" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
-    <row r="21" spans="1:90" ht="153">
+    <row r="21" spans="1:93" ht="153">
       <c r="A21" s="32" t="s">
         <v>58</v>
       </c>
@@ -4053,19 +4098,19 @@
         <v>90</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>58</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>55</v>
@@ -4077,7 +4122,7 @@
         <v>43865</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>142</v>
@@ -4086,64 +4131,64 @@
         <v>116</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="P21" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Q21" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="R21" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="X21" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="S21" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="U21" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="W21" s="1" t="s">
+      <c r="Y21" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="Z21" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="X21" s="1" t="s">
+      <c r="AA21" s="1">
+        <v>5</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="AC21" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="Y21" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="Z21" s="1">
+      <c r="AD21" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="AF21" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="AG21" s="1">
         <v>5</v>
       </c>
-      <c r="AA21" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="AB21" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="AC21" s="1">
-        <v>3</v>
-      </c>
-      <c r="AD21" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="AE21" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="AF21" s="1">
-        <v>5</v>
-      </c>
-      <c r="AN21" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BH21" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU21" s="1" t="s">
-        <v>304</v>
+      <c r="AP21" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BK21" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BX21" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
-    <row r="22" spans="1:90" ht="323">
+    <row r="22" spans="1:93" ht="323">
       <c r="A22" s="32" t="s">
         <v>58</v>
       </c>
@@ -4151,16 +4196,16 @@
         <v>98</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>58</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>55</v>
@@ -4172,58 +4217,58 @@
         <v>43865</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>115</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="P22" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="Q22" s="29" t="s">
         <v>388</v>
       </c>
-      <c r="Q22" s="29" t="s">
+      <c r="X22" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AP22" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BC22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BD22" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="BK22" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="BL22" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="BM22" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="BP22" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="BQ22" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="W22" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AN22" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BA22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BB22" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="BH22" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="BI22" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="BJ22" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="BM22" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="BN22" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="BQ22" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU22" s="1" t="s">
-        <v>304</v>
+      <c r="BT22" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BX22" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
-    <row r="23" spans="1:90" ht="323">
+    <row r="23" spans="1:93" ht="323">
       <c r="A23" s="17" t="s">
         <v>58</v>
       </c>
@@ -4231,61 +4276,63 @@
         <v>89</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D23" s="24" t="s">
         <v>58</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G23" s="11"/>
       <c r="H23" s="17" t="s">
         <v>55</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J23" s="16">
         <v>43896</v>
       </c>
       <c r="K23" s="13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="N23" s="17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="O23" s="17" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P23" s="18" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="Q23" s="19" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S23" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="T23" s="11"/>
-      <c r="U23" s="11"/>
+      <c r="U23" s="11" t="s">
+        <v>302</v>
+      </c>
       <c r="V23" s="11"/>
-      <c r="W23" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="X23" s="11"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11" t="s">
+        <v>303</v>
+      </c>
       <c r="Y23" s="11"/>
       <c r="Z23" s="11"/>
       <c r="AA23" s="11"/>
@@ -4294,92 +4341,96 @@
       <c r="AD23" s="11"/>
       <c r="AE23" s="11"/>
       <c r="AF23" s="11"/>
-      <c r="AG23" s="11" t="s">
-        <v>321</v>
-      </c>
+      <c r="AG23" s="11"/>
       <c r="AH23" s="11" t="s">
-        <v>331</v>
-      </c>
-      <c r="AI23" s="11"/>
-      <c r="AJ23" s="11"/>
+        <v>320</v>
+      </c>
+      <c r="AI23" s="11" t="s">
+        <v>425</v>
+      </c>
+      <c r="AJ23" s="11" t="s">
+        <v>330</v>
+      </c>
       <c r="AK23" s="11"/>
       <c r="AL23" s="11"/>
       <c r="AM23" s="11"/>
-      <c r="AN23" s="11" t="s">
+      <c r="AN23" s="11"/>
+      <c r="AO23" s="11"/>
+      <c r="AP23" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="AQ23" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="AR23" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="AO23" s="11" t="s">
+      <c r="AS23" s="11"/>
+      <c r="AT23" s="11">
+        <v>5</v>
+      </c>
+      <c r="AU23" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="AV23" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="AP23" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="AQ23" s="11"/>
-      <c r="AR23" s="11">
+      <c r="AW23" s="11"/>
+      <c r="AX23" s="11">
         <v>5</v>
       </c>
-      <c r="AS23" s="11" t="s">
-        <v>311</v>
-      </c>
-      <c r="AT23" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="AU23" s="11"/>
-      <c r="AV23" s="11">
-        <v>5</v>
-      </c>
-      <c r="AW23" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="AX23" s="11"/>
-      <c r="AY23" s="11"/>
+      <c r="AY23" s="11" t="s">
+        <v>303</v>
+      </c>
       <c r="AZ23" s="11"/>
-      <c r="BA23" s="1" t="s">
+      <c r="BA23" s="11"/>
+      <c r="BB23" s="11"/>
+      <c r="BC23" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BB23" s="11" t="s">
-        <v>396</v>
-      </c>
-      <c r="BC23" s="11"/>
-      <c r="BD23" s="11"/>
-      <c r="BE23" s="11">
-        <v>24</v>
+      <c r="BD23" s="11" t="s">
+        <v>425</v>
+      </c>
+      <c r="BE23" s="11" t="s">
+        <v>395</v>
       </c>
       <c r="BF23" s="11"/>
       <c r="BG23" s="11"/>
-      <c r="BH23" s="11" t="s">
+      <c r="BH23" s="11">
+        <v>24</v>
+      </c>
+      <c r="BI23" s="11"/>
+      <c r="BJ23" s="11"/>
+      <c r="BK23" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="BL23" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="BM23" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="BN23" s="11"/>
+      <c r="BO23" s="11"/>
+      <c r="BP23" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="BQ23" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="BI23" s="11" t="s">
-        <v>311</v>
-      </c>
-      <c r="BJ23" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="BK23" s="11"/>
-      <c r="BL23" s="11"/>
-      <c r="BM23" s="11" t="s">
-        <v>311</v>
-      </c>
-      <c r="BN23" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="BO23" s="11"/>
-      <c r="BP23" s="11">
+      <c r="BR23" s="11"/>
+      <c r="BS23" s="11">
         <v>5</v>
       </c>
-      <c r="BQ23" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="BR23" s="11"/>
-      <c r="BS23" s="11"/>
-      <c r="BT23" s="11"/>
-      <c r="BU23" s="11" t="s">
-        <v>304</v>
-      </c>
+      <c r="BT23" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="BU23" s="11"/>
       <c r="BV23" s="11"/>
       <c r="BW23" s="11"/>
-      <c r="BX23" s="11"/>
+      <c r="BX23" s="11" t="s">
+        <v>303</v>
+      </c>
       <c r="BY23" s="11"/>
       <c r="BZ23" s="11"/>
       <c r="CA23" s="11"/>
@@ -4394,8 +4445,11 @@
       <c r="CJ23" s="11"/>
       <c r="CK23" s="11"/>
       <c r="CL23" s="11"/>
+      <c r="CM23" s="11"/>
+      <c r="CN23" s="11"/>
+      <c r="CO23" s="11"/>
     </row>
-    <row r="24" spans="1:90" ht="182.25" customHeight="1">
+    <row r="24" spans="1:93" ht="182.25" customHeight="1">
       <c r="A24" s="32" t="s">
         <v>58</v>
       </c>
@@ -4403,16 +4457,16 @@
         <v>89</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>58</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G24" s="10"/>
       <c r="H24" s="10" t="s">
@@ -4425,25 +4479,25 @@
         <v>43896</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>140</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="P24" s="34" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
-    <row r="25" spans="1:90" ht="182.25" customHeight="1">
+    <row r="25" spans="1:93" ht="182.25" customHeight="1">
       <c r="A25" s="32" t="s">
         <v>58</v>
       </c>
@@ -4451,41 +4505,41 @@
         <v>98</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>58</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G25" s="10"/>
       <c r="H25" s="10" t="s">
         <v>55</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="J25" s="2">
         <v>43899</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="P25" s="7"/>
       <c r="Q25" s="8"/>
     </row>
-    <row r="26" spans="1:90" ht="51">
+    <row r="26" spans="1:93" ht="51">
       <c r="A26" s="32" t="s">
         <v>58</v>
       </c>
@@ -4502,182 +4556,183 @@
       <c r="P26" s="7"/>
       <c r="Q26" s="8"/>
       <c r="S26" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="T26" s="1">
         <v>20</v>
       </c>
       <c r="U26" s="22" t="s">
-        <v>303</v>
-      </c>
-      <c r="W26" s="1" t="s">
-        <v>304</v>
-      </c>
+        <v>302</v>
+      </c>
+      <c r="V26" s="22"/>
       <c r="X26" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="Z26" s="1">
+        <v>303</v>
+      </c>
+      <c r="Y26" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AA26" s="1">
         <v>5</v>
       </c>
-      <c r="AA26" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AC26" s="1">
+      <c r="AB26" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AD26" s="1">
         <v>5</v>
       </c>
-      <c r="AD26" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AF26" s="1">
+      <c r="AE26" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AG26" s="1">
         <v>5</v>
       </c>
-      <c r="AH26" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="AJ26" s="1">
+      <c r="AI26" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="AL26" s="1">
         <v>5</v>
       </c>
-      <c r="AK26" s="1">
+      <c r="AM26" s="1">
         <v>24</v>
       </c>
-      <c r="AL26" s="1">
+      <c r="AN26" s="1">
         <v>100</v>
       </c>
-      <c r="AM26" s="1">
+      <c r="AO26" s="1">
         <v>400</v>
       </c>
-      <c r="AN26" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AO26" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AQ26" s="1">
+      <c r="AP26" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AQ26" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AS26" s="1">
         <v>5</v>
       </c>
-      <c r="AR26" s="1">
+      <c r="AT26" s="1">
         <v>5</v>
       </c>
-      <c r="AS26" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AU26" s="1">
+      <c r="AU26" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AW26" s="1">
         <v>5</v>
       </c>
-      <c r="AV26" s="1">
+      <c r="AX26" s="1">
         <v>5</v>
       </c>
-      <c r="AW26" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AY26" s="1">
+      <c r="AY26" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BA26" s="1">
         <v>5</v>
       </c>
-      <c r="AZ26" s="1">
+      <c r="BB26" s="1">
         <v>5</v>
       </c>
-      <c r="BB26" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="BD26" s="1">
+      <c r="BD26" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="BG26" s="1">
         <v>5</v>
       </c>
-      <c r="BE26" s="1">
+      <c r="BH26" s="1">
         <v>24</v>
       </c>
-      <c r="BF26" s="1">
+      <c r="BI26" s="1">
         <v>100</v>
       </c>
-      <c r="BG26" s="1">
+      <c r="BJ26" s="1">
         <v>400</v>
       </c>
-      <c r="BH26" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BI26" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BK26" s="1">
+      <c r="BK26" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BL26" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BN26" s="1">
         <v>5</v>
-      </c>
-      <c r="BL26" s="1">
-        <v>5</v>
-      </c>
-      <c r="BM26" s="1" t="s">
-        <v>304</v>
       </c>
       <c r="BO26" s="1">
         <v>5</v>
       </c>
-      <c r="BP26" s="1">
+      <c r="BP26" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BR26" s="1">
         <v>5</v>
-      </c>
-      <c r="BQ26" s="1" t="s">
-        <v>304</v>
       </c>
       <c r="BS26" s="1">
         <v>5</v>
       </c>
-      <c r="BT26" s="1">
+      <c r="BT26" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BV26" s="1">
         <v>5</v>
       </c>
-      <c r="BU26" s="1" t="s">
+      <c r="BW26" s="1">
+        <v>5</v>
+      </c>
+      <c r="BX26" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BY26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BZ26" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="BV26" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BW26" s="1" t="s">
+      <c r="CA26" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="BX26" s="1" t="s">
+      <c r="CB26" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="CC26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CD26" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="BY26" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="BZ26" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="CA26" s="1" t="s">
+      <c r="CE26" s="1">
+        <v>5</v>
+      </c>
+      <c r="CF26" s="1">
+        <v>800</v>
+      </c>
+      <c r="CG26" s="1">
+        <v>5</v>
+      </c>
+      <c r="CH26" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="CB26" s="1">
+      <c r="CI26" s="1">
         <v>5</v>
       </c>
-      <c r="CC26" s="1">
+      <c r="CJ26" s="1">
         <v>800</v>
       </c>
-      <c r="CD26" s="1">
+      <c r="CK26" s="1">
         <v>5</v>
       </c>
-      <c r="CE26" s="1" t="s">
+      <c r="CL26" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="CF26" s="1">
+      <c r="CM26" s="1">
         <v>5</v>
       </c>
-      <c r="CG26" s="1">
+      <c r="CN26" s="1">
         <v>800</v>
       </c>
-      <c r="CH26" s="1">
-        <v>5</v>
-      </c>
-      <c r="CI26" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="CJ26" s="1">
-        <v>5</v>
-      </c>
-      <c r="CK26" s="1">
-        <v>800</v>
-      </c>
-      <c r="CL26" s="1">
+      <c r="CO26" s="1">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:CL26">
+  <sortState ref="A2:CO26">
     <sortCondition ref="J2:J26"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4891,13 +4946,13 @@
         <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>54</v>
@@ -4906,22 +4961,22 @@
         <v>42922</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>55</v>
@@ -4942,7 +4997,7 @@
         <v>60</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AF2" s="1" t="s">
         <v>57</v>
@@ -4965,34 +5020,34 @@
         <v>55</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="F3" s="2">
         <v>42852</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="L3" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>55</v>
@@ -5027,37 +5082,37 @@
         <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="F4" s="2">
         <v>42941</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>55</v>
@@ -5092,34 +5147,34 @@
         <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="F5" s="2">
         <v>42929</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="L5" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>55</v>
@@ -5154,31 +5209,31 @@
         <v>90</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="F6" s="2">
         <v>42941</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="L6" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>55</v>
@@ -5192,37 +5247,37 @@
         <v>55</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="F7" s="2">
         <v>42930</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="L7" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>57</v>
@@ -5263,37 +5318,37 @@
         <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="F8" s="2">
         <v>42933</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="L8" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>57</v>
@@ -5311,7 +5366,7 @@
         <v>55</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AF8" s="1" t="s">
         <v>57</v>
@@ -5337,10 +5392,10 @@
         <v>90</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>66</v>
@@ -5349,22 +5404,22 @@
         <v>43040</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>216</v>
-      </c>
       <c r="L9" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>57</v>
@@ -5381,10 +5436,10 @@
         <v>89</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>67</v>
@@ -5393,25 +5448,25 @@
         <v>43055</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="AE10" s="1" t="s">
         <v>61</v>
       </c>
       <c r="AF10" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AJ10" s="1" t="s">
         <v>55</v>
@@ -5422,7 +5477,7 @@
         <v>55</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>68</v>
@@ -5437,16 +5492,16 @@
         <v>70</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="AO11" s="1" t="s">
         <v>58</v>
@@ -5484,10 +5539,10 @@
         <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>77</v>
@@ -5505,13 +5560,13 @@
         <v>79</v>
       </c>
       <c r="I12" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="AO12" s="1" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
proposal results together working
</commit_message>
<xml_diff>
--- a/app/data/wto_proposal_settings_master.xlsx
+++ b/app/data/wto_proposal_settings_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kat/GitHub/SubsidyExplorer/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C80FCBD-1864-9048-9139-002C10F6F5FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A6FB34-C4B0-4B41-9D95-9713052C61A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35600" yWindow="-1980" windowWidth="34660" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="1" r:id="rId1"/>
@@ -2365,9 +2365,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CO26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P24" sqref="P24"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
adding new sliders for "best" cap option
</commit_message>
<xml_diff>
--- a/app/data/wto_proposal_settings_master.xlsx
+++ b/app/data/wto_proposal_settings_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kat/GitHub/SubsidyExplorer/app/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kat/GitHub/SubsidyExplorer/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259B112C-A482-494C-B214-AF84A500EBF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20387D3A-3246-FB48-8630-DA449BA5FEFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35700" yWindow="-2240" windowWidth="35700" windowHeight="19140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3300" windowWidth="35700" windowHeight="19140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="1" r:id="rId1"/>
@@ -1068,9 +1068,6 @@
   </si>
   <si>
     <t>doc_in_folder</t>
-  </si>
-  <si>
-    <t>Missing "best of" option</t>
   </si>
   <si>
     <t xml:space="preserve">This unofficial room document was circulated at the request of the Delegation of Canada on January 13, 2020. </t>
@@ -1396,17 +1393,20 @@
     <t>B1, B3, B4, B5, B6, B7, C1, C2, C3</t>
   </si>
   <si>
-    <t>FISHERS</t>
-  </si>
-  <si>
     <t>B1, B2, B3, B4, B5, B6, B7, C1, C2, C3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Missing "best of" option; also fix "per fisher" calculation. </t>
+  </si>
+  <si>
+    <t>BEST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1931,7 +1931,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2012,6 +2012,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2371,12 +2374,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CO26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="BP1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="CI5" sqref="CI5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="13"/>
     <col min="2" max="2" width="10.83203125" style="15"/>
@@ -2393,10 +2396,12 @@
     <col min="14" max="15" width="48.33203125" style="16" customWidth="1"/>
     <col min="16" max="16" width="56.1640625" style="15" customWidth="1"/>
     <col min="17" max="17" width="71" style="15" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="16"/>
+    <col min="18" max="84" width="10.83203125" style="16"/>
+    <col min="85" max="85" width="10.83203125" style="28"/>
+    <col min="86" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:93" s="9" customFormat="1" ht="42">
+    <row r="1" spans="1:93" s="9" customFormat="1" ht="42" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>141</v>
       </c>
@@ -2416,7 +2421,7 @@
         <v>0</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>260</v>
@@ -2461,7 +2466,7 @@
         <v>10</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="W1" s="9" t="s">
         <v>11</v>
@@ -2503,7 +2508,7 @@
         <v>17</v>
       </c>
       <c r="AJ1" s="9" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AK1" s="9" t="s">
         <v>18</v>
@@ -2566,7 +2571,7 @@
         <v>27</v>
       </c>
       <c r="BE1" s="9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="BF1" s="9" t="s">
         <v>28</v>
@@ -2677,7 +2682,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:93" s="9" customFormat="1" ht="282" customHeight="1">
+    <row r="2" spans="1:93" s="9" customFormat="1" ht="282" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>55</v>
       </c>
@@ -2691,13 +2696,13 @@
         <v>58</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>99</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H2" s="16" t="s">
         <v>55</v>
@@ -2725,7 +2730,7 @@
         <v>345</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="R2" s="16"/>
       <c r="S2" s="16"/>
@@ -2794,7 +2799,7 @@
       <c r="CD2" s="16"/>
       <c r="CE2" s="16"/>
       <c r="CF2" s="16"/>
-      <c r="CG2" s="16"/>
+      <c r="CG2" s="28"/>
       <c r="CH2" s="16"/>
       <c r="CI2" s="16"/>
       <c r="CJ2" s="16"/>
@@ -2804,7 +2809,7 @@
       <c r="CN2" s="16"/>
       <c r="CO2" s="16"/>
     </row>
-    <row r="3" spans="1:93" ht="182">
+    <row r="3" spans="1:93" ht="182" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>58</v>
       </c>
@@ -2818,13 +2823,13 @@
         <v>58</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>108</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H3" s="16" t="s">
         <v>55</v>
@@ -2851,7 +2856,7 @@
         <v>339</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="X3" s="16" t="s">
         <v>301</v>
@@ -2872,7 +2877,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:93" ht="238">
+    <row r="4" spans="1:93" ht="238" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>58</v>
       </c>
@@ -2880,7 +2885,7 @@
         <v>98</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>349</v>
+        <v>435</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>58</v>
@@ -2914,7 +2919,7 @@
         <v>339</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="X4" s="16" t="s">
         <v>301</v>
@@ -2929,22 +2934,25 @@
         <v>308</v>
       </c>
       <c r="BY4" s="16" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="BZ4" s="16" t="s">
         <v>320</v>
       </c>
       <c r="CD4" s="16" t="s">
-        <v>435</v>
-      </c>
-      <c r="CF4" s="16">
-        <v>600</v>
-      </c>
-      <c r="CG4" s="16">
-        <v>90</v>
+        <v>436</v>
+      </c>
+      <c r="CG4" s="28">
+        <v>55</v>
+      </c>
+      <c r="CK4" s="16">
+        <v>2.1</v>
+      </c>
+      <c r="CO4" s="16">
+        <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:93" ht="182">
+    <row r="5" spans="1:93" ht="182" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>58</v>
       </c>
@@ -2961,7 +2969,7 @@
         <v>132</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H5" s="16" t="s">
         <v>55</v>
@@ -2988,13 +2996,13 @@
         <v>339</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="X5" s="16" t="s">
         <v>301</v>
       </c>
       <c r="AH5" s="16" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AI5" s="16" t="s">
         <v>300</v>
@@ -3009,7 +3017,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="6" spans="1:93" ht="182">
+    <row r="6" spans="1:93" ht="182" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>58</v>
       </c>
@@ -3074,7 +3082,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="7" spans="1:93" ht="126">
+    <row r="7" spans="1:93" ht="126" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>58</v>
       </c>
@@ -3082,13 +3090,13 @@
         <v>98</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>58</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>102</v>
@@ -3118,7 +3126,7 @@
         <v>339</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="X7" s="16" t="s">
         <v>301</v>
@@ -3130,7 +3138,7 @@
         <v>61</v>
       </c>
       <c r="BD7" s="16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BE7" s="16" t="s">
         <v>62</v>
@@ -3145,7 +3153,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="8" spans="1:93" ht="182">
+    <row r="8" spans="1:93" ht="182" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>58</v>
       </c>
@@ -3165,7 +3173,7 @@
         <v>114</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H8" s="16" t="s">
         <v>55</v>
@@ -3186,13 +3194,13 @@
         <v>116</v>
       </c>
       <c r="N8" s="16" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="P8" s="19" t="s">
         <v>155</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="X8" s="16" t="s">
         <v>301</v>
@@ -3228,7 +3236,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="9" spans="1:93" ht="140">
+    <row r="9" spans="1:93" ht="140" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>58</v>
       </c>
@@ -3245,7 +3253,7 @@
         <v>130</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>55</v>
@@ -3266,22 +3274,22 @@
         <v>116</v>
       </c>
       <c r="N9" s="16" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="P9" s="21" t="s">
         <v>339</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="X9" s="16" t="s">
         <v>301</v>
       </c>
       <c r="AH9" s="16" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AI9" s="16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AJ9" s="16" t="s">
         <v>326</v>
@@ -3296,7 +3304,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="10" spans="1:93" ht="154">
+    <row r="10" spans="1:93" ht="154" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>55</v>
       </c>
@@ -3313,7 +3321,7 @@
         <v>68</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H10" s="15" t="s">
         <v>58</v>
@@ -3340,7 +3348,7 @@
         <v>339</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="X10" s="16" t="s">
         <v>301</v>
@@ -3355,7 +3363,7 @@
         <v>308</v>
       </c>
       <c r="BY10" s="16" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="BZ10" s="16" t="s">
         <v>302</v>
@@ -3369,7 +3377,7 @@
       <c r="CD10" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="CG10" s="16">
+      <c r="CG10" s="28">
         <v>90</v>
       </c>
       <c r="CH10" s="16" t="s">
@@ -3382,7 +3390,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="11" spans="1:93" ht="154">
+    <row r="11" spans="1:93" ht="154" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>58</v>
       </c>
@@ -3420,13 +3428,13 @@
         <v>113</v>
       </c>
       <c r="N11" s="16" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P11" s="21" t="s">
         <v>339</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="X11" s="16" t="s">
         <v>301</v>
@@ -3438,10 +3446,10 @@
         <v>61</v>
       </c>
       <c r="BD11" s="16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BE11" s="16" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="BH11" s="16">
         <v>24</v>
@@ -3459,7 +3467,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="12" spans="1:93" ht="84">
+    <row r="12" spans="1:93" ht="84" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>58</v>
       </c>
@@ -3500,7 +3508,7 @@
         <v>339</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="R12" s="16" t="s">
         <v>261</v>
@@ -3524,7 +3532,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="13" spans="1:93" ht="136.5" customHeight="1">
+    <row r="13" spans="1:93" ht="136.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>58</v>
       </c>
@@ -3541,7 +3549,7 @@
         <v>85</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H13" s="15" t="s">
         <v>58</v>
@@ -3553,7 +3561,7 @@
         <v>43759</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L13" s="16" t="s">
         <v>86</v>
@@ -3562,7 +3570,7 @@
         <v>87</v>
       </c>
       <c r="N13" s="16" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="O13" s="6" t="s">
         <v>324</v>
@@ -3571,7 +3579,7 @@
         <v>339</v>
       </c>
       <c r="Q13" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="X13" s="16" t="s">
         <v>301</v>
@@ -3583,7 +3591,7 @@
         <v>61</v>
       </c>
       <c r="BD13" s="16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BE13" s="16" t="s">
         <v>262</v>
@@ -3595,7 +3603,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="14" spans="1:93" ht="224">
+    <row r="14" spans="1:93" ht="224" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>58</v>
       </c>
@@ -3603,7 +3611,7 @@
         <v>98</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>58</v>
@@ -3615,7 +3623,7 @@
         <v>253</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H14" s="16" t="s">
         <v>55</v>
@@ -3636,13 +3644,13 @@
         <v>119</v>
       </c>
       <c r="N14" s="16" t="s">
+        <v>364</v>
+      </c>
+      <c r="P14" s="19" t="s">
         <v>365</v>
       </c>
-      <c r="P14" s="19" t="s">
+      <c r="Q14" s="5" t="s">
         <v>366</v>
-      </c>
-      <c r="Q14" s="5" t="s">
-        <v>367</v>
       </c>
       <c r="X14" s="16" t="s">
         <v>301</v>
@@ -3651,7 +3659,7 @@
         <v>317</v>
       </c>
       <c r="AI14" s="16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AJ14" s="16" t="s">
         <v>326</v>
@@ -3687,7 +3695,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="15" spans="1:93" ht="154">
+    <row r="15" spans="1:93" ht="154" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>58</v>
       </c>
@@ -3704,7 +3712,7 @@
         <v>91</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H15" s="16" t="s">
         <v>55</v>
@@ -3716,7 +3724,7 @@
         <v>43801</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="L15" s="16" t="s">
         <v>334</v>
@@ -3725,13 +3733,13 @@
         <v>92</v>
       </c>
       <c r="N15" s="16" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="P15" s="21" t="s">
         <v>339</v>
       </c>
       <c r="Q15" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="R15" s="16" t="s">
         <v>307</v>
@@ -3755,7 +3763,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="16" spans="1:93" ht="70">
+    <row r="16" spans="1:93" ht="70" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>55</v>
       </c>
@@ -3781,7 +3789,7 @@
         <v>43801</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L16" s="16" t="s">
         <v>149</v>
@@ -3795,7 +3803,7 @@
       <c r="P16" s="19"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:93" ht="112">
+    <row r="17" spans="1:93" ht="112" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>55</v>
       </c>
@@ -3822,7 +3830,7 @@
         <v>43801</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L17" s="16" t="s">
         <v>122</v>
@@ -3836,7 +3844,7 @@
       <c r="P17" s="19"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="1:93" ht="56">
+    <row r="18" spans="1:93" ht="56" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>55</v>
       </c>
@@ -3862,7 +3870,7 @@
         <v>43802</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="L18" s="16" t="s">
         <v>137</v>
@@ -3876,7 +3884,7 @@
       <c r="P18" s="19"/>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="1:93" ht="266">
+    <row r="19" spans="1:93" ht="266" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
         <v>58</v>
       </c>
@@ -3890,7 +3898,7 @@
         <v>58</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F19" s="16" t="s">
         <v>125</v>
@@ -3914,13 +3922,13 @@
         <v>127</v>
       </c>
       <c r="N19" s="16" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="P19" s="21" t="s">
         <v>339</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="X19" s="16" t="s">
         <v>301</v>
@@ -3941,7 +3949,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="20" spans="1:93" ht="196">
+    <row r="20" spans="1:93" ht="196" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
         <v>58</v>
       </c>
@@ -3976,17 +3984,17 @@
         <v>248</v>
       </c>
       <c r="M20" s="16" t="s">
+        <v>349</v>
+      </c>
+      <c r="N20" s="16" t="s">
         <v>350</v>
-      </c>
-      <c r="N20" s="16" t="s">
-        <v>351</v>
       </c>
       <c r="O20" s="20"/>
       <c r="P20" s="21" t="s">
         <v>339</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="X20" s="16" t="s">
         <v>301</v>
@@ -4004,7 +4012,7 @@
         <v>61</v>
       </c>
       <c r="BD20" s="16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BE20" s="16" t="s">
         <v>63</v>
@@ -4019,7 +4027,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="21" spans="1:93" ht="112">
+    <row r="21" spans="1:93" ht="112" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
         <v>58</v>
       </c>
@@ -4036,10 +4044,10 @@
         <v>327</v>
       </c>
       <c r="F21" s="16" t="s">
+        <v>426</v>
+      </c>
+      <c r="G21" s="16" t="s">
         <v>427</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>428</v>
       </c>
       <c r="H21" s="16" t="s">
         <v>55</v>
@@ -4117,7 +4125,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="22" spans="1:93" ht="238">
+    <row r="22" spans="1:93" ht="238" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>58</v>
       </c>
@@ -4125,7 +4133,7 @@
         <v>98</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>58</v>
@@ -4134,7 +4142,7 @@
         <v>243</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H22" s="16" t="s">
         <v>55</v>
@@ -4152,16 +4160,16 @@
         <v>115</v>
       </c>
       <c r="M22" s="16" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="N22" s="16" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="P22" s="19" t="s">
+        <v>376</v>
+      </c>
+      <c r="Q22" s="5" t="s">
         <v>377</v>
-      </c>
-      <c r="Q22" s="5" t="s">
-        <v>378</v>
       </c>
       <c r="X22" s="16" t="s">
         <v>301</v>
@@ -4188,7 +4196,7 @@
         <v>308</v>
       </c>
       <c r="BQ22" s="16" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="BT22" s="16" t="s">
         <v>301</v>
@@ -4197,7 +4205,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="23" spans="1:93" ht="252">
+    <row r="23" spans="1:93" ht="252" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>58</v>
       </c>
@@ -4205,7 +4213,7 @@
         <v>89</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D23" s="23" t="s">
         <v>58</v>
@@ -4233,19 +4241,19 @@
         <v>252</v>
       </c>
       <c r="M23" s="9" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="N23" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O23" s="6" t="s">
         <v>325</v>
       </c>
       <c r="P23" s="25" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="Q23" s="26" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="R23" s="16" t="s">
         <v>307</v>
@@ -4275,7 +4283,7 @@
         <v>317</v>
       </c>
       <c r="AI23" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AJ23" s="9" t="s">
         <v>326</v>
@@ -4318,10 +4326,10 @@
         <v>61</v>
       </c>
       <c r="BD23" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BE23" s="9" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="BF23" s="9"/>
       <c r="BG23" s="9"/>
@@ -4378,7 +4386,7 @@
       <c r="CN23" s="9"/>
       <c r="CO23" s="9"/>
     </row>
-    <row r="24" spans="1:93" ht="318" customHeight="1">
+    <row r="24" spans="1:93" ht="318" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="13" t="s">
         <v>58</v>
       </c>
@@ -4386,7 +4394,7 @@
         <v>89</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>58</v>
@@ -4411,17 +4419,17 @@
         <v>140</v>
       </c>
       <c r="M24" s="16" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="N24" s="16" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="O24" s="3"/>
       <c r="P24" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R24" s="16" t="s">
         <v>307</v>
@@ -4442,13 +4450,13 @@
         <v>308</v>
       </c>
       <c r="Z24" s="16" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AB24" s="16" t="s">
         <v>308</v>
       </c>
       <c r="AC24" s="16" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AE24" s="16" t="s">
         <v>301</v>
@@ -4466,7 +4474,7 @@
         <v>308</v>
       </c>
       <c r="AR24" s="16" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="AT24" s="16">
         <v>2</v>
@@ -4475,7 +4483,7 @@
         <v>308</v>
       </c>
       <c r="AV24" s="16" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="AX24" s="16">
         <v>2</v>
@@ -4487,10 +4495,10 @@
         <v>61</v>
       </c>
       <c r="BD24" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BE24" s="9" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="BH24" s="9">
         <v>24</v>
@@ -4508,13 +4516,13 @@
         <v>308</v>
       </c>
       <c r="BQ24" s="16" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="BT24" s="16" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="25" spans="1:93" ht="407" customHeight="1">
+    <row r="25" spans="1:93" ht="407" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
         <v>58</v>
       </c>
@@ -4522,47 +4530,47 @@
         <v>89</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>58</v>
       </c>
       <c r="E25" s="20"/>
       <c r="F25" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>414</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I25" s="16" t="s">
         <v>404</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>415</v>
-      </c>
-      <c r="H25" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="I25" s="16" t="s">
-        <v>405</v>
       </c>
       <c r="J25" s="17">
         <v>44007</v>
       </c>
       <c r="K25" s="18" t="s">
+        <v>405</v>
+      </c>
+      <c r="L25" s="16" t="s">
         <v>406</v>
       </c>
-      <c r="L25" s="16" t="s">
+      <c r="M25" s="16" t="s">
         <v>407</v>
       </c>
-      <c r="M25" s="16" t="s">
+      <c r="N25" s="16" t="s">
         <v>408</v>
       </c>
-      <c r="N25" s="16" t="s">
+      <c r="P25" s="19" t="s">
+        <v>412</v>
+      </c>
+      <c r="Q25" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="R25" s="16" t="s">
         <v>409</v>
-      </c>
-      <c r="P25" s="19" t="s">
-        <v>413</v>
-      </c>
-      <c r="Q25" s="5" t="s">
-        <v>429</v>
-      </c>
-      <c r="R25" s="16" t="s">
-        <v>410</v>
       </c>
       <c r="S25" s="16" t="s">
         <v>301</v>
@@ -4586,13 +4594,13 @@
         <v>308</v>
       </c>
       <c r="AR25" s="16" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AU25" s="16" t="s">
         <v>308</v>
       </c>
       <c r="AV25" s="16" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AY25" s="16" t="s">
         <v>301</v>
@@ -4601,7 +4609,7 @@
         <v>61</v>
       </c>
       <c r="BD25" s="16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BE25" s="16" t="s">
         <v>62</v>
@@ -4616,7 +4624,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="26" spans="1:93" ht="42">
+    <row r="26" spans="1:93" ht="42" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
         <v>58</v>
       </c>
@@ -4779,7 +4787,7 @@
       <c r="CF26" s="16">
         <v>800</v>
       </c>
-      <c r="CG26" s="16">
+      <c r="CG26" s="28">
         <v>5</v>
       </c>
       <c r="CH26" s="16" t="s">
@@ -4825,7 +4833,7 @@
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="13.1640625" style="1" customWidth="1"/>
@@ -4841,7 +4849,7 @@
     <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="51">
+    <row r="1" spans="1:58" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>141</v>
       </c>
@@ -5017,7 +5025,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:58" ht="308" customHeight="1">
+    <row r="2" spans="1:58" ht="308" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>55</v>
       </c>
@@ -5091,7 +5099,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:58" ht="153">
+    <row r="3" spans="1:58" ht="153" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
@@ -5153,7 +5161,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:58" ht="272">
+    <row r="4" spans="1:58" ht="272" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>55</v>
       </c>
@@ -5218,7 +5226,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:58" ht="221">
+    <row r="5" spans="1:58" ht="221" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>55</v>
       </c>
@@ -5277,7 +5285,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:58" ht="136">
+    <row r="6" spans="1:58" ht="136" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>55</v>
       </c>
@@ -5318,7 +5326,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:58" ht="187">
+    <row r="7" spans="1:58" ht="187" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>55</v>
       </c>
@@ -5389,7 +5397,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:58" ht="187">
+    <row r="8" spans="1:58" ht="187" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>55</v>
       </c>
@@ -5460,7 +5468,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:58" ht="102">
+    <row r="9" spans="1:58" ht="102" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
@@ -5504,7 +5512,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:58" ht="102">
+    <row r="10" spans="1:58" ht="102" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
@@ -5548,7 +5556,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:58" ht="238">
+    <row r="11" spans="1:58" ht="238" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>55</v>
       </c>
@@ -5610,7 +5618,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:58" ht="306">
+    <row r="12" spans="1:58" ht="306" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
@@ -5663,7 +5671,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:58" ht="51">
+    <row r="13" spans="1:58" ht="51" x14ac:dyDescent="0.2">
       <c r="D13" s="1" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
last tweaking of the proposals
</commit_message>
<xml_diff>
--- a/app/data/wto_proposal_settings_master.xlsx
+++ b/app/data/wto_proposal_settings_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kat/GitHub/SubsidyExplorer/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8F0ED8-679D-4142-B69B-3B89AE032A0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6ED5F85-361C-7A43-9812-5878ED18E801}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="460" windowWidth="35700" windowHeight="19140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14200" yWindow="7000" windowWidth="35700" windowHeight="19140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="452">
   <si>
     <t>proposal</t>
   </si>
@@ -1028,12 +1028,6 @@
     <t>Elimination of subsidies that contribute to illegal, unreported and unregulated (IUU) fishing - Facilitator's working paper</t>
   </si>
   <si>
-    <t xml:space="preserve">Developing countries not engaged in large-scale industrial distant water fishing are entitled to an additional transition period. LDCs and SVEs are entitled to a different transition period.  </t>
-  </si>
-  <si>
-    <t>Just missing time delay (two different time delays: 1) developing countries not engaged in large scale industrial fishing; 2) LDCs and SVEs)</t>
-  </si>
-  <si>
     <t>This document builds on ACP text proposal TN/RL/GEN/192, as reflected in TN/RL/W/274/Rev.6. It specifies that IUU determinations could be made by coastal Member states for activities in waters under their jurisdictions with respect to a foreign vessel or operator, or by RFMO/As in areas (and for species) under their juridscitions. Members are encouraged to refrain from invoking the discipline based on minor infringements.</t>
   </si>
   <si>
@@ -1058,12 +1052,6 @@
     <t xml:space="preserve">This communication advocates for Member-specific de minimis limits, below which Members may maintain, grant, or provide subsidies. Four criteria are provided to determine de minimis limits. 1) The de minimis limit for developed country Members and developing country Members belonging to the top [10] global marine capture fisheries producers shall be [X]% of the average total landed value of the Member's marine capture fisheries in the period [2015-2017]. 2) For developing country Members not included in 1), the de minimis limit shall by [Y]% plus [10/15]% of the average total landed value in the most recent three year period for which data are available. 3) Developing country Members included in 1) whose large-scale commercial fisheries are responsible for less than [5/10]% of the average total landed value may instead take the de minimis limit determined under 2). 4) The de minimis level for LDC Members shall be [Z]% plus [20/30]% of the average total landed value in the most recent three year period for which data are available. </t>
   </si>
   <si>
-    <t xml:space="preserve">Subsidies in excess of a Member's de minimis limit in the first year of the implementation shall be reduced or phased down to the de minimis level in equal annual installments over [X] years for developed country Members, [X+3] years for developing country Members, and [X+5] years for LDC Members. Subsidies to fishing and fishing-related activities solely within the Member's territorial waters shall not be included in the de minimis for developing and LDC Members. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add top 10 global producers option for cap/tier (and related option for other developing members). Also add three year selection for global production data. </t>
-  </si>
-  <si>
     <t>TN/RL/GEN/200/Rev.1</t>
   </si>
   <si>
@@ -1091,16 +1079,6 @@
     <t xml:space="preserve">1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) It is not possible to simulate whether Members could demonstrate that they have policies in place that would negate this prohibition. </t>
   </si>
   <si>
-    <t xml:space="preserve">1) We assume that each Member's base subsidy level is represented by the total amount of capacity-enhancing subsidies estimated for that Member by Sumaila et al. 2019, and we estimate the landed value of marine capture fisheries from the FAO Global Capture Production Database. 2) We assume the de minimis limit for developed and developing country members belonging to the top 10 marine capture fisheries producers to be 50% of the average total landed value of the Member's marine capture fisheries between 2016-2018. For all other developing country Members, we assume the de minimis limit to be 70% of the average total landed value between 2016-2018. For LDC Members, we assume the de minimis limit to be 90% of the average total landed value between 2016-2018. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) We assume that each Member's base for capping is represented by the total amount of capacity-enhancing subsidies estimated by Sumaila et al. 2019. 2) Each Member's cap is equal to whichever of the three proposed approaches for calculating a cap yields the largest amount. By default, caps based on the first approach are calculated as 90% of each Member's base for capping; caps based on the second approach are calculated as 90% of each Member's estimated landed value (calculated from the FAO Global Marine Capture Production Database in 2018); caps based on the third approach are calculated assuming a value of $600 per fisherman, and each Member's most recently reported total number of fishers (from the FAO Yearbook of Fishery and Aquaculture Statistics 2017). 3) Users are free to explore different values by changing the respective sliders on the advanced policy selection tab. 4) We assume that provision of the following types of capacity-enhancing subsidies as defined by Sumaila et al. 2019 are allowed to continue irrespective of a Member's total cap: i) subsidies for fishing access agreements; ii) fisheries development projects. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) We assume that all capacity-enhancing subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 
-2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas to be prohibited. Users can set a different threshold on the advanced policy selection tab if they wish. </t>
-  </si>
-  <si>
     <t>1) We assume that the following types of subsidies as defined by Sumaila et al. 2019 are prohibited: i) boat construction and renovation, ii) fuel. 2) This prohibition is assumed to only apply to developed and developing country Members</t>
   </si>
   <si>
@@ -1110,21 +1088,12 @@
     <t xml:space="preserve">This communication advocates for prohibiting subsidies in disputed waters, unless all parties have jointly notified the WTO of any agreement to subsidize. Members should attempt to reach an agreement through bilateral consultations before going to Dispute Settlement. </t>
   </si>
   <si>
-    <t xml:space="preserve">1) We assume that all capacity-enhancing subsidies as defined by Sumaila et al. 2019 are prohibited to vessels satisfying the three following characteristics: i) total length of more than 24 meters; ii) gross tonnage of more than 100 GT; iii) engine power of more than 130 kW. 2) In general, the tool does not include many vessels with fishing gears that are not hauled by a motor driven equipment, thus this characteristic is assumed to be satisfied. 3) The other 2 conditions are not modeled as it is difficult to determine which vessels have onboard freezing equipment, or the characteristics of a vessel's owning or operating company. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) We assume that each Member's base for capping is represented by the total amount of capacity-enhancing subsidies estimated by Sumaila et al. 2019. Members are sorted into three tiers based on a three-year average of FAO marine capture production (2015-2017). 2) Members accounting for 0.7% or more of global marine capture production are in "Tier 1"; Members accounting for 0.05% or more, but less than 0.7%, of global marine capture production are in "Tier 2"; Members accounting for less than 0.05% of global marine capture production are in "Tier 3". 3) This proposal advocates for allowing both Tier 1 and Tier 2 Members to negotiate their own subsidy caps or to accept a default cap of $50 million annually. For the purposes of modeling, we assume that Tier 1 Members receive a subsidy cap equal to 90% of their base for capping, and Tier 2 Members receive the default cap of $50 million. Tier 3 Members do not receive a cap. </t>
-  </si>
-  <si>
     <t>This communication advocates for a general prohibition of subsidies that contribute to overcapacity and overfishing. However, it allows for subsidies if the subsidising Member can demonstrate that the stock(s) targeted by the subsidy recipient are managed on the based on the best publically available scientific evidence taking into account the following elements: 1) scientific stock assessments; 2) legal institutions for resource management (i.e. vessel registration and fishery permits); 3) specific conservation and management measures for fish stocks (i.e. input, output, and technical controls taking account of fishery status); 4) monitoring, control and surveillance measures. It also provides a list of subsidies that shall be deemed not to be prohibited. Includes a reference to the precautionary principle to be included in a preamble. Prohibition should not apply to subsistence fishing.</t>
   </si>
   <si>
     <t xml:space="preserve">A transition period shall be allowed for developing country Members and LDCs. We assume these transition periods to be 4 and 6 years respectively. </t>
   </si>
   <si>
-    <t xml:space="preserve">1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) It is difficult to identify subsidies for subsistence fishing, so we approximate this condition by assuming that subsidies for fishing within a Member's territorial waters are allowed.       </t>
-  </si>
-  <si>
     <t>Transition period missing.</t>
   </si>
   <si>
@@ -1149,39 +1118,12 @@
     <t>This unofficial room document was circulated at the request of the Delegation of Jamaica on behalf of the African, Caribbean and Pacific Countries (ACP) Group on February 4, 2020.</t>
   </si>
   <si>
-    <t xml:space="preserve">1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) We assume that all capacity-enhancing subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing on the high seas. By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas to be prohibited. Users can set a different threshold on the advanced policy selection tab if they wish. </t>
-  </si>
-  <si>
-    <t>Developing country Members that individually account for less than [2%] of global marine capture production shall be exempt, and this prohibition shall not apply to LDC Members.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) We assume that the following types of subsidies as defined by Sumaila et al. 2019 are prohibited: i) boat construction and renovation, ii) fuel. 2) This prohibition is assumed to only apply to developed and developing country Members. </t>
-  </si>
-  <si>
-    <t>PERCENT_CAPTURE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Need to add new S&amp;DT option for developing and LDC (% capture). Alternatively could do this as a scope option. </t>
-  </si>
-  <si>
     <t xml:space="preserve">This communication builds on TN/RL/GEN/192, as reflected in TN/RL/W/274/Rev.6, and advocates for a prohibition on subsidies for capital and operating costs, provided to large-scale industrial fishing. Capital cost subsidies include those for construction, acquisition, modernization, renovation or upgrading of vessels, direct transfers for vessel construction and modernization, purchase of machines and equipment for fishing vessels. Operating cost subsidies include those for fuel, ice, bait, personnel, income support of vessels or operators or the workers they employ, social chargers, insurance, payments based on the price of fish caught, gear, and at-sea support, or operating losses of such vessels or activities. This text includes a list of subsidies that shall not be prohibited (Green Box): fisheries management, permanent cessation of fishing; implementation of international agreements, disaster relief, health and safety conditions, promotion of human capital. </t>
   </si>
   <si>
     <t>This unofficial room document was circulated at the request of the Delegation of Chad on behalf of the Least Developed Countries (LDC) Group on March 6, 2020.</t>
   </si>
   <si>
-    <t xml:space="preserve">1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, and coastal Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal Member. The possible effects is a conservative interpretation of this text. 3) Users are free to explore a more ambitious interpretation by making their own assumptions about the expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, and coastal Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal Member. The possible effects is a conservative interpretation of this text. 3) Users are free to explore a more ambitious interpretation by making their own assumptions about the expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. For OFOC: 1) We assume that all capacity-enhancing subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing on the high seas, and to vessels greater than 24 m in length or with a tonnage greater than 100 GT. </t>
-  </si>
-  <si>
-    <t>LENGTH</t>
-  </si>
-  <si>
-    <t>Transition period missing; need to add the ability to select multiple scope options - for now this just does length</t>
-  </si>
-  <si>
     <t xml:space="preserve">This communication was circulated at the request of the Delegation of India on March 6, 2020. </t>
   </si>
   <si>
@@ -1215,9 +1157,6 @@
     <t>Facilitator's working text - S&amp;DT</t>
   </si>
   <si>
-    <t>Subsidies for fishing in a Member's territorial waters are excluded. Prohibition of subsidies to OFOC shall not apply to LDCs. A transition period of 5 years shall be allowed for Overfished and OFOC disciplines for developing country and LDC Members.</t>
-  </si>
-  <si>
     <t>oa_scope_select</t>
   </si>
   <si>
@@ -1257,25 +1196,13 @@
     <t>TER</t>
   </si>
   <si>
-    <t xml:space="preserve">DONE. Data does not exist to model the prohibition on subsidies being provided to vessels flagged to another state. </t>
-  </si>
-  <si>
     <t>For IUU: No S&amp;DT is considered. For Overfished: Subsidies granted by developing and LDC Members for fishing within their own territorial sea shall be allowed. For OCOF: No S&amp;DT is considered.</t>
   </si>
   <si>
-    <t>Add two options for OCOF? (complete prohibition on boat building/fuel + HS only prohibition on all bad subs)</t>
-  </si>
-  <si>
     <t>RD/TN/RL/126/A1</t>
   </si>
   <si>
-    <t xml:space="preserve">1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - we have chosen to model the more ambitious of the two. </t>
-  </si>
-  <si>
     <t>1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 0.8) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text requires that there be a causal negative effect to the stock as a result of the subsidy. This is difficult to establish given existing data on subsidy provisioning and stock status, and is not possible to model, but we have chosen a more conservative reference point in regards to this condition.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) As written, this proposal does specify potential disciplines within each of the three categories, but rather the S&amp;DT that should be allowed for them. 2) To model the possible effects of such a proposal, we therefore use the disciplines proposed in LDC - Full text (excluding any S&amp;DT). Those are as follows: For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, and coastal Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal Member. The possible effects is a conservative interpretation of this text. 3) Users are free to explore a more ambitious interpretation by making their own assumptions about the expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. For OFOC: 1) We assume that all capacity-enhancing subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing on the high seas, and to vessels greater than 24 m in length or with a tonnage greater than 100 GT. </t>
   </si>
   <si>
     <t>Is basically the same as the cap. Different structure, tiers and flexibilities. It loks like is all based on global marine capture. There are no values as the de minimis will be the (x) of the average of landed value for 3 years. What should we use for the (x) value? a scale bar as we use in other cases?) Also there is an exception for 12 miles for all developing countries</t>
@@ -1342,20 +1269,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">1) We assume that all capacity-enhancing subsidies as defined by Sumaila et al. 2019 are prohibited in areas classified as "disputed" in the Marine Regions' Maritime Boundaries World EEZ dataset (v10). 2) We note that this is a very ambitious interpretation of the possible effects of this proposal. 3) It is materially impossible to model non-existing agreements to subsidize in disputed areas.                                                                                                         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="3"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Disclaimer: We recognize that disputed areas are a political matter and our interpretation of this text is not meant to imply the expression of any opinion whatsoever concerning the status of any country, territory, city or area or of its authorities, or concerning the delimitation of its frontier or boundaries. </t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">RD/TN/RL/97/Rev.3, TN/RL/W/274/Rev.6, RD/TN/RL/104, </t>
     </r>
     <r>
@@ -1375,30 +1288,15 @@
     <t>RD/TN/RL/89/Rev.1, TN/RL/GEN/192, TN/RL/W/274/Rev.6</t>
   </si>
   <si>
-    <t xml:space="preserve">For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. The possible effects is a conservative interpretation of this text. 3) Users are free to explore a more ambitious interpretation by making their own assumptions about the expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternate definitions for an overfished stock subsidy prohibition - we have chosen to model the more ambitious interpretation of the two. For OFOC: 1) We assume that all capacity-enhancing subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. Users can set a different threshold on the advanced policy selection tab if they wish. </t>
-  </si>
-  <si>
     <t>For IUU: Subsidies granted by developing and LDC Members shall be allowed for small scale fishing: a) within their own territorial waters and b) within their own EEZs and high seas for 7 years. For Overfished: Subsidies granted by developing and LDC Members shall be allowed for fishing a) within their own territorial waters and b) within their own EEZs for 2 years. For OCOF: Subsidies granted by LDCs shall be allowed, and subsidies granted by developing countries shall be allowed for fishing in their territorial seas, or for fishing in their EEZs and high seas unless any of the following conditions are met for three consecutive years: a) GNI per capita is greater than US $5000 (constant 2010 US$), b) they engage in distant water fishing, or c) the contribution from Agriculture, Forestry and Fishing to their national GDP (World Bank) is greater than 10%.</t>
   </si>
   <si>
-    <t>TER, TIME</t>
-  </si>
-  <si>
-    <t>Need to add new S&amp;DT option for developing and LDC (non-industrial). The three options associated with defining it could be calculated on the back-end. Also need to build in time delays somehow</t>
-  </si>
-  <si>
     <t>This communication advocates for special and differential treatment for all three classes of proposed disciplines. As written, this proposal does specify potential disciplines within each of the three categories, but rather the S&amp;DT that should be allowed for them. To model the possible effects of such a proposal, we therefore use the disciplines proposed in LDC - Full text (excluding any S&amp;DT).</t>
   </si>
   <si>
-    <t>B1, B3, B4, B5, B6, B7, C1, C2, C3</t>
-  </si>
-  <si>
     <t>B1, B2, B3, B4, B5, B6, B7, C1, C2, C3</t>
   </si>
   <si>
-    <t xml:space="preserve">Missing "best of" option; also fix "per fisher" calculation. </t>
-  </si>
-  <si>
     <t>BEST</t>
   </si>
   <si>
@@ -1427,6 +1325,125 @@
   </si>
   <si>
     <t>tier3_cap_best_percent_fishers</t>
+  </si>
+  <si>
+    <t>B1, B2, B3, B4, B5, B7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DONE. Note: data does not exist to model the prohibition on subsidies being provided to vessels flagged to another state. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas to be prohibited. Users can set a different threshold on the advanced policy selection tab if they wish. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) We assume each Member's cap is equal to whichever of the three proposed approaches for calculating a cap yields the largest amount. By default, caps based on the first approach are calculated as 55% of each Member's base for capping; caps based on the second approach are calculated as 2% of each Member's estimated landed value (calculated from the FAO Global Marine Capture Production Database, average between 2016-2018); caps based on the third approach are calculated as 55% of the global average subsidies per fisher (capacity-enhancing and ambiguous) multiplied by each Member's most recently reported total number of fishers (from the FAO Yearbook of Fishery and Aquaculture Statistics 2017). 2) We assume that provision of the following types of subsidies as defined by Sumaila et al. 2019 are allowed to continue irrespective of a Member's total cap: i) subsidies for fishing access agreements; ii) fisher assistance programs; iii) vessel buyback programs; iv) rural fishers' community development programs. Therefore each Member's base for capping is represented by the total amount of all other capacity-enhancing and ambiguous subsidies estimated by Sumaila et al. 2019. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) We assume that each Member's base for capping is represented by the total amount of capacity-enhancing and ambiguos subsidies estimated by Sumaila et al. 2019. 2) Members are sorted into three tiers based on a three-year average of FAO marine capture production (2016-2018). Members accounting for 0.7% or more of global marine capture production are in "Tier 1"; Members accounting for 0.05% or more, but less than 0.7%, of global marine capture production are in "Tier 2"; Members accounting for less than 0.05% of global marine capture production are in "Tier 3". 3) This proposal advocates for allowing both Tier 1 and Tier 2 Members to negotiate their own subsidy caps or to accept a default cap of $50 million annually. For the purposes of modeling, we assume that Tier 1 Members receive a subsidy cap equal to 50% of their base for capping; Tier 2 Members receive the default cap of $50 million; Tier 3 Members do not receive a cap. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels satisfying the three following characteristics: i) total length of more than 24 meters; ii) gross tonnage of more than 100 GT; iii) engine power of more than 130 kW. 2) In general, the tool does not include many vessels with fishing gears that are not hauled by a motor driven equipment, thus this characteristic is assumed to be satisfied. 3) The other 2 conditions are not considered as it is difficult to determine which vessels have onboard freezing equipment, or the characteristics of a vessel's owning or operating company. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited in areas classified as "disputed" in the Marine Regions' Maritime Boundaries World EEZ dataset (v10). 2) We note that this is a very ambitious interpretation of the possible effects of this proposal. 3) It is materially impossible to model non-existing agreements to subsidize in disputed areas.                                                                                                         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Disclaimer: We recognize that disputed areas are a political matter and our interpretation of this text is not meant to imply the expression of any opinion whatsoever concerning the status of any country, territory, city or area or of its authorities, or concerning the delimitation of its frontier or boundaries. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) It is difficult to identify subsidies for subsistence fishing, so we approximate this condition by assuming that subsidies for fishing within a Member's territorial waters are allowed.       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, and coastal Member states. 2) No publically available data exist for most flag and subsidizing Member states, nor for coastal Member states. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about the expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. </t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - we have chosen to model our interpretation of the more ambitious of the two (see New Zealand/Iceland - Overfishing and overcapacity). </t>
+  </si>
+  <si>
+    <t>1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) We assume that all capacity-enhancing subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing on the high seas. By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas to be prohibited.</t>
+  </si>
+  <si>
+    <t>Developing countries not engaged in large-scale industrial distant water fishing are entitled to a transition period of 3 years. LDCs and SVEs are entitled to a transition period of 6 years.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, and coastal Member states. 2) No publically available data exist for most flag and subsidizing Members, nor for coastal Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) We assume that the following types of subsidies as defined by Sumaila et al. 2019 are prohibited: i) boat construction and renovation, ii) fuel. 2) This prohibition is assumed to only apply to Members responsible for more than 1% of global marine capture production (calculcated as the annual average between 2016-2018). </t>
+  </si>
+  <si>
+    <t>This prohibition shall not apply to LDC Members.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, and coastal Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal Member. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing on the high seas, and to vessels greater than 24 m in length or with a tonnage greater than 100 GT. </t>
+  </si>
+  <si>
+    <t>LENGTH, TONNAGE</t>
+  </si>
+  <si>
+    <t>For Overfished: Subsidies for fishing in a Member's territorial waters are excluded. For OFOC: This prohibition shall not apply to LDCs. Additionally, a transition period of 5 years shall be allowed for Overfished and OFOC disciplines for both developing country and LDC Members.</t>
+  </si>
+  <si>
+    <t>Transition period missing. Two separate delays: 1) developing countries not engaged in large scale industrial fishing; 2) LDCs and SVEs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) As written, this proposal does specify potential disciplines within each of the three categories, but rather the S&amp;DT that should be allowed for them. 2) To model the possible effects of such a proposal, we therefore use the disciplines proposed in LDC - Full text (excluding any S&amp;DT). Those are as follows: For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, and coastal Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal Member. The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about the expected IUU-findings. 3) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing on the high seas, and to vessels greater than 24 m in length or with a tonnage greater than 100 GT. </t>
+  </si>
+  <si>
+    <t>Transition periods missing. Also need to identify developing countries meeting non-industrial criteria. The three options associated with defining it could be calculated on the back-end.</t>
+  </si>
+  <si>
+    <t>As witten, this proposal places different prohibtions on boat building/fuel subsidies and all other subsidies. This is not accounted for (HS only vs. all)</t>
+  </si>
+  <si>
+    <t>These are the values for the Chair's text + China cap proposal</t>
+  </si>
+  <si>
+    <t>For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternate definitions for an overfished stock subsidy prohibition - we have chosen to model the more ambitious interpretation of the two. For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. No cap-based approach is included.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternate definitions for an overfished stock subsidy prohibition - we have chosen to model the more ambitious interpretation of the two. For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: 1) We assume each Member's cap is equal to whichever of the three proposed approaches for calculating a cap yields the largest amount. By default, caps based on the first approach are calculated as 55% of each Member's base for capping; caps based on the second approach are calculated as 2% of each Member's estimated landed value (calculated from the FAO Global Marine Capture Production Database, average between 2016-2018); caps based on the third approach are calculated as 55% of the global average subsidies per fisher (capacity-enhancing and ambiguous) multiplied by each Member's most recently reported total number of fishers (from the FAO Yearbook of Fishery and Aquaculture Statistics 2017). 2) We assume that provision of the following types of subsidies as defined by Sumaila et al. 2019 are allowed to continue irrespective of a Member's total cap: i) subsidies for fishing access agreements; ii) fisher assistance programs; iii) vessel buyback programs; iv) rural fishers' community development programs. Therefore each Member's base for capping is represented by the total amount of all other capacity-enhancing and ambiguous subsidies estimated by Sumaila et al. 2019. </t>
+  </si>
+  <si>
+    <t>Chair's text - Consolidated text (w/ China - Cap)</t>
+  </si>
+  <si>
+    <t>These are the values for the Chair's text + USA cap proposal</t>
+  </si>
+  <si>
+    <t>Chair's text - Consolidated text (w/ US and others -  Cap/Tier)</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126 (TN/RL/GEN/197/Rev.2)</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126 (TN/RL/GEN/199)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternate definitions for an overfished stock subsidy prohibition - we have chosen to model the more ambitious interpretation of the two. For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: 1) 1) We assume that each Member's base for capping is represented by the total amount of capacity-enhancing and ambiguos subsidies estimated by Sumaila et al. 2019. 2) Members are sorted into three tiers based on a three-year average of FAO marine capture production (2016-2018). Members accounting for 0.7% or more of global marine capture production are in "Tier 1"; Members accounting for 0.05% or more, but less than 0.7%, of global marine capture production are in "Tier 2"; Members accounting for less than 0.05% of global marine capture production are in "Tier 3". 3) This proposal advocates for allowing both Tier 1 and Tier 2 Members to negotiate their own subsidy caps or to accept a default cap of $50 million annually. For the purposes of modeling, we assume that Tier 1 Members receive a subsidy cap equal to 50% of their base for capping; Tier 2 Members receive the default cap of $50 million; Tier 3 Members do not receive a cap. </t>
+  </si>
+  <si>
+    <t>TOP10</t>
+  </si>
+  <si>
+    <t>PERCENT_REV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) We assume that provision of the following types of subsidies as defined by Sumaila et al. 2019 are allowed to continue irrespective of a Member's total de minimus limit: i) fisher assistance programs; ii) rural fishers' community development programs.subsidies (both programs relevant to fishing in territorial waters). Therefore each Member's base subsidy level is represented by the total amount of all other capacity-enhancing and ambiguous subsidies estimated by Sumaila et al. 2019. 2) we estimate the landed value of marine capture fisheries from the FAO Global Capture Production Database. 3) We assume the de minimis limit for developed and developing country members belonging to the top 10 marine capture fisheries producers to be 50% of the average total landed value of the Member's marine capture fisheries between 2016-2018. For all other developing country Members, we assume the de minimis limit to be 70% of the average total landed value between 2016-2018. For LDC Members, we assume the de minimis limit to be 90% of the average total landed value between 2016-2018. </t>
+  </si>
+  <si>
+    <t>B1, B2, B3, B4, B5, B6, B7, C2</t>
   </si>
 </sst>
 </file>
@@ -1958,7 +1975,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2043,6 +2060,12 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2399,11 +2422,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CU26"/>
+  <dimension ref="A1:CU28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BV1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="CT33" sqref="CT33"/>
+    <sheetView tabSelected="1" topLeftCell="BT1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BX2" sqref="BX2:CR2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2443,7 +2466,7 @@
         <v>333</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>321</v>
@@ -2452,7 +2475,7 @@
         <v>0</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>388</v>
+        <v>369</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>260</v>
@@ -2497,7 +2520,7 @@
         <v>10</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="W1" s="9" t="s">
         <v>11</v>
@@ -2539,7 +2562,7 @@
         <v>17</v>
       </c>
       <c r="AJ1" s="9" t="s">
-        <v>398</v>
+        <v>378</v>
       </c>
       <c r="AK1" s="9" t="s">
         <v>18</v>
@@ -2602,7 +2625,7 @@
         <v>27</v>
       </c>
       <c r="BE1" s="9" t="s">
-        <v>400</v>
+        <v>380</v>
       </c>
       <c r="BF1" s="9" t="s">
         <v>28</v>
@@ -2686,13 +2709,13 @@
         <v>45</v>
       </c>
       <c r="CG1" s="9" t="s">
-        <v>437</v>
+        <v>407</v>
       </c>
       <c r="CH1" s="9" t="s">
-        <v>438</v>
+        <v>408</v>
       </c>
       <c r="CI1" s="9" t="s">
-        <v>439</v>
+        <v>409</v>
       </c>
       <c r="CJ1" s="9" t="s">
         <v>46</v>
@@ -2704,13 +2727,13 @@
         <v>49</v>
       </c>
       <c r="CM1" s="9" t="s">
-        <v>440</v>
+        <v>410</v>
       </c>
       <c r="CN1" s="9" t="s">
-        <v>441</v>
+        <v>411</v>
       </c>
       <c r="CO1" s="9" t="s">
-        <v>442</v>
+        <v>412</v>
       </c>
       <c r="CP1" s="9" t="s">
         <v>50</v>
@@ -2722,36 +2745,36 @@
         <v>53</v>
       </c>
       <c r="CS1" s="9" t="s">
-        <v>443</v>
+        <v>413</v>
       </c>
       <c r="CT1" s="9" t="s">
-        <v>444</v>
+        <v>414</v>
       </c>
       <c r="CU1" s="9" t="s">
-        <v>445</v>
+        <v>415</v>
       </c>
     </row>
     <row r="2" spans="1:99" s="9" customFormat="1" ht="282" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>98</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>346</v>
+        <v>318</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>58</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>418</v>
+        <v>394</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>99</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>390</v>
+        <v>371</v>
       </c>
       <c r="H2" s="16" t="s">
         <v>55</v>
@@ -2763,7 +2786,7 @@
         <v>43545</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="L2" s="16" t="s">
         <v>147</v>
@@ -2772,14 +2795,14 @@
         <v>148</v>
       </c>
       <c r="N2" s="16" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="O2" s="16"/>
-      <c r="P2" s="19" t="s">
-        <v>345</v>
+      <c r="P2" s="21" t="s">
+        <v>337</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>356</v>
+        <v>450</v>
       </c>
       <c r="R2" s="16"/>
       <c r="S2" s="16"/>
@@ -2787,7 +2810,9 @@
       <c r="U2" s="16"/>
       <c r="V2" s="16"/>
       <c r="W2" s="16"/>
-      <c r="X2" s="16"/>
+      <c r="X2" s="16" t="s">
+        <v>301</v>
+      </c>
       <c r="Y2" s="16"/>
       <c r="Z2" s="16"/>
       <c r="AA2" s="16"/>
@@ -2805,7 +2830,9 @@
       <c r="AM2" s="16"/>
       <c r="AN2" s="16"/>
       <c r="AO2" s="16"/>
-      <c r="AP2" s="16"/>
+      <c r="AP2" s="16" t="s">
+        <v>301</v>
+      </c>
       <c r="AQ2" s="16"/>
       <c r="AR2" s="16"/>
       <c r="AS2" s="16"/>
@@ -2826,7 +2853,9 @@
       <c r="BH2" s="16"/>
       <c r="BI2" s="16"/>
       <c r="BJ2" s="16"/>
-      <c r="BK2" s="16"/>
+      <c r="BK2" s="16" t="s">
+        <v>301</v>
+      </c>
       <c r="BL2" s="16"/>
       <c r="BM2" s="16"/>
       <c r="BN2" s="16"/>
@@ -2839,27 +2868,46 @@
       <c r="BU2" s="16"/>
       <c r="BV2" s="16"/>
       <c r="BW2" s="16"/>
-      <c r="BX2" s="16"/>
-      <c r="BY2" s="16"/>
-      <c r="BZ2" s="16"/>
-      <c r="CA2" s="16"/>
+      <c r="BX2" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="BY2" s="16" t="s">
+        <v>451</v>
+      </c>
+      <c r="BZ2" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="CA2" s="16" t="s">
+        <v>448</v>
+      </c>
       <c r="CB2" s="16"/>
       <c r="CC2" s="16"/>
-      <c r="CD2" s="16"/>
+      <c r="CD2" s="30" t="s">
+        <v>449</v>
+      </c>
       <c r="CE2" s="16"/>
-      <c r="CF2" s="28"/>
+      <c r="CF2" s="28">
+        <v>50</v>
+      </c>
       <c r="CG2" s="28"/>
       <c r="CH2" s="28"/>
       <c r="CI2" s="28"/>
-      <c r="CJ2" s="16"/>
-      <c r="CK2" s="16"/>
-      <c r="CL2" s="16"/>
+      <c r="CJ2" s="16" t="s">
+        <v>449</v>
+      </c>
+      <c r="CL2" s="16">
+        <v>70</v>
+      </c>
       <c r="CM2" s="28"/>
       <c r="CN2" s="28"/>
       <c r="CO2" s="28"/>
-      <c r="CP2" s="16"/>
+      <c r="CP2" s="16" t="s">
+        <v>449</v>
+      </c>
       <c r="CQ2" s="16"/>
-      <c r="CR2" s="16"/>
+      <c r="CR2" s="16">
+        <v>90</v>
+      </c>
       <c r="CS2" s="28"/>
       <c r="CT2" s="28"/>
       <c r="CU2" s="28"/>
@@ -2878,13 +2926,13 @@
         <v>58</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>108</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>391</v>
+        <v>372</v>
       </c>
       <c r="H3" s="16" t="s">
         <v>55</v>
@@ -2908,10 +2956,10 @@
         <v>154</v>
       </c>
       <c r="P3" s="21" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="X3" s="16" t="s">
         <v>301</v>
@@ -2940,7 +2988,7 @@
         <v>98</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>435</v>
+        <v>318</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>58</v>
@@ -2968,13 +3016,13 @@
         <v>79</v>
       </c>
       <c r="N4" s="16" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="P4" s="21" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>357</v>
+        <v>419</v>
       </c>
       <c r="X4" s="16" t="s">
         <v>301</v>
@@ -2989,13 +3037,13 @@
         <v>308</v>
       </c>
       <c r="BY4" s="16" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="BZ4" s="16" t="s">
         <v>320</v>
       </c>
       <c r="CD4" s="16" t="s">
-        <v>436</v>
+        <v>406</v>
       </c>
       <c r="CG4" s="28">
         <v>55</v>
@@ -3024,7 +3072,7 @@
         <v>132</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>419</v>
+        <v>395</v>
       </c>
       <c r="H5" s="16" t="s">
         <v>55</v>
@@ -3048,16 +3096,16 @@
         <v>157</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>416</v>
+        <v>393</v>
       </c>
       <c r="X5" s="16" t="s">
         <v>301</v>
       </c>
       <c r="AH5" s="16" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="AI5" s="16" t="s">
         <v>300</v>
@@ -3107,10 +3155,10 @@
         <v>146</v>
       </c>
       <c r="N6" s="16" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="Q6" s="5" t="s">
         <v>239</v>
@@ -3145,13 +3193,13 @@
         <v>98</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>58</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>420</v>
+        <v>396</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>102</v>
@@ -3178,10 +3226,10 @@
         <v>153</v>
       </c>
       <c r="P7" s="21" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>358</v>
+        <v>418</v>
       </c>
       <c r="X7" s="16" t="s">
         <v>301</v>
@@ -3190,10 +3238,10 @@
         <v>301</v>
       </c>
       <c r="BC7" s="16" t="s">
-        <v>61</v>
+        <v>405</v>
       </c>
       <c r="BD7" s="16" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="BE7" s="16" t="s">
         <v>62</v>
@@ -3228,7 +3276,7 @@
         <v>114</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>392</v>
+        <v>373</v>
       </c>
       <c r="H8" s="16" t="s">
         <v>55</v>
@@ -3249,13 +3297,13 @@
         <v>116</v>
       </c>
       <c r="N8" s="16" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="P8" s="19" t="s">
         <v>155</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="X8" s="16" t="s">
         <v>301</v>
@@ -3308,7 +3356,7 @@
         <v>130</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>392</v>
+        <v>373</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>55</v>
@@ -3329,22 +3377,22 @@
         <v>116</v>
       </c>
       <c r="N9" s="16" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="P9" s="21" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="X9" s="16" t="s">
         <v>301</v>
       </c>
       <c r="AH9" s="16" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="AI9" s="16" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="AJ9" s="16" t="s">
         <v>326</v>
@@ -3359,7 +3407,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="10" spans="1:99" ht="154" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:99" ht="168" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>55</v>
       </c>
@@ -3376,7 +3424,7 @@
         <v>68</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>421</v>
+        <v>397</v>
       </c>
       <c r="H10" s="15" t="s">
         <v>58</v>
@@ -3388,7 +3436,7 @@
         <v>43657</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="L10" s="16" t="s">
         <v>70</v>
@@ -3397,13 +3445,13 @@
         <v>128</v>
       </c>
       <c r="N10" s="16" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>363</v>
+        <v>420</v>
       </c>
       <c r="X10" s="16" t="s">
         <v>301</v>
@@ -3418,7 +3466,7 @@
         <v>308</v>
       </c>
       <c r="BY10" s="16" t="s">
-        <v>434</v>
+        <v>405</v>
       </c>
       <c r="BZ10" s="16" t="s">
         <v>302</v>
@@ -3433,7 +3481,7 @@
         <v>304</v>
       </c>
       <c r="CF10" s="28">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="CJ10" s="16" t="s">
         <v>305</v>
@@ -3483,13 +3531,13 @@
         <v>113</v>
       </c>
       <c r="N11" s="16" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="P11" s="21" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>362</v>
+        <v>421</v>
       </c>
       <c r="X11" s="16" t="s">
         <v>301</v>
@@ -3498,13 +3546,13 @@
         <v>301</v>
       </c>
       <c r="BC11" s="16" t="s">
-        <v>61</v>
+        <v>405</v>
       </c>
       <c r="BD11" s="16" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="BE11" s="16" t="s">
-        <v>401</v>
+        <v>381</v>
       </c>
       <c r="BH11" s="16">
         <v>24</v>
@@ -3560,10 +3608,10 @@
         <v>151</v>
       </c>
       <c r="P12" s="21" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>422</v>
+        <v>398</v>
       </c>
       <c r="R12" s="16" t="s">
         <v>261</v>
@@ -3604,7 +3652,7 @@
         <v>85</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>423</v>
+        <v>399</v>
       </c>
       <c r="H13" s="15" t="s">
         <v>58</v>
@@ -3616,7 +3664,7 @@
         <v>43759</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>389</v>
+        <v>370</v>
       </c>
       <c r="L13" s="16" t="s">
         <v>86</v>
@@ -3625,16 +3673,16 @@
         <v>87</v>
       </c>
       <c r="N13" s="16" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="O13" s="6" t="s">
         <v>324</v>
       </c>
       <c r="P13" s="21" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="Q13" s="5" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="X13" s="16" t="s">
         <v>301</v>
@@ -3643,10 +3691,10 @@
         <v>301</v>
       </c>
       <c r="BC13" s="16" t="s">
-        <v>61</v>
+        <v>405</v>
       </c>
       <c r="BD13" s="16" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="BE13" s="16" t="s">
         <v>262</v>
@@ -3666,7 +3714,7 @@
         <v>98</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>58</v>
@@ -3678,7 +3726,7 @@
         <v>253</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>393</v>
+        <v>374</v>
       </c>
       <c r="H14" s="16" t="s">
         <v>55</v>
@@ -3699,13 +3747,13 @@
         <v>119</v>
       </c>
       <c r="N14" s="16" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="P14" s="19" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>366</v>
+        <v>423</v>
       </c>
       <c r="X14" s="16" t="s">
         <v>301</v>
@@ -3714,7 +3762,7 @@
         <v>317</v>
       </c>
       <c r="AI14" s="16" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="AJ14" s="16" t="s">
         <v>326</v>
@@ -3767,7 +3815,7 @@
         <v>91</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>425</v>
+        <v>400</v>
       </c>
       <c r="H15" s="16" t="s">
         <v>55</v>
@@ -3779,7 +3827,7 @@
         <v>43801</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="L15" s="16" t="s">
         <v>334</v>
@@ -3788,13 +3836,13 @@
         <v>92</v>
       </c>
       <c r="N15" s="16" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="P15" s="21" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="Q15" s="5" t="s">
-        <v>382</v>
+        <v>424</v>
       </c>
       <c r="R15" s="16" t="s">
         <v>307</v>
@@ -3825,6 +3873,9 @@
       <c r="B16" s="14" t="s">
         <v>98</v>
       </c>
+      <c r="C16" s="29" t="s">
+        <v>425</v>
+      </c>
       <c r="D16" s="15" t="s">
         <v>58</v>
       </c>
@@ -3844,7 +3895,7 @@
         <v>43801</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>394</v>
+        <v>375</v>
       </c>
       <c r="L16" s="16" t="s">
         <v>149</v>
@@ -3865,6 +3916,9 @@
       <c r="B17" s="14" t="s">
         <v>98</v>
       </c>
+      <c r="C17" s="29" t="s">
+        <v>425</v>
+      </c>
       <c r="D17" s="15" t="s">
         <v>58</v>
       </c>
@@ -3885,7 +3939,7 @@
         <v>43801</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>395</v>
+        <v>376</v>
       </c>
       <c r="L17" s="16" t="s">
         <v>122</v>
@@ -3906,6 +3960,9 @@
       <c r="B18" s="14" t="s">
         <v>89</v>
       </c>
+      <c r="C18" s="29" t="s">
+        <v>425</v>
+      </c>
       <c r="D18" s="15" t="s">
         <v>58</v>
       </c>
@@ -3925,7 +3982,7 @@
         <v>43802</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>396</v>
+        <v>377</v>
       </c>
       <c r="L18" s="16" t="s">
         <v>137</v>
@@ -3953,7 +4010,7 @@
         <v>58</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="F19" s="16" t="s">
         <v>125</v>
@@ -3977,13 +4034,13 @@
         <v>127</v>
       </c>
       <c r="N19" s="16" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="P19" s="21" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>415</v>
+        <v>426</v>
       </c>
       <c r="X19" s="16" t="s">
         <v>301</v>
@@ -4004,7 +4061,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="20" spans="1:99" ht="196" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:99" ht="182" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
         <v>58</v>
       </c>
@@ -4039,17 +4096,17 @@
         <v>248</v>
       </c>
       <c r="M20" s="16" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="N20" s="16" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="O20" s="20"/>
       <c r="P20" s="21" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>375</v>
+        <v>427</v>
       </c>
       <c r="X20" s="16" t="s">
         <v>301</v>
@@ -4067,7 +4124,7 @@
         <v>61</v>
       </c>
       <c r="BD20" s="16" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="BE20" s="16" t="s">
         <v>63</v>
@@ -4090,7 +4147,7 @@
         <v>90</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>336</v>
+        <v>435</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>58</v>
@@ -4099,10 +4156,10 @@
         <v>327</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>426</v>
+        <v>401</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>427</v>
+        <v>402</v>
       </c>
       <c r="H21" s="16" t="s">
         <v>55</v>
@@ -4123,13 +4180,13 @@
         <v>116</v>
       </c>
       <c r="N21" s="16" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P21" s="19" t="s">
-        <v>335</v>
+        <v>428</v>
       </c>
       <c r="Q21" s="5" t="s">
-        <v>239</v>
+        <v>429</v>
       </c>
       <c r="R21" s="16" t="s">
         <v>307</v>
@@ -4150,7 +4207,7 @@
         <v>309</v>
       </c>
       <c r="AA21" s="16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AB21" s="16" t="s">
         <v>308</v>
@@ -4168,7 +4225,7 @@
         <v>309</v>
       </c>
       <c r="AG21" s="16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AP21" s="16" t="s">
         <v>301</v>
@@ -4188,7 +4245,7 @@
         <v>98</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>379</v>
+        <v>318</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>58</v>
@@ -4197,7 +4254,7 @@
         <v>243</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="H22" s="16" t="s">
         <v>55</v>
@@ -4215,16 +4272,16 @@
         <v>115</v>
       </c>
       <c r="M22" s="16" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="N22" s="16" t="s">
-        <v>380</v>
+        <v>365</v>
       </c>
       <c r="P22" s="19" t="s">
-        <v>376</v>
+        <v>431</v>
       </c>
       <c r="Q22" s="5" t="s">
-        <v>377</v>
+        <v>430</v>
       </c>
       <c r="X22" s="16" t="s">
         <v>301</v>
@@ -4236,7 +4293,7 @@
         <v>64</v>
       </c>
       <c r="BD22" s="16" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="BK22" s="16" t="s">
         <v>308</v>
@@ -4248,10 +4305,7 @@
         <v>300</v>
       </c>
       <c r="BP22" s="16" t="s">
-        <v>308</v>
-      </c>
-      <c r="BQ22" s="16" t="s">
-        <v>378</v>
+        <v>301</v>
       </c>
       <c r="BT22" s="16" t="s">
         <v>301</v>
@@ -4268,7 +4322,7 @@
         <v>89</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>385</v>
+        <v>357</v>
       </c>
       <c r="D23" s="23" t="s">
         <v>58</v>
@@ -4296,19 +4350,19 @@
         <v>252</v>
       </c>
       <c r="M23" s="9" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="N23" s="6" t="s">
-        <v>387</v>
+        <v>368</v>
       </c>
       <c r="O23" s="6" t="s">
         <v>325</v>
       </c>
       <c r="P23" s="25" t="s">
-        <v>397</v>
+        <v>434</v>
       </c>
       <c r="Q23" s="26" t="s">
-        <v>383</v>
+        <v>432</v>
       </c>
       <c r="R23" s="16" t="s">
         <v>307</v>
@@ -4338,7 +4392,7 @@
         <v>317</v>
       </c>
       <c r="AI23" s="9" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="AJ23" s="9" t="s">
         <v>326</v>
@@ -4378,20 +4432,22 @@
       <c r="BA23" s="9"/>
       <c r="BB23" s="9"/>
       <c r="BC23" s="16" t="s">
-        <v>61</v>
+        <v>405</v>
       </c>
       <c r="BD23" s="9" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="BE23" s="9" t="s">
-        <v>384</v>
+        <v>433</v>
       </c>
       <c r="BF23" s="9"/>
       <c r="BG23" s="9"/>
       <c r="BH23" s="9">
         <v>24</v>
       </c>
-      <c r="BI23" s="9"/>
+      <c r="BI23" s="9">
+        <v>100</v>
+      </c>
       <c r="BJ23" s="9"/>
       <c r="BK23" s="9" t="s">
         <v>308</v>
@@ -4455,13 +4511,13 @@
         <v>89</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>58</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="G24" s="15"/>
       <c r="H24" s="15" t="s">
@@ -4480,17 +4536,17 @@
         <v>140</v>
       </c>
       <c r="M24" s="16" t="s">
-        <v>386</v>
+        <v>367</v>
       </c>
       <c r="N24" s="16" t="s">
-        <v>432</v>
+        <v>404</v>
       </c>
       <c r="O24" s="3"/>
       <c r="P24" s="4" t="s">
-        <v>429</v>
+        <v>403</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>417</v>
+        <v>436</v>
       </c>
       <c r="R24" s="16" t="s">
         <v>307</v>
@@ -4511,13 +4567,13 @@
         <v>308</v>
       </c>
       <c r="Z24" s="16" t="s">
-        <v>410</v>
+        <v>331</v>
       </c>
       <c r="AB24" s="16" t="s">
         <v>308</v>
       </c>
       <c r="AC24" s="16" t="s">
-        <v>410</v>
+        <v>331</v>
       </c>
       <c r="AE24" s="16" t="s">
         <v>301</v>
@@ -4526,6 +4582,9 @@
         <v>317</v>
       </c>
       <c r="AI24" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="AJ24" s="16" t="s">
         <v>300</v>
       </c>
       <c r="AP24" s="16" t="s">
@@ -4535,35 +4594,32 @@
         <v>308</v>
       </c>
       <c r="AR24" s="16" t="s">
-        <v>430</v>
-      </c>
-      <c r="AT24" s="16">
-        <v>2</v>
+        <v>331</v>
       </c>
       <c r="AU24" s="16" t="s">
         <v>308</v>
       </c>
       <c r="AV24" s="16" t="s">
-        <v>430</v>
-      </c>
-      <c r="AX24" s="16">
-        <v>2</v>
+        <v>331</v>
       </c>
       <c r="AY24" s="16" t="s">
         <v>301</v>
       </c>
       <c r="BC24" s="16" t="s">
-        <v>61</v>
+        <v>405</v>
       </c>
       <c r="BD24" s="9" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="BE24" s="9" t="s">
-        <v>384</v>
+        <v>433</v>
       </c>
       <c r="BH24" s="9">
         <v>24</v>
       </c>
+      <c r="BI24" s="16">
+        <v>100</v>
+      </c>
       <c r="BK24" s="16" t="s">
         <v>308</v>
       </c>
@@ -4577,9 +4633,12 @@
         <v>308</v>
       </c>
       <c r="BQ24" s="16" t="s">
-        <v>410</v>
+        <v>390</v>
       </c>
       <c r="BT24" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="BX24" s="16" t="s">
         <v>301</v>
       </c>
     </row>
@@ -4591,47 +4650,47 @@
         <v>89</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>413</v>
+        <v>438</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>58</v>
       </c>
       <c r="E25" s="20"/>
       <c r="F25" s="15" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>414</v>
+        <v>392</v>
       </c>
       <c r="H25" s="15" t="s">
         <v>55</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="J25" s="17">
         <v>44007</v>
       </c>
       <c r="K25" s="18" t="s">
-        <v>405</v>
+        <v>385</v>
       </c>
       <c r="L25" s="16" t="s">
-        <v>406</v>
+        <v>386</v>
       </c>
       <c r="M25" s="16" t="s">
-        <v>407</v>
+        <v>387</v>
       </c>
       <c r="N25" s="16" t="s">
-        <v>408</v>
+        <v>388</v>
       </c>
       <c r="P25" s="19" t="s">
-        <v>412</v>
+        <v>391</v>
       </c>
       <c r="Q25" s="5" t="s">
-        <v>428</v>
+        <v>440</v>
       </c>
       <c r="R25" s="16" t="s">
-        <v>409</v>
+        <v>389</v>
       </c>
       <c r="S25" s="16" t="s">
         <v>301</v>
@@ -4642,8 +4701,11 @@
       <c r="X25" s="16" t="s">
         <v>301</v>
       </c>
+      <c r="AH25" s="16" t="s">
+        <v>317</v>
+      </c>
       <c r="AI25" s="16" t="s">
-        <v>317</v>
+        <v>379</v>
       </c>
       <c r="AJ25" s="16" t="s">
         <v>300</v>
@@ -4655,22 +4717,22 @@
         <v>308</v>
       </c>
       <c r="AR25" s="16" t="s">
-        <v>410</v>
+        <v>390</v>
       </c>
       <c r="AU25" s="16" t="s">
         <v>308</v>
       </c>
       <c r="AV25" s="16" t="s">
-        <v>410</v>
+        <v>390</v>
       </c>
       <c r="AY25" s="16" t="s">
         <v>301</v>
       </c>
       <c r="BC25" s="16" t="s">
-        <v>61</v>
+        <v>405</v>
       </c>
       <c r="BD25" s="16" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="BE25" s="16" t="s">
         <v>62</v>
@@ -4685,27 +4747,55 @@
         <v>301</v>
       </c>
     </row>
-    <row r="26" spans="1:99" ht="42" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:99" ht="407" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
         <v>58</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="H26" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="K26" s="27"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="5"/>
+        <v>89</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>439</v>
+      </c>
+      <c r="E26" s="20"/>
+      <c r="F26" s="15" t="s">
+        <v>446</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>392</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>384</v>
+      </c>
+      <c r="J26" s="17">
+        <v>44007</v>
+      </c>
+      <c r="K26" s="18" t="s">
+        <v>442</v>
+      </c>
+      <c r="L26" s="16" t="s">
+        <v>386</v>
+      </c>
+      <c r="M26" s="16" t="s">
+        <v>387</v>
+      </c>
+      <c r="N26" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="P26" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="Q26" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="R26" s="16" t="s">
+        <v>389</v>
+      </c>
       <c r="S26" s="16" t="s">
         <v>301</v>
-      </c>
-      <c r="T26" s="16">
-        <v>20</v>
       </c>
       <c r="U26" s="16" t="s">
         <v>300</v>
@@ -4713,190 +4803,411 @@
       <c r="X26" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="Y26" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="AA26" s="16">
-        <v>5</v>
-      </c>
-      <c r="AB26" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="AD26" s="16">
-        <v>5</v>
-      </c>
-      <c r="AE26" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="AG26" s="16">
-        <v>5</v>
+      <c r="AH26" s="16" t="s">
+        <v>317</v>
+      </c>
+      <c r="AI26" s="16" t="s">
+        <v>379</v>
       </c>
       <c r="AJ26" s="16" t="s">
         <v>300</v>
       </c>
-      <c r="AL26" s="16">
-        <v>5</v>
-      </c>
-      <c r="AM26" s="16">
-        <v>24</v>
-      </c>
-      <c r="AN26" s="16">
-        <v>100</v>
-      </c>
-      <c r="AO26" s="16">
-        <v>400</v>
-      </c>
       <c r="AP26" s="16" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="AQ26" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="AS26" s="16">
-        <v>5</v>
-      </c>
-      <c r="AT26" s="16">
-        <v>5</v>
+        <v>308</v>
+      </c>
+      <c r="AR26" s="16" t="s">
+        <v>390</v>
       </c>
       <c r="AU26" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="AW26" s="16">
-        <v>5</v>
-      </c>
-      <c r="AX26" s="16">
-        <v>5</v>
+        <v>308</v>
+      </c>
+      <c r="AV26" s="16" t="s">
+        <v>390</v>
       </c>
       <c r="AY26" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="BA26" s="16">
-        <v>5</v>
-      </c>
-      <c r="BB26" s="16">
-        <v>5</v>
+      <c r="BC26" s="16" t="s">
+        <v>405</v>
       </c>
       <c r="BD26" s="16" t="s">
-        <v>300</v>
+        <v>379</v>
+      </c>
+      <c r="BE26" s="16" t="s">
+        <v>62</v>
       </c>
       <c r="BG26" s="16">
         <v>5</v>
       </c>
-      <c r="BH26" s="16">
+      <c r="BK26" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="BX26" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="BY26" s="16" t="s">
+        <v>416</v>
+      </c>
+      <c r="BZ26" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="CD26" s="16" t="s">
+        <v>406</v>
+      </c>
+      <c r="CG26" s="28">
+        <v>55</v>
+      </c>
+      <c r="CH26" s="28">
+        <v>2.1</v>
+      </c>
+      <c r="CI26" s="28">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:99" ht="407" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>443</v>
+      </c>
+      <c r="E27" s="20"/>
+      <c r="F27" s="15" t="s">
+        <v>445</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>392</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>384</v>
+      </c>
+      <c r="J27" s="17">
+        <v>44007</v>
+      </c>
+      <c r="K27" s="18" t="s">
+        <v>444</v>
+      </c>
+      <c r="L27" s="16" t="s">
+        <v>386</v>
+      </c>
+      <c r="M27" s="16" t="s">
+        <v>387</v>
+      </c>
+      <c r="N27" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="P27" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="Q27" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="R27" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="S27" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="U27" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="X27" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="AH27" s="16" t="s">
+        <v>317</v>
+      </c>
+      <c r="AI27" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="AJ27" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="AP27" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="AQ27" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="AR27" s="16" t="s">
+        <v>390</v>
+      </c>
+      <c r="AU27" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="AV27" s="16" t="s">
+        <v>390</v>
+      </c>
+      <c r="AY27" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="BC27" s="16" t="s">
+        <v>405</v>
+      </c>
+      <c r="BD27" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="BE27" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="BG27" s="16">
+        <v>5</v>
+      </c>
+      <c r="BK27" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="BX27" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="BY27" s="16" t="s">
+        <v>405</v>
+      </c>
+      <c r="BZ27" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="CA27" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="CC27" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="CD27" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="CF27" s="28">
+        <v>50</v>
+      </c>
+      <c r="CJ27" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="CK27" s="16">
+        <v>50</v>
+      </c>
+      <c r="CP27" s="16" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="28" spans="1:99" ht="42" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="K28" s="27"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="5"/>
+      <c r="S28" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="T28" s="16">
+        <v>20</v>
+      </c>
+      <c r="U28" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="X28" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="Y28" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="AA28" s="16">
+        <v>5</v>
+      </c>
+      <c r="AB28" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="AD28" s="16">
+        <v>5</v>
+      </c>
+      <c r="AE28" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="AG28" s="16">
+        <v>5</v>
+      </c>
+      <c r="AJ28" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="AL28" s="16">
+        <v>5</v>
+      </c>
+      <c r="AM28" s="16">
         <v>24</v>
       </c>
-      <c r="BI26" s="16">
+      <c r="AN28" s="16">
         <v>100</v>
       </c>
-      <c r="BJ26" s="16">
+      <c r="AO28" s="16">
         <v>400</v>
       </c>
-      <c r="BK26" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="BL26" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="BN26" s="16">
+      <c r="AP28" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="AQ28" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="AS28" s="16">
         <v>5</v>
       </c>
-      <c r="BO26" s="16">
+      <c r="AT28" s="16">
         <v>5</v>
       </c>
-      <c r="BP26" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="BR26" s="16">
+      <c r="AU28" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="AW28" s="16">
         <v>5</v>
       </c>
-      <c r="BS26" s="16">
+      <c r="AX28" s="16">
         <v>5</v>
       </c>
-      <c r="BT26" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="BV26" s="16">
+      <c r="AY28" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="BA28" s="16">
         <v>5</v>
       </c>
-      <c r="BW26" s="16">
+      <c r="BB28" s="16">
         <v>5</v>
       </c>
-      <c r="BX26" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="BY26" s="16" t="s">
+      <c r="BD28" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="BG28" s="16">
+        <v>5</v>
+      </c>
+      <c r="BH28" s="16">
+        <v>24</v>
+      </c>
+      <c r="BI28" s="16">
+        <v>100</v>
+      </c>
+      <c r="BJ28" s="16">
+        <v>400</v>
+      </c>
+      <c r="BK28" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="BL28" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="BN28" s="16">
+        <v>5</v>
+      </c>
+      <c r="BO28" s="16">
+        <v>5</v>
+      </c>
+      <c r="BP28" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="BR28" s="16">
+        <v>5</v>
+      </c>
+      <c r="BS28" s="16">
+        <v>5</v>
+      </c>
+      <c r="BT28" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="BV28" s="16">
+        <v>5</v>
+      </c>
+      <c r="BW28" s="16">
+        <v>5</v>
+      </c>
+      <c r="BX28" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="BY28" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="BZ26" s="16" t="s">
+      <c r="BZ28" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="CA26" s="16" t="s">
+      <c r="CA28" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="CB26" s="16">
+      <c r="CB28" s="16">
         <v>0.7</v>
       </c>
-      <c r="CC26" s="16" t="s">
+      <c r="CC28" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CD26" s="16" t="s">
+      <c r="CD28" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="CE26" s="16">
+      <c r="CE28" s="16">
         <v>50</v>
       </c>
-      <c r="CF26" s="28">
+      <c r="CF28" s="28">
         <v>5</v>
       </c>
-      <c r="CG26" s="28">
+      <c r="CG28" s="28">
         <v>5</v>
       </c>
-      <c r="CH26" s="28">
+      <c r="CH28" s="28">
         <v>5</v>
       </c>
-      <c r="CI26" s="28">
+      <c r="CI28" s="28">
         <v>5</v>
       </c>
-      <c r="CJ26" s="16" t="s">
+      <c r="CJ28" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="CK26" s="16">
+      <c r="CK28" s="16">
         <v>5</v>
       </c>
-      <c r="CL26" s="16">
+      <c r="CL28" s="16">
         <v>5</v>
       </c>
-      <c r="CM26" s="28">
+      <c r="CM28" s="28">
         <v>5</v>
       </c>
-      <c r="CN26" s="28">
+      <c r="CN28" s="28">
         <v>5</v>
       </c>
-      <c r="CO26" s="28">
+      <c r="CO28" s="28">
         <v>5</v>
       </c>
-      <c r="CP26" s="16" t="s">
+      <c r="CP28" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="CQ26" s="16">
+      <c r="CQ28" s="16">
         <v>5</v>
       </c>
-      <c r="CR26" s="16">
+      <c r="CR28" s="16">
         <v>5</v>
       </c>
-      <c r="CS26" s="28">
+      <c r="CS28" s="28">
         <v>5</v>
       </c>
-      <c r="CT26" s="28">
+      <c r="CT28" s="28">
         <v>5</v>
       </c>
-      <c r="CU26" s="28">
+      <c r="CU28" s="28">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:CR26">
-    <sortCondition ref="J2:J26"/>
+  <sortState ref="A2:CR28">
+    <sortCondition ref="J2:J28"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
brazil proposal and chair's text alternate overfished
</commit_message>
<xml_diff>
--- a/app/data/wto_proposal_settings_master.xlsx
+++ b/app/data/wto_proposal_settings_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kat/GitHub/SubsidyExplorer/app/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kat/GitHub/SubsidyExplorer/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97665D2A-6CBE-6942-8EB5-FDC47E43F293}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A9FF8B-6C44-764D-9E9F-5E0F0775FE6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16600" yWindow="4500" windowWidth="35700" windowHeight="19140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25220" windowHeight="15220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="507">
   <si>
     <t>proposal</t>
   </si>
@@ -1146,9 +1146,6 @@
   </si>
   <si>
     <t>iuu_scope_select</t>
-  </si>
-  <si>
-    <t>RD/TN/RL/126</t>
   </si>
   <si>
     <t>Chair's draft consolidated text</t>
@@ -1365,18 +1362,9 @@
     <t>These are the values for the Chair's text + China cap proposal</t>
   </si>
   <si>
-    <t>For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternate definitions for an overfished stock subsidy prohibition - we have chosen to model the more ambitious interpretation of the two. For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. No cap-based approach is included.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternate definitions for an overfished stock subsidy prohibition - we have chosen to model the more ambitious interpretation of the two. For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: 1) We assume each Member's cap is equal to whichever of the three proposed approaches for calculating a cap yields the largest amount. By default, caps based on the first approach are calculated as 55% of each Member's base for capping; caps based on the second approach are calculated as 2% of each Member's estimated landed value (calculated from the FAO Global Marine Capture Production Database, average between 2016-2018); caps based on the third approach are calculated as 55% of the global average subsidies per fisher (capacity-enhancing and ambiguous) multiplied by each Member's most recently reported total number of fishers (from the FAO Yearbook of Fishery and Aquaculture Statistics 2017). 2) We assume that provision of the following types of subsidies as defined by Sumaila et al. 2019 are allowed to continue irrespective of a Member's total cap: i) subsidies for fishing access agreements; ii) fisher assistance programs; iii) vessel buyback programs; iv) rural fishers' community development programs. Therefore each Member's base for capping is represented by the total amount of all other capacity-enhancing and ambiguous subsidies estimated by Sumaila et al. 2019. </t>
-  </si>
-  <si>
     <t>These are the values for the Chair's text + USA cap proposal</t>
   </si>
   <si>
-    <t xml:space="preserve">For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternate definitions for an overfished stock subsidy prohibition - we have chosen to model the more ambitious interpretation of the two. For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: 1) 1) We assume that each Member's base for capping is represented by the total amount of capacity-enhancing and ambiguos subsidies estimated by Sumaila et al. 2019. 2) Members are sorted into three tiers based on a three-year average of FAO marine capture production (2016-2018). Members accounting for 0.7% or more of global marine capture production are in "Tier 1"; Members accounting for 0.05% or more, but less than 0.7%, of global marine capture production are in "Tier 2"; Members accounting for less than 0.05% of global marine capture production are in "Tier 3". 3) This proposal advocates for allowing both Tier 1 and Tier 2 Members to negotiate their own subsidy caps or to accept a default cap of $50 million annually. For the purposes of modeling, we assume that Tier 1 Members receive a subsidy cap equal to 50% of their base for capping; Tier 2 Members receive the default cap of $50 million; Tier 3 Members do not receive a cap. </t>
-  </si>
-  <si>
     <t>TOP10</t>
   </si>
   <si>
@@ -1431,21 +1419,6 @@
     <t>Modelled using LDC proposal for prohibitions (except for their S&amp;DT - used that from this proposal instead)</t>
   </si>
   <si>
-    <t>RD/TN/RL/126 &amp; TN/RL/GEN/199</t>
-  </si>
-  <si>
-    <t>RD/TN/RL/126 &amp; TN/RL/GEN/197/Rev.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As written, this proposal places different scopes on prohibtions for boat building and fuel subsidies (all) vs. all other harmful subsidies (HS only). This is not accounted for. OCOF prohibition is assumed to apply to high seas and distant water fishing for all subsidy types. </t>
-  </si>
-  <si>
-    <t>Using the same values for the US proposal above.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Using the same values for the China proposal as above. </t>
-  </si>
-  <si>
     <t>RD/TN/RL/124</t>
   </si>
   <si>
@@ -1461,9 +1434,6 @@
     <t xml:space="preserve">1) We assume that provision of the following types of subsidies as defined by Sumaila et al. 2019 are allowed to continue irrespective of a Member's total de minimus limit: i) fisher assistance programs; ii) rural fishers' community development programs.subsidies (both programs relevant to fishing in territorial waters). Therefore each Member's base subsidy level is represented by the total amount of all other capacity-enhancing and ambiguous subsidies estimated by Sumaila et al. 2019. 2) we estimate the landed value of marine capture fisheries from the FAO Global Capture Production Database. 3) We assume the de minimis limit for developed and developing country members belonging to the top 10 marine capture fisheries producers to be 10% of the average total landed value of the Member's marine capture fisheries between 2016-2018. For all other developing country Members, we assume the de minimis limit to be 20% of the average total landed value between 2016-2018. For LDC Members, we assume the de minimis limit to be 30% of the average total landed value between 2016-2018. </t>
   </si>
   <si>
-    <t xml:space="preserve">1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 0.8) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - this is the less ambitious interpretation of the two (see Australia - Overfishing and overcapacity). </t>
-  </si>
-  <si>
     <t xml:space="preserve">1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text places prohibitions on subsidies for fishing outside of the jurisdictions of coastal Members or relevant RFMO/As. Very few areas of the ocean are not under the jurisdiction of a RFMO/A, but it is difficult to determine on a global scale whether vessels are fishing for species governed by those RFMO/As at any given point in time. We therefore assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels spending at least 5% of their total annual effort fishing on the high seas outside of the jurisdictions of coastal Members. We note that this is an ambitious interpretation of this prohibition. </t>
   </si>
   <si>
@@ -1476,48 +1446,21 @@
     <t>For IUU: Subsidies granted by developing and LDC Members shall be allowed for small scale fishing: a) within their own territorial waters. For Overfished: Subsidies granted by developing and LDC Members for fishing within their own territorial sea shall be allowed. For OCOF: Subsidies granted by LDCs shall be allowed, and subsidies granted by developing countries shall be allowed for fishing in their territorial seas, or for fishing in their EEZs and high seas unless any of the following conditions are met for three consecutive years: a) GNI per capita is greater than US $5000 (constant 2010 US$), b) they engage in distant water fishing, or c) the contribution from Agriculture, Forestry and Fishing to their national GDP (World Bank) is greater than 10%.</t>
   </si>
   <si>
-    <t xml:space="preserve">1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - choose which to model use using the buttons above. </t>
-  </si>
-  <si>
     <t>This is the real entry for this proposal - others are just for options and text</t>
   </si>
   <si>
     <t>Alternate</t>
   </si>
   <si>
-    <t xml:space="preserve">These are the options for the facilitator's text + new zeland/iceland </t>
-  </si>
-  <si>
-    <t>These are the options for the facilitator's text + Australia</t>
-  </si>
-  <si>
     <t>These are the values for the Chair's text + Philipines de mininus proposal</t>
   </si>
   <si>
-    <t>RD/TN/RL/126 &amp; RD/TN/RL/81</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternate definitions for an overfished stock subsidy prohibition - we have chosen to model the more ambitious interpretation of the two. For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: 1) We assume that provision of the following types of subsidies as defined by Sumaila et al. 2019 are allowed to continue irrespective of a Member's total de minimus limit: i) fisher assistance programs; ii) rural fishers' community development programs.subsidies (both programs relevant to fishing in territorial waters). Therefore each Member's base subsidy level is represented by the total amount of all other capacity-enhancing and ambiguous subsidies estimated by Sumaila et al. 2019. 2) we estimate the landed value of marine capture fisheries from the FAO Global Capture Production Database. 3) We assume the de minimis limit for developed and developing country members belonging to the top 10 marine capture fisheries producers to be 10% of the average total landed value of the Member's marine capture fisheries between 2016-2018. For all other developing country Members, we assume the de minimis limit to be 20% of the average total landed value between 2016-2018. For LDC Members, we assume the de minimis limit to be 30% of the average total landed value between 2016-2018. </t>
-  </si>
-  <si>
-    <t>Using the same values for the Philippines proposal above.</t>
-  </si>
-  <si>
-    <t>Using the same values for the Brazil proposal below</t>
-  </si>
-  <si>
-    <t>RD/TN/RL/126 &amp; RD/TN/RL/124</t>
-  </si>
-  <si>
     <t>Brazil - Formula</t>
   </si>
   <si>
     <t>NOT DONE - These are the values for the Chair's text + Brazil formula proposal</t>
   </si>
   <si>
-    <t>NOT DONE</t>
-  </si>
-  <si>
     <t xml:space="preserve">This communication proposes a quantitative approach of reductions and limits to maritime fisheries subsidies. The baseline of reductions is to be the annual average monetary value of fisheries subsidies (3 prior years). A cumulative ranges (8 ranges: 0-15mn to over 1,2bn) of subsidy in monetary values, where each range corresponds to a specific percentage reduction will be applicable (from 0% to 45% in increments of 5). The total subsidy reduction shall equal the sum of the cuts on each range. </t>
   </si>
   <si>
@@ -1545,26 +1488,134 @@
     <t xml:space="preserve">1) We assume each Member's baseline to the total magnitude of capacity-enhancing and ambiguous subsidies estimated by Sumaila et al. 2019. 2) The formula ranges and percentages of reduction are then applied to all Members. </t>
   </si>
   <si>
-    <t xml:space="preserve">For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternate definitions for an overfished stock subsidy prohibition - we have chosen to model the more ambitious interpretation of the two. For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: 1) We assume each Member's baseline to the total magnitude of capacity-enhancing and ambiguous subsidies estimated by Sumaila et al. 2019. 2) The formula ranges and percentages of reduction are then applied to all Members. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Chair's text - Consolidated text </t>
   </si>
   <si>
-    <t>RD/TN/RL/119 &amp; RD/TN/RL/79/Rev.1</t>
-  </si>
-  <si>
-    <t>RD/TN/RL/119 &amp; RD/TN/RL/77/Rev.2</t>
-  </si>
-  <si>
     <t>EU and others - Overfishing and overcapacity</t>
+  </si>
+  <si>
+    <t>BRAZIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chair's text + Brazil proposal + More ambitious overfished </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chair's text + Brazil proposal + Less ambitious overfished </t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126 | RD/TN/RL/124 | Relevant Authorities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chair's text + Phillipines proposal + Less ambitious overfished </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chair's text + Phillipines proposal + More ambitious overfished </t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126 | RD/TN/RL/81 | Objective Definition</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126 | RD/TN/RL/81 | Relevant Authorities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chair's text + USA proposal + More ambitious overfished </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chair's text + USA proposal + Less ambitious overfished </t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126 | TN/RL/GEN/197/Rev.2 | Objective Definition</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126 | TN/RL/GEN/197/Rev.2 | Relevant Authorities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chair's text + China proposal + More ambitious overfished </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chair's text + China proposal + Less ambitious overfished </t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126 | TN/RL/GEN/199 | Objective Definition</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126 | TN/RL/GEN/199 | Relevant Authorities</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/119 | RD/TN/RL/77/Rev.2</t>
+  </si>
+  <si>
+    <t>These are the options for the facilitator's text + less ambitious overfished</t>
+  </si>
+  <si>
+    <t>These are the options for the facilitator's text + more ambitious overfished</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/119 | RD/TN/RL/79/Rev.1</t>
+  </si>
+  <si>
+    <t>1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - this is the more ambitious interpretation of the two (see New Zealand/Iceland - Overfishing and overcapacity).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 0.8) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - this is the less ambitious interpretation of the two (see Australia - Overfished). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - this is the more ambitious interpretation of the two (see New Zealand/Iceland - Overfishing and overcapacity). For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: 1) 1) We assume that each Member's base for capping is represented by the total amount of capacity-enhancing and ambiguos subsidies estimated by Sumaila et al. 2019. 2) Members are sorted into three tiers based on a three-year average of FAO marine capture production (2016-2018). Members accounting for 0.7% or more of global marine capture production are in "Tier 1"; Members accounting for 0.05% or more, but less than 0.7%, of global marine capture production are in "Tier 2"; Members accounting for less than 0.05% of global marine capture production are in "Tier 3". 3) This proposal advocates for allowing both Tier 1 and Tier 2 Members to negotiate their own subsidy caps or to accept a default cap of $50 million annually. For the purposes of modeling, we assume that Tier 1 Members receive a subsidy cap equal to 50% of their base for capping; Tier 2 Members receive the default cap of $50 million; Tier 3 Members do not receive a cap. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - this is the more ambitious interpretation of the two (see New Zealand/Iceland - Overfishing and overcapacity). For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: 1) We assume that provision of the following types of subsidies as defined by Sumaila et al. 2019 are allowed to continue irrespective of a Member's total de minimus limit: i) fisher assistance programs; ii) rural fishers' community development programs.subsidies (both programs relevant to fishing in territorial waters). Therefore each Member's base subsidy level is represented by the total amount of all other capacity-enhancing and ambiguous subsidies estimated by Sumaila et al. 2019. 2) we estimate the landed value of marine capture fisheries from the FAO Global Capture Production Database. 3) We assume the de minimis limit for developed and developing country members belonging to the top 10 marine capture fisheries producers to be 10% of the average total landed value of the Member's marine capture fisheries between 2016-2018. For all other developing country Members, we assume the de minimis limit to be 20% of the average total landed value between 2016-2018. For LDC Members, we assume the de minimis limit to be 30% of the average total landed value between 2016-2018. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - this is the more ambitious interpretation of the two (see New Zealand/Iceland - Overfishing and overcapacity). For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: 1) We assume each Member's baseline to the total magnitude of capacity-enhancing and ambiguous subsidies estimated by Sumaila et al. 2019. 2) The formula ranges and percentages of reduction are then applied to all Members. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 0.8) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - this is the less ambitious interpretation of the two (see Australia - Overfished).  For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: 1) We assume each Member's cap is equal to whichever of the three proposed approaches for calculating a cap yields the largest amount. By default, caps based on the first approach are calculated as 55% of each Member's base for capping; caps based on the second approach are calculated as 2% of each Member's estimated landed value (calculated from the FAO Global Marine Capture Production Database, average between 2016-2018); caps based on the third approach are calculated as 55% of the global average subsidies per fisher (capacity-enhancing and ambiguous) multiplied by each Member's most recently reported total number of fishers (from the FAO Yearbook of Fishery and Aquaculture Statistics 2017). 2) We assume that provision of the following types of subsidies as defined by Sumaila et al. 2019 are allowed to continue irrespective of a Member's total cap: i) subsidies for fishing access agreements; ii) fisher assistance programs; iii) vessel buyback programs; iv) rural fishers' community development programs. Therefore each Member's base for capping is represented by the total amount of all other capacity-enhancing and ambiguous subsidies estimated by Sumaila et al. 2019. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 0.8) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - this is the less ambitious interpretation of the two (see Australia - Overfished). For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: 1) 1) We assume that each Member's base for capping is represented by the total amount of capacity-enhancing and ambiguos subsidies estimated by Sumaila et al. 2019. 2) Members are sorted into three tiers based on a three-year average of FAO marine capture production (2016-2018). Members accounting for 0.7% or more of global marine capture production are in "Tier 1"; Members accounting for 0.05% or more, but less than 0.7%, of global marine capture production are in "Tier 2"; Members accounting for less than 0.05% of global marine capture production are in "Tier 3". 3) This proposal advocates for allowing both Tier 1 and Tier 2 Members to negotiate their own subsidy caps or to accept a default cap of $50 million annually. For the purposes of modeling, we assume that Tier 1 Members receive a subsidy cap equal to 50% of their base for capping; Tier 2 Members receive the default cap of $50 million; Tier 3 Members do not receive a cap. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 0.8) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - this is the less ambitious interpretation of the two (see Australia - Overfished). For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: 1) We assume each Member's baseline to the total magnitude of capacity-enhancing and ambiguous subsidies estimated by Sumaila et al. 2019. 2) The formula ranges and percentages of reduction are then applied to all Members. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 0.8) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - this is the less ambitious interpretation of the two (see Australia - Overfished). For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: 1) We assume that provision of the following types of subsidies as defined by Sumaila et al. 2019 are allowed to continue irrespective of a Member's total de minimus limit: i) fisher assistance programs; ii) rural fishers' community development programs.subsidies (both programs relevant to fishing in territorial waters). Therefore each Member's base subsidy level is represented by the total amount of all other capacity-enhancing and ambiguous subsidies estimated by Sumaila et al. 2019. 2) we estimate the landed value of marine capture fisheries from the FAO Global Capture Production Database. 3) We assume the de minimis limit for developed and developing country members belonging to the top 10 marine capture fisheries producers to be 10% of the average total landed value of the Member's marine capture fisheries between 2016-2018. For all other developing country Members, we assume the de minimis limit to be 20% of the average total landed value between 2016-2018. For LDC Members, we assume the de minimis limit to be 30% of the average total landed value between 2016-2018. </t>
+  </si>
+  <si>
+    <t>Need to check that it's working</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chair's text + Less ambitious overfished </t>
+  </si>
+  <si>
+    <t>Blank entry for Chair's text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chair's text + More ambitious overfished </t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126 | Objective Definition</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126 | Relevant Authorities</t>
+  </si>
+  <si>
+    <t>For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 0.8) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - this is the less ambitious interpretation of the two (see Australia - Overfished).  For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: None.</t>
+  </si>
+  <si>
+    <t>For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - this is the more ambitious interpretation of the two (see New Zealand/Iceland - Overfishing and overcapacity). For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: None.</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126 | RD/TN/RL/124 | Objective Definition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2548,14 +2599,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CU33"/>
+  <dimension ref="A1:CU39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="12"/>
     <col min="2" max="2" width="10.83203125" style="14"/>
@@ -2582,7 +2633,7 @@
     <col min="100" max="16384" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" s="8" customFormat="1" ht="56" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:99" s="8" customFormat="1" ht="56">
       <c r="A1" s="5" t="s">
         <v>141</v>
       </c>
@@ -2590,7 +2641,7 @@
         <v>88</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>329</v>
@@ -2836,13 +2887,13 @@
         <v>45</v>
       </c>
       <c r="CG1" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="CH1" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="CH1" s="8" t="s">
+      <c r="CI1" s="8" t="s">
         <v>398</v>
-      </c>
-      <c r="CI1" s="8" t="s">
-        <v>399</v>
       </c>
       <c r="CJ1" s="8" t="s">
         <v>46</v>
@@ -2854,13 +2905,13 @@
         <v>49</v>
       </c>
       <c r="CM1" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="CN1" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="CN1" s="8" t="s">
+      <c r="CO1" s="8" t="s">
         <v>401</v>
-      </c>
-      <c r="CO1" s="8" t="s">
-        <v>402</v>
       </c>
       <c r="CP1" s="8" t="s">
         <v>50</v>
@@ -2872,16 +2923,16 @@
         <v>53</v>
       </c>
       <c r="CS1" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="CT1" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="CT1" s="8" t="s">
+      <c r="CU1" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="CU1" s="8" t="s">
-        <v>405</v>
-      </c>
     </row>
-    <row r="2" spans="1:99" s="8" customFormat="1" ht="282" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:99" s="8" customFormat="1" ht="282" customHeight="1">
       <c r="A2" s="12" t="s">
         <v>58</v>
       </c>
@@ -2889,7 +2940,7 @@
         <v>98</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>317</v>
@@ -2898,7 +2949,7 @@
         <v>58</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>99</v>
@@ -2931,7 +2982,7 @@
         <v>333</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="R2" s="15"/>
       <c r="S2" s="15"/>
@@ -3001,18 +3052,18 @@
         <v>307</v>
       </c>
       <c r="BY2" s="15" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="BZ2" s="15" t="s">
         <v>301</v>
       </c>
       <c r="CA2" s="15" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="CB2" s="15"/>
       <c r="CC2" s="15"/>
       <c r="CD2" s="29" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="CE2" s="15"/>
       <c r="CF2" s="27">
@@ -3022,7 +3073,7 @@
       <c r="CH2" s="27"/>
       <c r="CI2" s="27"/>
       <c r="CJ2" s="15" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="CL2" s="15">
         <v>20</v>
@@ -3031,7 +3082,7 @@
       <c r="CN2" s="27"/>
       <c r="CO2" s="27"/>
       <c r="CP2" s="15" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="CQ2" s="15"/>
       <c r="CR2" s="15">
@@ -3041,7 +3092,7 @@
       <c r="CT2" s="27"/>
       <c r="CU2" s="27"/>
     </row>
-    <row r="3" spans="1:99" ht="182" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:99" ht="182">
       <c r="A3" s="12" t="s">
         <v>58</v>
       </c>
@@ -3049,7 +3100,7 @@
         <v>98</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>317</v>
@@ -3112,7 +3163,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:99" ht="238" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:99" ht="238">
       <c r="A4" s="12" t="s">
         <v>58</v>
       </c>
@@ -3120,7 +3171,7 @@
         <v>98</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>317</v>
@@ -3157,7 +3208,7 @@
         <v>333</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="X4" s="15" t="s">
         <v>300</v>
@@ -3172,13 +3223,13 @@
         <v>307</v>
       </c>
       <c r="BY4" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="BZ4" s="15" t="s">
         <v>319</v>
       </c>
       <c r="CD4" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="CG4" s="27">
         <v>55</v>
@@ -3190,7 +3241,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:99" ht="182" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:99" ht="182">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -3198,7 +3249,7 @@
         <v>124</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>317</v>
@@ -3210,7 +3261,7 @@
         <v>132</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I5" s="15" t="s">
         <v>55</v>
@@ -3237,7 +3288,7 @@
         <v>333</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="X5" s="15" t="s">
         <v>300</v>
@@ -3258,7 +3309,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:99" ht="182" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:99" ht="182">
       <c r="A6" s="12" t="s">
         <v>58</v>
       </c>
@@ -3266,7 +3317,7 @@
         <v>90</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>317</v>
@@ -3326,7 +3377,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:99" ht="112" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:99" ht="112">
       <c r="A7" s="12" t="s">
         <v>58</v>
       </c>
@@ -3334,16 +3385,16 @@
         <v>98</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>58</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>102</v>
@@ -3373,7 +3424,7 @@
         <v>333</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="X7" s="15" t="s">
         <v>300</v>
@@ -3382,7 +3433,7 @@
         <v>300</v>
       </c>
       <c r="BC7" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="BD7" s="15" t="s">
         <v>371</v>
@@ -3400,7 +3451,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:99" ht="182" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:99" ht="182">
       <c r="A8" s="12" t="s">
         <v>58</v>
       </c>
@@ -3483,7 +3534,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:99" ht="140" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:99" ht="140">
       <c r="A9" s="12" t="s">
         <v>58</v>
       </c>
@@ -3491,7 +3542,7 @@
         <v>124</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>317</v>
@@ -3554,7 +3605,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:99" ht="168" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:99" ht="168">
       <c r="A10" s="12" t="s">
         <v>58</v>
       </c>
@@ -3562,7 +3613,7 @@
         <v>98</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>317</v>
@@ -3574,7 +3625,7 @@
         <v>68</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I10" s="14" t="s">
         <v>58</v>
@@ -3595,13 +3646,13 @@
         <v>128</v>
       </c>
       <c r="O10" s="15" t="s">
-        <v>477</v>
+        <v>458</v>
       </c>
       <c r="P10" s="20" t="s">
         <v>333</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="X10" s="15" t="s">
         <v>300</v>
@@ -3616,7 +3667,7 @@
         <v>307</v>
       </c>
       <c r="BY10" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="BZ10" s="15" t="s">
         <v>301</v>
@@ -3643,7 +3694,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="11" spans="1:99" ht="154" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:99" ht="154">
       <c r="A11" s="12" t="s">
         <v>58</v>
       </c>
@@ -3651,7 +3702,7 @@
         <v>98</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>317</v>
@@ -3690,7 +3741,7 @@
         <v>333</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="X11" s="15" t="s">
         <v>300</v>
@@ -3699,7 +3750,7 @@
         <v>300</v>
       </c>
       <c r="BC11" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="BD11" s="15" t="s">
         <v>371</v>
@@ -3723,7 +3774,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:99" ht="84" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:99" ht="84">
       <c r="A12" s="12" t="s">
         <v>58</v>
       </c>
@@ -3731,7 +3782,7 @@
         <v>90</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>317</v>
@@ -3767,7 +3818,7 @@
         <v>333</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="R12" s="15" t="s">
         <v>260</v>
@@ -3791,7 +3842,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:99" ht="136.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:99" ht="136.5" customHeight="1">
       <c r="A13" s="12" t="s">
         <v>58</v>
       </c>
@@ -3808,7 +3859,7 @@
         <v>85</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I13" s="14" t="s">
         <v>58</v>
@@ -3835,7 +3886,7 @@
         <v>333</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="X13" s="15" t="s">
         <v>300</v>
@@ -3844,7 +3895,7 @@
         <v>300</v>
       </c>
       <c r="BC13" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="BD13" s="15" t="s">
         <v>371</v>
@@ -3859,7 +3910,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:99" ht="224" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:99" ht="224">
       <c r="A14" s="12" t="s">
         <v>58</v>
       </c>
@@ -3867,7 +3918,7 @@
         <v>98</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>352</v>
@@ -3894,7 +3945,7 @@
         <v>43775</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>489</v>
+        <v>467</v>
       </c>
       <c r="M14" s="15" t="s">
         <v>118</v>
@@ -3909,7 +3960,7 @@
         <v>351</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="X14" s="15" t="s">
         <v>300</v>
@@ -3954,7 +4005,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:99" ht="154" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:99" ht="154">
       <c r="A15" s="12" t="s">
         <v>58</v>
       </c>
@@ -3962,7 +4013,7 @@
         <v>90</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>317</v>
@@ -3974,7 +4025,7 @@
         <v>91</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I15" s="15" t="s">
         <v>55</v>
@@ -3995,13 +4046,13 @@
         <v>92</v>
       </c>
       <c r="O15" s="15" t="s">
-        <v>480</v>
+        <v>461</v>
       </c>
       <c r="P15" s="20" t="s">
         <v>333</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="R15" s="15" t="s">
         <v>306</v>
@@ -4025,7 +4076,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:99" ht="70" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:99" ht="70">
       <c r="A16" s="12" t="s">
         <v>55</v>
       </c>
@@ -4033,7 +4084,7 @@
         <v>98</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E16" s="14" t="s">
         <v>58</v>
@@ -4067,10 +4118,10 @@
       </c>
       <c r="P16" s="18"/>
       <c r="Q16" s="4" t="s">
-        <v>483</v>
+        <v>464</v>
       </c>
     </row>
-    <row r="17" spans="1:99" ht="112" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:99" ht="112">
       <c r="A17" s="12" t="s">
         <v>55</v>
       </c>
@@ -4078,7 +4129,7 @@
         <v>98</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>58</v>
@@ -4112,13 +4163,13 @@
         <v>156</v>
       </c>
       <c r="P17" s="18" t="s">
-        <v>481</v>
+        <v>462</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>482</v>
+        <v>463</v>
       </c>
     </row>
-    <row r="18" spans="1:99" ht="56" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:99" ht="56">
       <c r="A18" s="12" t="s">
         <v>55</v>
       </c>
@@ -4126,7 +4177,7 @@
         <v>89</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>58</v>
@@ -4160,10 +4211,10 @@
       </c>
       <c r="P18" s="18"/>
       <c r="Q18" s="4" t="s">
-        <v>483</v>
+        <v>464</v>
       </c>
     </row>
-    <row r="19" spans="1:99" ht="224" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:99" ht="224">
       <c r="A19" s="12" t="s">
         <v>58</v>
       </c>
@@ -4171,7 +4222,7 @@
         <v>124</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>58</v>
@@ -4198,20 +4249,20 @@
         <v>127</v>
       </c>
       <c r="O19" s="15" t="s">
-        <v>479</v>
+        <v>460</v>
       </c>
       <c r="P19" s="18"/>
       <c r="Q19" s="4"/>
     </row>
-    <row r="20" spans="1:99" ht="224" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:99" ht="224">
       <c r="A20" s="12" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>124</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>465</v>
+        <v>486</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>58</v>
@@ -4238,13 +4289,13 @@
         <v>127</v>
       </c>
       <c r="O20" s="15" t="s">
-        <v>479</v>
+        <v>460</v>
       </c>
       <c r="P20" s="20" t="s">
         <v>333</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>462</v>
+        <v>488</v>
       </c>
       <c r="X20" s="15" t="s">
         <v>300</v>
@@ -4265,21 +4316,21 @@
         <v>300</v>
       </c>
     </row>
-    <row r="21" spans="1:99" ht="224" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:99" ht="224">
       <c r="A21" s="12" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>124</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>466</v>
+        <v>485</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>58</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="I21" s="15" t="s">
         <v>55</v>
@@ -4300,13 +4351,13 @@
         <v>127</v>
       </c>
       <c r="O21" s="15" t="s">
-        <v>479</v>
+        <v>460</v>
       </c>
       <c r="P21" s="20" t="s">
         <v>333</v>
       </c>
       <c r="Q21" s="4" t="s">
-        <v>457</v>
+        <v>489</v>
       </c>
       <c r="X21" s="15" t="s">
         <v>300</v>
@@ -4327,7 +4378,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="22" spans="1:99" ht="238" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:99" ht="238">
       <c r="A22" s="12" t="s">
         <v>58</v>
       </c>
@@ -4335,7 +4386,7 @@
         <v>98</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>317</v>
@@ -4374,7 +4425,7 @@
         <v>333</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
       <c r="X22" s="15" t="s">
         <v>300</v>
@@ -4389,7 +4440,7 @@
         <v>300</v>
       </c>
       <c r="BC22" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="BD22" s="15" t="s">
         <v>371</v>
@@ -4407,7 +4458,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="23" spans="1:99" ht="112" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:99" ht="112">
       <c r="A23" s="12" t="s">
         <v>58</v>
       </c>
@@ -4415,7 +4466,7 @@
         <v>90</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>58</v>
@@ -4424,10 +4475,10 @@
         <v>323</v>
       </c>
       <c r="G23" s="15" t="s">
+        <v>391</v>
+      </c>
+      <c r="H23" s="15" t="s">
         <v>392</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>393</v>
       </c>
       <c r="I23" s="15" t="s">
         <v>55</v>
@@ -4451,10 +4502,10 @@
         <v>331</v>
       </c>
       <c r="P23" s="18" t="s">
+        <v>414</v>
+      </c>
+      <c r="Q23" s="4" t="s">
         <v>415</v>
-      </c>
-      <c r="Q23" s="4" t="s">
-        <v>416</v>
       </c>
       <c r="R23" s="15" t="s">
         <v>306</v>
@@ -4505,7 +4556,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="24" spans="1:99" ht="238" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:99" ht="238">
       <c r="A24" s="12" t="s">
         <v>58</v>
       </c>
@@ -4513,7 +4564,7 @@
         <v>98</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>317</v>
@@ -4549,10 +4600,10 @@
         <v>357</v>
       </c>
       <c r="P24" s="18" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="X24" s="15" t="s">
         <v>300</v>
@@ -4585,7 +4636,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="25" spans="1:99" ht="266" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:99" ht="266">
       <c r="A25" s="5" t="s">
         <v>58</v>
       </c>
@@ -4628,10 +4679,10 @@
         <v>360</v>
       </c>
       <c r="P25" s="24" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="Q25" s="25" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
       <c r="R25" s="15" t="s">
         <v>306</v>
@@ -4701,13 +4752,13 @@
       <c r="BA25" s="8"/>
       <c r="BB25" s="8"/>
       <c r="BC25" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="BD25" s="8" t="s">
         <v>371</v>
       </c>
       <c r="BE25" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="BF25" s="8"/>
       <c r="BG25" s="8"/>
@@ -4772,7 +4823,7 @@
       <c r="CT25" s="8"/>
       <c r="CU25" s="8"/>
     </row>
-    <row r="26" spans="1:99" ht="318" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:99" ht="318" customHeight="1">
       <c r="A26" s="12" t="s">
         <v>58</v>
       </c>
@@ -4780,10 +4831,10 @@
         <v>89</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E26" s="14" t="s">
         <v>58</v>
@@ -4811,13 +4862,13 @@
         <v>359</v>
       </c>
       <c r="O26" s="15" t="s">
-        <v>478</v>
+        <v>459</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="R26" s="15" t="s">
         <v>306</v>
@@ -4865,25 +4916,25 @@
         <v>307</v>
       </c>
       <c r="AR26" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AU26" s="15" t="s">
         <v>307</v>
       </c>
       <c r="AV26" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AY26" s="15" t="s">
         <v>300</v>
       </c>
       <c r="BC26" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="BD26" s="8" t="s">
         <v>371</v>
       </c>
       <c r="BE26" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="BH26" s="8">
         <v>24</v>
@@ -4904,7 +4955,7 @@
         <v>307</v>
       </c>
       <c r="BQ26" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="BT26" s="15" t="s">
         <v>300</v>
@@ -4913,7 +4964,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="27" spans="1:99" ht="407" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:99" ht="318" customHeight="1">
       <c r="A27" s="12" t="s">
         <v>58</v>
       </c>
@@ -4921,185 +4972,107 @@
         <v>89</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>449</v>
+        <v>499</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E27" s="14" t="s">
         <v>58</v>
       </c>
       <c r="F27" s="19"/>
       <c r="G27" s="14" t="s">
+        <v>505</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J27" s="15" t="s">
         <v>375</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="I27" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="J27" s="15" t="s">
-        <v>376</v>
       </c>
       <c r="K27" s="16">
         <v>44007</v>
       </c>
       <c r="L27" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="M27" s="15" t="s">
         <v>377</v>
       </c>
-      <c r="M27" s="15" t="s">
+      <c r="N27" s="15" t="s">
         <v>378</v>
       </c>
-      <c r="N27" s="15" t="s">
+      <c r="O27" s="15" t="s">
         <v>379</v>
       </c>
-      <c r="O27" s="15" t="s">
-        <v>380</v>
-      </c>
-      <c r="P27" s="18" t="s">
-        <v>461</v>
-      </c>
-      <c r="Q27" s="4" t="s">
-        <v>425</v>
-      </c>
-      <c r="R27" s="15" t="s">
-        <v>381</v>
-      </c>
-      <c r="S27" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="U27" s="15" t="s">
-        <v>299</v>
-      </c>
-      <c r="X27" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="Y27" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="Z27" s="15" t="s">
-        <v>382</v>
-      </c>
-      <c r="AB27" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="AC27" s="15" t="s">
-        <v>382</v>
-      </c>
-      <c r="AE27" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="AH27" s="15" t="s">
-        <v>316</v>
-      </c>
-      <c r="AI27" s="15" t="s">
-        <v>371</v>
-      </c>
-      <c r="AJ27" s="15" t="s">
-        <v>299</v>
-      </c>
-      <c r="AP27" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="AQ27" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="AR27" s="15" t="s">
-        <v>382</v>
-      </c>
-      <c r="AU27" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="AV27" s="15" t="s">
-        <v>382</v>
-      </c>
-      <c r="AY27" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="BC27" s="15" t="s">
-        <v>395</v>
-      </c>
-      <c r="BD27" s="15" t="s">
-        <v>371</v>
-      </c>
-      <c r="BE27" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="BG27" s="15">
-        <v>5</v>
-      </c>
-      <c r="BK27" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="BL27" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="BM27" s="15" t="s">
-        <v>299</v>
-      </c>
-      <c r="BP27" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="BQ27" s="15" t="s">
-        <v>382</v>
-      </c>
-      <c r="BT27" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="BX27" s="15" t="s">
-        <v>300</v>
-      </c>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="4"/>
+      <c r="S27" s="8"/>
+      <c r="T27" s="8"/>
+      <c r="U27" s="8"/>
+      <c r="V27" s="8"/>
+      <c r="W27" s="8"/>
+      <c r="X27" s="8"/>
+      <c r="AH27" s="8"/>
+      <c r="BD27" s="8"/>
+      <c r="BE27" s="8"/>
+      <c r="BH27" s="8"/>
     </row>
-    <row r="28" spans="1:99" ht="407" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:99" ht="407" customHeight="1">
       <c r="A28" s="12" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>451</v>
+        <v>500</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>424</v>
+        <v>422</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>58</v>
       </c>
       <c r="F28" s="19"/>
       <c r="G28" s="14" t="s">
-        <v>447</v>
+        <v>501</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I28" s="14" t="s">
         <v>55</v>
       </c>
       <c r="J28" s="15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K28" s="16">
         <v>44007</v>
       </c>
       <c r="L28" s="17" t="s">
-        <v>486</v>
+        <v>376</v>
       </c>
       <c r="M28" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="N28" s="15" t="s">
         <v>378</v>
       </c>
-      <c r="N28" s="15" t="s">
+      <c r="O28" s="15" t="s">
         <v>379</v>
       </c>
-      <c r="O28" s="15" t="s">
+      <c r="P28" s="18" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q28" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="R28" s="15" t="s">
         <v>380</v>
-      </c>
-      <c r="P28" s="18" t="s">
-        <v>461</v>
-      </c>
-      <c r="Q28" s="4" t="s">
-        <v>426</v>
-      </c>
-      <c r="R28" s="15" t="s">
-        <v>381</v>
       </c>
       <c r="S28" s="15" t="s">
         <v>300</v>
@@ -5114,13 +5087,13 @@
         <v>307</v>
       </c>
       <c r="Z28" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AB28" s="15" t="s">
         <v>307</v>
       </c>
       <c r="AC28" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AE28" s="15" t="s">
         <v>300</v>
@@ -5141,19 +5114,19 @@
         <v>307</v>
       </c>
       <c r="AR28" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AU28" s="15" t="s">
         <v>307</v>
       </c>
       <c r="AV28" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AY28" s="15" t="s">
         <v>300</v>
       </c>
       <c r="BC28" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="BD28" s="15" t="s">
         <v>371</v>
@@ -5177,82 +5150,67 @@
         <v>307</v>
       </c>
       <c r="BQ28" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="BT28" s="15" t="s">
         <v>300</v>
       </c>
       <c r="BX28" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="BY28" s="15" t="s">
-        <v>406</v>
-      </c>
-      <c r="BZ28" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="CD28" s="15" t="s">
-        <v>396</v>
-      </c>
-      <c r="CG28" s="27">
-        <v>55</v>
-      </c>
-      <c r="CH28" s="27">
-        <v>2.1</v>
-      </c>
-      <c r="CI28" s="27">
-        <v>55</v>
+        <v>300</v>
       </c>
     </row>
-    <row r="29" spans="1:99" ht="407" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:99" ht="407" customHeight="1">
       <c r="A29" s="12" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>450</v>
+        <v>498</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>427</v>
+        <v>422</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>58</v>
       </c>
       <c r="F29" s="19"/>
       <c r="G29" s="14" t="s">
-        <v>448</v>
+        <v>502</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I29" s="14" t="s">
         <v>55</v>
       </c>
       <c r="J29" s="15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K29" s="16">
         <v>44007</v>
       </c>
       <c r="L29" s="17" t="s">
-        <v>486</v>
+        <v>376</v>
       </c>
       <c r="M29" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="N29" s="15" t="s">
         <v>378</v>
       </c>
-      <c r="N29" s="15" t="s">
+      <c r="O29" s="15" t="s">
         <v>379</v>
       </c>
-      <c r="O29" s="15" t="s">
+      <c r="P29" s="18" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q29" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="R29" s="15" t="s">
         <v>380</v>
-      </c>
-      <c r="P29" s="18" t="s">
-        <v>461</v>
-      </c>
-      <c r="Q29" s="4" t="s">
-        <v>428</v>
-      </c>
-      <c r="R29" s="15" t="s">
-        <v>381</v>
       </c>
       <c r="S29" s="15" t="s">
         <v>300</v>
@@ -5261,10 +5219,25 @@
         <v>299</v>
       </c>
       <c r="X29" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="Y29" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="Z29" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="AB29" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="AC29" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="AE29" s="15" t="s">
         <v>300</v>
       </c>
       <c r="AH29" s="15" t="s">
-        <v>316</v>
+        <v>342</v>
       </c>
       <c r="AI29" s="15" t="s">
         <v>371</v>
@@ -5279,19 +5252,19 @@
         <v>307</v>
       </c>
       <c r="AR29" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AU29" s="15" t="s">
         <v>307</v>
       </c>
       <c r="AV29" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AY29" s="15" t="s">
         <v>300</v>
       </c>
       <c r="BC29" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="BD29" s="15" t="s">
         <v>371</v>
@@ -5303,88 +5276,76 @@
         <v>5</v>
       </c>
       <c r="BK29" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="BL29" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="BM29" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="BP29" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="BQ29" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="BT29" s="15" t="s">
         <v>300</v>
       </c>
       <c r="BX29" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="BY29" s="15" t="s">
-        <v>395</v>
-      </c>
-      <c r="BZ29" s="15" t="s">
-        <v>301</v>
-      </c>
-      <c r="CA29" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="CC29" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="CD29" s="15" t="s">
-        <v>303</v>
-      </c>
-      <c r="CF29" s="27">
-        <v>50</v>
-      </c>
-      <c r="CJ29" s="15" t="s">
-        <v>304</v>
-      </c>
-      <c r="CK29" s="15">
-        <v>50</v>
-      </c>
-      <c r="CP29" s="15" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:99" ht="407" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:99" ht="407" customHeight="1">
       <c r="A30" s="12" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="B30" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>470</v>
+        <v>480</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>467</v>
+        <v>423</v>
       </c>
       <c r="F30" s="19"/>
       <c r="G30" s="14" t="s">
-        <v>468</v>
+        <v>482</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I30" s="14" t="s">
         <v>55</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K30" s="16">
         <v>44007</v>
       </c>
       <c r="L30" s="17" t="s">
+        <v>466</v>
+      </c>
+      <c r="M30" s="15" t="s">
         <v>377</v>
       </c>
-      <c r="M30" s="15" t="s">
+      <c r="N30" s="15" t="s">
         <v>378</v>
       </c>
-      <c r="N30" s="15" t="s">
+      <c r="O30" s="15" t="s">
         <v>379</v>
       </c>
-      <c r="O30" s="15" t="s">
+      <c r="P30" s="18" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q30" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="R30" s="15" t="s">
         <v>380</v>
-      </c>
-      <c r="P30" s="18" t="s">
-        <v>461</v>
-      </c>
-      <c r="Q30" s="4" t="s">
-        <v>469</v>
-      </c>
-      <c r="R30" s="15" t="s">
-        <v>381</v>
       </c>
       <c r="S30" s="15" t="s">
         <v>300</v>
@@ -5393,6 +5354,21 @@
         <v>299</v>
       </c>
       <c r="X30" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="Y30" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="Z30" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="AB30" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="AC30" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="AE30" s="15" t="s">
         <v>300</v>
       </c>
       <c r="AH30" s="15" t="s">
@@ -5411,19 +5387,19 @@
         <v>307</v>
       </c>
       <c r="AR30" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AU30" s="15" t="s">
         <v>307</v>
       </c>
       <c r="AV30" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AY30" s="15" t="s">
         <v>300</v>
       </c>
       <c r="BC30" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="BD30" s="15" t="s">
         <v>371</v>
@@ -5435,89 +5411,94 @@
         <v>5</v>
       </c>
       <c r="BK30" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="BL30" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="BM30" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="BP30" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="BQ30" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="BT30" s="15" t="s">
         <v>300</v>
       </c>
       <c r="BX30" s="15" t="s">
         <v>307</v>
       </c>
       <c r="BY30" s="15" t="s">
-        <v>431</v>
+        <v>405</v>
       </c>
       <c r="BZ30" s="15" t="s">
-        <v>301</v>
-      </c>
-      <c r="CA30" s="15" t="s">
-        <v>429</v>
-      </c>
-      <c r="CD30" s="29" t="s">
-        <v>430</v>
-      </c>
-      <c r="CF30" s="27">
-        <v>10</v>
-      </c>
-      <c r="CJ30" s="15" t="s">
-        <v>430</v>
-      </c>
-      <c r="CK30" s="8"/>
-      <c r="CL30" s="15">
-        <v>20</v>
-      </c>
-      <c r="CP30" s="15" t="s">
-        <v>430</v>
-      </c>
-      <c r="CR30" s="15">
-        <v>30</v>
+        <v>319</v>
+      </c>
+      <c r="CD30" s="15" t="s">
+        <v>395</v>
+      </c>
+      <c r="CG30" s="27">
+        <v>55</v>
+      </c>
+      <c r="CH30" s="27">
+        <v>2.1</v>
+      </c>
+      <c r="CI30" s="27">
+        <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:99" ht="407" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:99" ht="407" customHeight="1">
       <c r="A31" s="12" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="B31" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>471</v>
+        <v>481</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>474</v>
+        <v>423</v>
       </c>
       <c r="F31" s="19"/>
       <c r="G31" s="14" t="s">
-        <v>472</v>
+        <v>483</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I31" s="14" t="s">
         <v>55</v>
       </c>
       <c r="J31" s="15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K31" s="16">
         <v>44007</v>
       </c>
       <c r="L31" s="17" t="s">
+        <v>466</v>
+      </c>
+      <c r="M31" s="15" t="s">
         <v>377</v>
       </c>
-      <c r="M31" s="15" t="s">
+      <c r="N31" s="15" t="s">
         <v>378</v>
       </c>
-      <c r="N31" s="15" t="s">
+      <c r="O31" s="15" t="s">
         <v>379</v>
       </c>
-      <c r="O31" s="15" t="s">
+      <c r="P31" s="18" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q31" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="R31" s="15" t="s">
         <v>380</v>
-      </c>
-      <c r="P31" s="18" t="s">
-        <v>461</v>
-      </c>
-      <c r="Q31" s="4" t="s">
-        <v>485</v>
-      </c>
-      <c r="R31" s="15" t="s">
-        <v>381</v>
       </c>
       <c r="S31" s="15" t="s">
         <v>300</v>
@@ -5526,6 +5507,21 @@
         <v>299</v>
       </c>
       <c r="X31" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="Y31" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="Z31" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="AB31" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="AC31" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="AE31" s="15" t="s">
         <v>300</v>
       </c>
       <c r="AH31" s="15" t="s">
@@ -5544,19 +5540,19 @@
         <v>307</v>
       </c>
       <c r="AR31" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AU31" s="15" t="s">
         <v>307</v>
       </c>
       <c r="AV31" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AY31" s="15" t="s">
         <v>300</v>
       </c>
       <c r="BC31" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="BD31" s="15" t="s">
         <v>371</v>
@@ -5568,81 +5564,229 @@
         <v>5</v>
       </c>
       <c r="BK31" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="BL31" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="BM31" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="BP31" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="BQ31" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="BT31" s="15" t="s">
         <v>300</v>
       </c>
       <c r="BX31" s="15" t="s">
-        <v>300</v>
+        <v>307</v>
+      </c>
+      <c r="BY31" s="15" t="s">
+        <v>405</v>
+      </c>
+      <c r="BZ31" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="CD31" s="15" t="s">
+        <v>395</v>
+      </c>
+      <c r="CG31" s="27">
+        <v>55</v>
+      </c>
+      <c r="CH31" s="27">
+        <v>2.1</v>
+      </c>
+      <c r="CI31" s="27">
+        <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:99" ht="407" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:99" ht="407" customHeight="1">
       <c r="A32" s="12" t="s">
-        <v>58</v>
+        <v>453</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>98</v>
+        <v>89</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>476</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>475</v>
+        <v>424</v>
       </c>
       <c r="F32" s="19"/>
-      <c r="G32" s="8" t="s">
-        <v>452</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>452</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="J32" s="8" t="s">
+      <c r="G32" s="14" t="s">
+        <v>478</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J32" s="15" t="s">
+        <v>375</v>
+      </c>
+      <c r="K32" s="16">
+        <v>44007</v>
+      </c>
+      <c r="L32" s="17" t="s">
+        <v>466</v>
+      </c>
+      <c r="M32" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="N32" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="O32" s="15" t="s">
+        <v>379</v>
+      </c>
+      <c r="P32" s="18" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q32" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="R32" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="S32" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="U32" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="X32" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="AH32" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="AI32" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="AJ32" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="AP32" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="AQ32" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="AR32" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="AU32" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="AV32" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="AY32" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="BC32" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="BD32" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="BE32" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="BG32" s="15">
+        <v>5</v>
+      </c>
+      <c r="BK32" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="BX32" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="BY32" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="BZ32" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="CA32" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="CC32" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="CD32" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="CF32" s="27">
+        <v>50</v>
+      </c>
+      <c r="CJ32" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="CK32" s="15">
+        <v>50</v>
+      </c>
+      <c r="CP32" s="15" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="33" spans="1:99" ht="407" customHeight="1">
+      <c r="A33" s="12" t="s">
         <v>453</v>
       </c>
-      <c r="K32" s="23">
-        <v>43890</v>
-      </c>
-      <c r="L32" s="9" t="s">
-        <v>473</v>
-      </c>
-      <c r="M32" s="8" t="s">
-        <v>454</v>
-      </c>
-      <c r="N32" s="8" t="s">
-        <v>455</v>
-      </c>
-      <c r="O32" s="15" t="s">
-        <v>476</v>
-      </c>
-      <c r="P32" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="Q32" s="25" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="33" spans="1:99" ht="42" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
-        <v>58</v>
-      </c>
       <c r="B33" s="13" t="s">
-        <v>83</v>
+        <v>89</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>477</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>475</v>
-      </c>
-      <c r="G33" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="I33" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="L33" s="26"/>
-      <c r="P33" s="18"/>
-      <c r="Q33" s="4"/>
+        <v>424</v>
+      </c>
+      <c r="F33" s="19"/>
+      <c r="G33" s="14" t="s">
+        <v>479</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J33" s="15" t="s">
+        <v>375</v>
+      </c>
+      <c r="K33" s="16">
+        <v>44007</v>
+      </c>
+      <c r="L33" s="17" t="s">
+        <v>466</v>
+      </c>
+      <c r="M33" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="N33" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="O33" s="15" t="s">
+        <v>379</v>
+      </c>
+      <c r="P33" s="18" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q33" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="R33" s="15" t="s">
+        <v>380</v>
+      </c>
       <c r="S33" s="15" t="s">
         <v>300</v>
-      </c>
-      <c r="T33" s="15">
-        <v>20</v>
       </c>
       <c r="U33" s="15" t="s">
         <v>299</v>
@@ -5650,119 +5794,53 @@
       <c r="X33" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="Y33" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="AA33" s="15">
-        <v>5</v>
-      </c>
-      <c r="AB33" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="AD33" s="15">
-        <v>5</v>
-      </c>
-      <c r="AE33" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="AG33" s="15">
-        <v>5</v>
+      <c r="AH33" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="AI33" s="15" t="s">
+        <v>371</v>
       </c>
       <c r="AJ33" s="15" t="s">
         <v>299</v>
       </c>
-      <c r="AL33" s="15">
-        <v>5</v>
-      </c>
-      <c r="AM33" s="15">
-        <v>24</v>
-      </c>
-      <c r="AN33" s="15">
-        <v>100</v>
-      </c>
-      <c r="AO33" s="15">
-        <v>400</v>
-      </c>
       <c r="AP33" s="15" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="AQ33" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="AS33" s="15">
-        <v>5</v>
-      </c>
-      <c r="AT33" s="15">
-        <v>5</v>
+        <v>307</v>
+      </c>
+      <c r="AR33" s="15" t="s">
+        <v>381</v>
       </c>
       <c r="AU33" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="AW33" s="15">
-        <v>5</v>
-      </c>
-      <c r="AX33" s="15">
-        <v>5</v>
+        <v>307</v>
+      </c>
+      <c r="AV33" s="15" t="s">
+        <v>381</v>
       </c>
       <c r="AY33" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="BA33" s="15">
-        <v>5</v>
-      </c>
-      <c r="BB33" s="15">
-        <v>5</v>
+      <c r="BC33" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="BD33" s="15" t="s">
-        <v>299</v>
+        <v>371</v>
+      </c>
+      <c r="BE33" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="BG33" s="15">
         <v>5</v>
       </c>
-      <c r="BH33" s="15">
-        <v>24</v>
-      </c>
-      <c r="BI33" s="15">
-        <v>100</v>
-      </c>
-      <c r="BJ33" s="15">
-        <v>400</v>
-      </c>
       <c r="BK33" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="BL33" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="BN33" s="15">
-        <v>5</v>
-      </c>
-      <c r="BO33" s="15">
-        <v>5</v>
-      </c>
-      <c r="BP33" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="BR33" s="15">
-        <v>5</v>
-      </c>
-      <c r="BS33" s="15">
-        <v>5</v>
-      </c>
-      <c r="BT33" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="BV33" s="15">
-        <v>5</v>
-      </c>
-      <c r="BW33" s="15">
-        <v>5</v>
-      </c>
       <c r="BX33" s="15" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="BY33" s="15" t="s">
-        <v>61</v>
+        <v>394</v>
       </c>
       <c r="BZ33" s="15" t="s">
         <v>301</v>
@@ -5770,70 +5848,792 @@
       <c r="CA33" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="CB33" s="15">
-        <v>0.7</v>
-      </c>
       <c r="CC33" s="15" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="CD33" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="CE33" s="15">
+      <c r="CF33" s="27">
         <v>50</v>
-      </c>
-      <c r="CF33" s="27">
-        <v>5</v>
-      </c>
-      <c r="CG33" s="27">
-        <v>5</v>
-      </c>
-      <c r="CH33" s="27">
-        <v>5</v>
-      </c>
-      <c r="CI33" s="27">
-        <v>5</v>
       </c>
       <c r="CJ33" s="15" t="s">
         <v>304</v>
       </c>
       <c r="CK33" s="15">
-        <v>5</v>
-      </c>
-      <c r="CL33" s="15">
-        <v>5</v>
-      </c>
-      <c r="CM33" s="27">
-        <v>5</v>
-      </c>
-      <c r="CN33" s="27">
-        <v>5</v>
-      </c>
-      <c r="CO33" s="27">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="CP33" s="15" t="s">
         <v>305</v>
       </c>
-      <c r="CQ33" s="15">
+    </row>
+    <row r="34" spans="1:99" ht="407" customHeight="1">
+      <c r="A34" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>473</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>454</v>
+      </c>
+      <c r="F34" s="19"/>
+      <c r="G34" s="14" t="s">
+        <v>474</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="I34" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J34" s="15" t="s">
+        <v>375</v>
+      </c>
+      <c r="K34" s="16">
+        <v>44007</v>
+      </c>
+      <c r="L34" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="M34" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="N34" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="O34" s="15" t="s">
+        <v>379</v>
+      </c>
+      <c r="P34" s="18" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q34" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="R34" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="S34" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="U34" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="X34" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="AH34" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="AI34" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="AJ34" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="AP34" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="AQ34" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="AR34" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="AU34" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="AV34" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="AY34" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="BC34" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="BD34" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="BE34" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="BG34" s="15">
         <v>5</v>
       </c>
-      <c r="CR33" s="15">
+      <c r="BK34" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="BX34" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="BY34" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="BZ34" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="CA34" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="CD34" s="29" t="s">
+        <v>426</v>
+      </c>
+      <c r="CF34" s="27">
+        <v>10</v>
+      </c>
+      <c r="CJ34" s="15" t="s">
+        <v>426</v>
+      </c>
+      <c r="CK34" s="8"/>
+      <c r="CL34" s="15">
+        <v>20</v>
+      </c>
+      <c r="CP34" s="15" t="s">
+        <v>426</v>
+      </c>
+      <c r="CR34" s="15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:99" ht="407" customHeight="1">
+      <c r="A35" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>472</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>454</v>
+      </c>
+      <c r="F35" s="19"/>
+      <c r="G35" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="H35" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="I35" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J35" s="15" t="s">
+        <v>375</v>
+      </c>
+      <c r="K35" s="16">
+        <v>44007</v>
+      </c>
+      <c r="L35" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="M35" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="N35" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="O35" s="15" t="s">
+        <v>379</v>
+      </c>
+      <c r="P35" s="18" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q35" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="R35" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="S35" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="U35" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="X35" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="AH35" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="AI35" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="AJ35" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="AP35" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="AQ35" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="AR35" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="AU35" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="AV35" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="AY35" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="BC35" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="BD35" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="BE35" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="BG35" s="15">
         <v>5</v>
       </c>
-      <c r="CS33" s="27">
+      <c r="BK35" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="BX35" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="BY35" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="BZ35" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="CA35" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="CD35" s="29" t="s">
+        <v>426</v>
+      </c>
+      <c r="CF35" s="27">
+        <v>10</v>
+      </c>
+      <c r="CJ35" s="15" t="s">
+        <v>426</v>
+      </c>
+      <c r="CK35" s="8"/>
+      <c r="CL35" s="15">
+        <v>20</v>
+      </c>
+      <c r="CP35" s="15" t="s">
+        <v>426</v>
+      </c>
+      <c r="CR35" s="15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:99" ht="407" customHeight="1">
+      <c r="A36" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>469</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="F36" s="19"/>
+      <c r="G36" s="14" t="s">
+        <v>506</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J36" s="15" t="s">
+        <v>375</v>
+      </c>
+      <c r="K36" s="16">
+        <v>44007</v>
+      </c>
+      <c r="L36" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="M36" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="N36" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="O36" s="15" t="s">
+        <v>379</v>
+      </c>
+      <c r="P36" s="18" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q36" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="R36" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="S36" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="U36" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="X36" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="AH36" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="AI36" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="AJ36" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="AP36" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="AQ36" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="AR36" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="AU36" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="AV36" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="AY36" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="BC36" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="BD36" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="BE36" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="BG36" s="15">
         <v>5</v>
       </c>
-      <c r="CT33" s="27">
+      <c r="BK36" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="BX36" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="BY36" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="BZ36" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="CD36" s="15" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="37" spans="1:99" ht="407" customHeight="1">
+      <c r="A37" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>470</v>
+      </c>
+      <c r="F37" s="19"/>
+      <c r="G37" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J37" s="15" t="s">
+        <v>375</v>
+      </c>
+      <c r="K37" s="16">
+        <v>44007</v>
+      </c>
+      <c r="L37" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="M37" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="N37" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="O37" s="15" t="s">
+        <v>379</v>
+      </c>
+      <c r="P37" s="18" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q37" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="R37" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="S37" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="U37" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="X37" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="AH37" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="AI37" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="AJ37" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="AP37" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="AQ37" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="AR37" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="AU37" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="AV37" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="AY37" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="BC37" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="BD37" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="BE37" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="BG37" s="15">
         <v>5</v>
       </c>
-      <c r="CU33" s="27">
+      <c r="BK37" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="BX37" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="BY37" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="BZ37" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="CD37" s="15" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="38" spans="1:99" ht="407" customHeight="1">
+      <c r="A38" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>497</v>
+      </c>
+      <c r="F38" s="19"/>
+      <c r="G38" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="K38" s="23">
+        <v>43890</v>
+      </c>
+      <c r="L38" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="M38" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="N38" s="8" t="s">
+        <v>446</v>
+      </c>
+      <c r="O38" s="15" t="s">
+        <v>457</v>
+      </c>
+      <c r="P38" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q38" s="25" t="s">
+        <v>465</v>
+      </c>
+      <c r="X38" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="AP38" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="BK38" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="BX38" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="BY38" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="BZ38" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="CD38" s="15" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="39" spans="1:99" ht="42">
+      <c r="A39" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="L39" s="26"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="4"/>
+      <c r="S39" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="T39" s="15">
+        <v>20</v>
+      </c>
+      <c r="U39" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="X39" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="Y39" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="AA39" s="15">
+        <v>5</v>
+      </c>
+      <c r="AB39" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="AD39" s="15">
+        <v>5</v>
+      </c>
+      <c r="AE39" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="AG39" s="15">
+        <v>5</v>
+      </c>
+      <c r="AJ39" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="AL39" s="15">
+        <v>5</v>
+      </c>
+      <c r="AM39" s="15">
+        <v>24</v>
+      </c>
+      <c r="AN39" s="15">
+        <v>100</v>
+      </c>
+      <c r="AO39" s="15">
+        <v>400</v>
+      </c>
+      <c r="AP39" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="AQ39" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="AS39" s="15">
+        <v>5</v>
+      </c>
+      <c r="AT39" s="15">
+        <v>5</v>
+      </c>
+      <c r="AU39" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="AW39" s="15">
+        <v>5</v>
+      </c>
+      <c r="AX39" s="15">
+        <v>5</v>
+      </c>
+      <c r="AY39" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="BA39" s="15">
+        <v>5</v>
+      </c>
+      <c r="BB39" s="15">
+        <v>5</v>
+      </c>
+      <c r="BD39" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="BG39" s="15">
+        <v>5</v>
+      </c>
+      <c r="BH39" s="15">
+        <v>24</v>
+      </c>
+      <c r="BI39" s="15">
+        <v>100</v>
+      </c>
+      <c r="BJ39" s="15">
+        <v>400</v>
+      </c>
+      <c r="BK39" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="BL39" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="BN39" s="15">
+        <v>5</v>
+      </c>
+      <c r="BO39" s="15">
+        <v>5</v>
+      </c>
+      <c r="BP39" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="BR39" s="15">
+        <v>5</v>
+      </c>
+      <c r="BS39" s="15">
+        <v>5</v>
+      </c>
+      <c r="BT39" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="BV39" s="15">
+        <v>5</v>
+      </c>
+      <c r="BW39" s="15">
+        <v>5</v>
+      </c>
+      <c r="BX39" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="BY39" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="BZ39" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="CA39" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="CB39" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="CC39" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="CD39" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="CE39" s="15">
+        <v>50</v>
+      </c>
+      <c r="CF39" s="27">
+        <v>5</v>
+      </c>
+      <c r="CG39" s="27">
+        <v>5</v>
+      </c>
+      <c r="CH39" s="27">
+        <v>5</v>
+      </c>
+      <c r="CI39" s="27">
+        <v>5</v>
+      </c>
+      <c r="CJ39" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="CK39" s="15">
+        <v>5</v>
+      </c>
+      <c r="CL39" s="15">
+        <v>5</v>
+      </c>
+      <c r="CM39" s="27">
+        <v>5</v>
+      </c>
+      <c r="CN39" s="27">
+        <v>5</v>
+      </c>
+      <c r="CO39" s="27">
+        <v>5</v>
+      </c>
+      <c r="CP39" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="CQ39" s="15">
+        <v>5</v>
+      </c>
+      <c r="CR39" s="15">
+        <v>5</v>
+      </c>
+      <c r="CS39" s="27">
+        <v>5</v>
+      </c>
+      <c r="CT39" s="27">
+        <v>5</v>
+      </c>
+      <c r="CU39" s="27">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:CR33">
-    <sortCondition ref="K2:K33"/>
+  <sortState ref="A2:CR39">
+    <sortCondition ref="K2:K39"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5849,7 +6649,7 @@
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="13.1640625" style="1" customWidth="1"/>
@@ -5865,7 +6665,7 @@
     <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:58" ht="51">
       <c r="A1" s="1" t="s">
         <v>141</v>
       </c>
@@ -6041,7 +6841,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:58" ht="308" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:58" ht="308" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>55</v>
       </c>
@@ -6115,7 +6915,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:58" ht="153" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:58" ht="153">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
@@ -6177,7 +6977,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:58" ht="272" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:58" ht="272">
       <c r="A4" s="1" t="s">
         <v>55</v>
       </c>
@@ -6242,7 +7042,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:58" ht="221" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:58" ht="221">
       <c r="A5" s="1" t="s">
         <v>55</v>
       </c>
@@ -6301,7 +7101,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:58" ht="136" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:58" ht="136">
       <c r="A6" s="1" t="s">
         <v>55</v>
       </c>
@@ -6342,7 +7142,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:58" ht="187" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:58" ht="187">
       <c r="A7" s="1" t="s">
         <v>55</v>
       </c>
@@ -6413,7 +7213,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:58" ht="187" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:58" ht="187">
       <c r="A8" s="1" t="s">
         <v>55</v>
       </c>
@@ -6484,7 +7284,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:58" ht="102" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:58" ht="102">
       <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
@@ -6528,7 +7328,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:58" ht="102" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:58" ht="102">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
@@ -6572,7 +7372,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:58" ht="238" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:58" ht="238">
       <c r="A11" s="1" t="s">
         <v>55</v>
       </c>
@@ -6634,7 +7434,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:58" ht="306" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:58" ht="306">
       <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
@@ -6687,7 +7487,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:58" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:58" ht="51">
       <c r="D13" s="1" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
placeholders added for new proposals - newest Chair's text and artisinal exemptions still to be added.
</commit_message>
<xml_diff>
--- a/app/data/wto_proposal_settings_master.xlsx
+++ b/app/data/wto_proposal_settings_master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kat/GitHub/SubsidyExplorer/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E15F70A-210A-2542-85A0-EDE0FE947993}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C7FB74-4C21-A84D-B9E4-62782A9B6241}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2968,8 +2968,8 @@
   <dimension ref="A1:DC43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
@@ -7748,7 +7748,7 @@
     </row>
     <row r="41" spans="1:107" ht="297" customHeight="1">
       <c r="A41" s="12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B41" s="13" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
new chair's text added
</commit_message>
<xml_diff>
--- a/app/data/wto_proposal_settings_master.xlsx
+++ b/app/data/wto_proposal_settings_master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kat/GitHub/SubsidyExplorer/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C7FB74-4C21-A84D-B9E4-62782A9B6241}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FC9B77-642D-C648-AA19-79AF7F74FFCB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1734" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1854" uniqueCount="629">
   <si>
     <t>proposal</t>
   </si>
@@ -1080,9 +1080,6 @@
   </si>
   <si>
     <t>Chair's text - Consolidated text</t>
-  </si>
-  <si>
-    <t>This communication was circulated at the request of the Chair of the Negotiating Group on Rules on June 25, 2020.</t>
   </si>
   <si>
     <t>IUU1, IUU2, IUU3, IUU4, IUU5</t>
@@ -1222,45 +1219,24 @@
     <t xml:space="preserve">Chair's text + Brazil proposal + Less ambitious overfished </t>
   </si>
   <si>
-    <t>RD/TN/RL/126 | RD/TN/RL/124 | Relevant Authorities</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chair's text + Phillipines proposal + Less ambitious overfished </t>
   </si>
   <si>
     <t xml:space="preserve">Chair's text + Phillipines proposal + More ambitious overfished </t>
   </si>
   <si>
-    <t>RD/TN/RL/126 | RD/TN/RL/81 | Objective Definition</t>
-  </si>
-  <si>
-    <t>RD/TN/RL/126 | RD/TN/RL/81 | Relevant Authorities</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chair's text + USA proposal + More ambitious overfished </t>
   </si>
   <si>
     <t xml:space="preserve">Chair's text + USA proposal + Less ambitious overfished </t>
   </si>
   <si>
-    <t>RD/TN/RL/126 | TN/RL/GEN/197/Rev.2 | Objective Definition</t>
-  </si>
-  <si>
-    <t>RD/TN/RL/126 | TN/RL/GEN/197/Rev.2 | Relevant Authorities</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chair's text + China proposal + More ambitious overfished </t>
   </si>
   <si>
     <t xml:space="preserve">Chair's text + China proposal + Less ambitious overfished </t>
   </si>
   <si>
-    <t>RD/TN/RL/126 | TN/RL/GEN/199 | Objective Definition</t>
-  </si>
-  <si>
-    <t>RD/TN/RL/126 | TN/RL/GEN/199 | Relevant Authorities</t>
-  </si>
-  <si>
     <t>These are the options for the facilitator's text + less ambitious overfished</t>
   </si>
   <si>
@@ -1273,18 +1249,6 @@
     <t xml:space="preserve">Chair's text + More ambitious overfished </t>
   </si>
   <si>
-    <t>RD/TN/RL/126 | Objective Definition</t>
-  </si>
-  <si>
-    <t>RD/TN/RL/126 | Relevant Authorities</t>
-  </si>
-  <si>
-    <t>RD/TN/RL/126</t>
-  </si>
-  <si>
-    <t>RD/TN/RL/126 | RD/TN/RL/124 | Objective Definition</t>
-  </si>
-  <si>
     <t xml:space="preserve">1) We assume that provision of the following types of subsidies as defined by Sumaila et al. 2019 are allowed to continue irrespective of a Member's total de minimus limit: i) fisher assistance programs; ii) rural fishers' community development programs.subsidies (both programs relevant to fishing in territorial waters). Therefore each Member's base subsidy level is represented by the total amount of all other capacity-enhancing and ambiguous subsidies estimated by Sumaila et al. 2019. 2) We estimate the landed value of marine capture fisheries from the FAO Global Capture Production Database. 3) We assume the de minimis limit for developed and developing country members belonging to the top 10 marine capture fisheries producers to be 10% of the average total landed value of the Member's marine capture fisheries between 2016-2018. For all other developing country Members, we assume the de minimis limit to be 20% of the average total landed value between 2016-2018. For LDC Members, we assume the de minimis limit to be 30% of the average total landed value between 2016-2018. </t>
   </si>
   <si>
@@ -1540,9 +1504,6 @@
     <t>This communication proposes a quantitative approach of reductions and limits to maritime fisheries subsidies that is complementary to the main prohibition. The baseline of reductions is to be the annual average monetary value of fisheries subsidies (3 prior years or 1 year -optional) minus exempted subsidies (cessation, stock protection, artisanal fishing in 12nm zone, disaster relief). It specifies cumulative ranges (8 ranges: 0-15mn to over 1,2bn) of subsidies in monetary value. Members falling in each range will be subject to a specific percentage reduction in total fisheries subsidies (from 0% to 15% and then to 45% in increments of 5). The total subsidy reduction shall equal the sum of the cuts on each range, the upper ranges carry larger reduction obligations. The proposal contains a default option of $25mn in cases where a Member fails to notify to establish the baseline. It also provides for a flexibility for Members with a baseline below $25mn that could be uplifted by $5mn under certain considitions (timebound, MSY and capture limit).</t>
   </si>
   <si>
-    <t xml:space="preserve">1) We assume each Member's baseline to the total magnitude of capacity-enhancing subsidies estimated by Sumaila et al. 2019. 2) The formula ranges and percentages of reduction from the proposal are then applied to all Members. </t>
-  </si>
-  <si>
     <t>This proposal build on the Chair's text. Can it be model based on the Chair's text with the adjustments they propose that can be modeled, if any?</t>
   </si>
   <si>
@@ -1564,9 +1525,6 @@
     <t>This communication proposes a set of amendments to the Chair's text: 1) Article 1.2. Exclusion of artisanal and small scale fisheries from scope with transparency requirements. 2) Article 3.2.b. Determination of Flag states in the high seas. 3) Sustainability test of article 5.2 subject to all members approaval and for a 3 year period if members demostrate that stock is biologically sustainable. 4) Article 9. Revison of the agreement and termination of the agreement.</t>
   </si>
   <si>
-    <t>No special and diffrential treatment is considered</t>
-  </si>
-  <si>
     <t xml:space="preserve">This  proposal is focus on artisanal fisheries, with some socio economic conditions and spacial flexiblity. Can it be model or just model with certain limitations,? Can we moel just the impact of exclusing fishing in the 12 nm? Can we model the chair's text with the exclusion of 12nm? </t>
   </si>
   <si>
@@ -1588,9 +1546,6 @@
     <t>This proposal excludes subsidies to artisanal fisheries from the prohibition of Articles 4 and 5. The criteria to consider the exemption is low income, resource poor or livelihood fishing to ensure food security and limited to 12 nautical miles and applicable dometic legislation.</t>
   </si>
   <si>
-    <t>Blank entry for NEW Chair's text</t>
-  </si>
-  <si>
     <t>RD/TN/RL/W/276</t>
   </si>
   <si>
@@ -1601,20 +1556,6 @@
   </si>
   <si>
     <t>This communication was circulated at the request of the Chair of the Negotiating Group on Rules on May 11, 2021.</t>
-  </si>
-  <si>
-    <r>
-      <t>This communication aims to represent the progress made since the last consolidated text was released, and to provide some suggested compromises on remaining outstanding issues. As written, it still provides two possible ways of characterizing and determining what constitutes an overfished stock:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> i) those recognized as such by the Member under whose jurisdiction the fishing is taking place or by the relevant RFMO/A; ii) those for which the mortality from fishing needs to be restricted to allow the stock to rebuild to some reference point. Additionally, it includes a blank placeholder for inclusion of a cap-based proposal.</t>
-    </r>
   </si>
   <si>
     <t>TN/RL/W/276</t>
@@ -1723,12 +1664,6 @@
     <t>Fisheries Subsidies Text Proposal</t>
   </si>
   <si>
-    <t>Chair's text - Consolidated text (June 2020)</t>
-  </si>
-  <si>
-    <t>Draft consolidated text (June 2020)</t>
-  </si>
-  <si>
     <t xml:space="preserve">NOTE: Modeled using parameters of overfished stocks - assumed to have a similar biological interpretation as New Zealand/Iceland, but less ambitious because of S&amp;DT and subsistence fishing exemption. Transition period is not modeled. </t>
   </si>
   <si>
@@ -1830,18 +1765,12 @@
     <t>&lt;ol&gt;&lt;li&gt;We assume each Member's baseline to the total magnitude of capacity-enhancing subsidies estimated by Sumaila et al. 2019.&lt;/li&gt;&lt;li&gt;The formula ranges and percentages of reduction from the proposal are then applied to all Members.&lt;/li&gt;&lt;li&gt;The"uplift" allowance for Members demonstrating a need to develop capacity within their own EEZ cannot be modeled here.&lt;/li&gt;&lt;/ol&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">NEW (May 13, 2021) - pretty sure we can not model the S&amp;DT "uplift" criteria here. </t>
-  </si>
-  <si>
     <t>The ammendments proposed in this communication cannot be modeled in our current framework, but it is included here for reference.</t>
   </si>
   <si>
     <t xml:space="preserve">NEW (May 13, 2021) - included for reference now, not sure we can model it. </t>
   </si>
   <si>
-    <t>This data underlying this tool only includes vessels that transmit AIS, primarily vessels 24 meters in length or larger. This tool therefore doesn't capture the vast majority of small scale vessels as they don't usually have AIS. Tor this reason is difficult to simulate an exception to artisanal or small scale fisheries. However, the tool is able to model the impact of the fishing in the 12 nautical miles from all Members providing a proxy to what it would mean to exclude fishing in the 12 nautical miles from the prohibition.</t>
-  </si>
-  <si>
     <t xml:space="preserve">1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 0.8) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - this is the less ambitious interpretation of the two (see Overfished - Negative effects (Option A)). </t>
   </si>
   <si>
@@ -1851,9 +1780,6 @@
     <t>For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 0.8) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - this is the less ambitious interpretation of the two (see Overfished - Negative effects (Option A)).  For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: None.</t>
   </si>
   <si>
-    <t>&lt;ol&gt;&lt;li&gt;There is uncertainty regarding the status of many fish stocks.&lt;/li&gt;&lt;li&gt;For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited.&lt;/li&gt;&lt;li&gt;The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database.&lt;/li&gt;&lt;li&gt;The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text.&lt;/li&gt;&lt;li&gt;Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - this is the more ambitious interpretation of the two (see Overfished - Negative effects (Option A)).&lt;/li&gt;&lt;/ol&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 0.8) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - this is the less ambitious interpretation of the two (see Overfished - Negative effects (Option A)).  For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: 1) We assume each Member's cap is equal to whichever of the three proposed approaches for calculating a cap yields the largest amount. By default, caps based on the first approach are calculated as 55% of each Member's base for capping; caps based on the second approach are calculated as 2% of each Member's estimated landed value (calculated from the FAO Global Marine Capture Production Database, average between 2016-2018); caps based on the third approach are calculated as 55% of the global average subsidies per fisher (capacity-enhancing and ambiguous) multiplied by each Member's most recently reported total number of fishers (from the FAO Yearbook of Fishery and Aquaculture Statistics 2017). 2) We assume that provision of the following types of subsidies as defined by Sumaila et al. 2019 are allowed to continue irrespective of a Member's total cap: i) subsidies for fishing access agreements; ii) fisher assistance programs; iii) vessel buyback programs; iv) rural fishers' community development programs. Therefore each Member's base for capping is represented by the total amount of all other capacity-enhancing and ambiguous subsidies estimated by Sumaila et al. 2019. </t>
   </si>
   <si>
@@ -1872,9 +1798,6 @@
     <t xml:space="preserve">For IUU: Subsidies granted by developing and LDC Members shall be allowed for small scale fishing: a) for unreported and unregulated fishing: b) within their own territorial waters. Transition periods are also consider as an alternative but are not modeled here. For Overfished: Subsidies granted by developing and LDC Members for fishing within their own territorial sea shall be allowed. Transition periods are also consider as an alternative but are not modeled here. For OCOF: Subsidies granted by LDCs shall be allowed, and subsidies granted by developing countries shall be allowed for fishing in their territorial seas, or for fishing in their EEZs and high seas unless any of the following conditions are met for three consecutive years (2016-2018): a) GNI per capita is greater than US $5000 (constant 2010 US$), b) they engage in distant water fishing, or c) the contribution from Agriculture, Forestry and Fishing to their national GDP (World Bank) is greater than 10%. Transition periods are also considered as an alternative but are not modeled here. If transition periods are employed, LDCs would enjoy a transition period specifically for them. </t>
   </si>
   <si>
-    <t xml:space="preserve">NEW (May 13, 2021) - I think we just pick an Overfished definition and our broadest definition of OFOC and simulate the 12nm exception Need guidance on which Chair's text to apply it to. </t>
-  </si>
-  <si>
     <t>Missing - need to identify developing countries meeting non-industrial criteria. The three options associated with defining it could be calculated on the back-end.</t>
   </si>
   <si>
@@ -1924,6 +1847,138 @@
   </si>
   <si>
     <t>Blank entry for Chair's text. NOTE: As witten, this proposal places different prohibtions on boat building/fuel subsidies and all other subsidies. This is not accounted for (HS only vs. all)</t>
+  </si>
+  <si>
+    <t>This data underlying this tool only includes vessels that transmit AIS, primarily vessels 24 meters in length or larger. This tool therefore doesn't capture the vast majority of small scale vessels as they don't usually have AIS. Tor this reason is difficult to simulate an exception to artisanal or small scale fisheries. However, the tool is able to model the impact of the fishing in the 12 nautical miles from all Members providing a proxy to what it would mean to exclude fishing in the 12 nautical miles from the prohibition. For the purposes of modeling this exception, we use articles 3, 4, and 5 from the Chair's text - Consolidated text (June 2020). For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, coastal, and port Member states. 2) No publically available data exist for most flag and subsidizing Member, nor for coastal or port Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 1) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - this is the more ambitious interpretation of the two (see OFOC - Negative effects (Option A)). For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: None.</t>
+  </si>
+  <si>
+    <t>Subsidies granted by all Members shall be allowed for fishing within their own territorial waters.</t>
+  </si>
+  <si>
+    <t>Subsidies granted by LDCs shall be allowed, and subsidies granted by all other Members shall be allowed for fishing in their territorial seas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For IUU: Subsidies granted by developing and LDC Members shall be allowed for small scale fishing: a) for unreported and unregulated fishing: b) within their own territorial waters. Transition periods are also considered as an alternative but are not modeled here. For Overfished: Subsidies granted by all Members for fishing within their own territorial sea shall be allowed. Transition periods are also considered as an alternative but are not modeled here. For OCOF: Subsidies granted by LDCs shall be allowed, and subsidies granted by all other Members shall be allowed for fishing in their territorial seas. Transition periods are also considered as an alternative but are not modeled here. If transition periods were employed, we assume that LDCs would enjoy a transition period specifically for them. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added (May 25, 2021) - Does do something different for Overfished, but with the OFOC provisions from the old Chair's text, it doesn't do anything there. NEW (May 13, 2021). I think we just pick an Overfished definition and our broadest definition of OFOC and simulate the 12nm exception Need guidance on which Chair's text to apply it to. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not modeling. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) We assume each Member's baseline to the total magnitude of capacity-enhancing subsidies estimated by Sumaila et al. 2019. 2) The formula ranges and percentages of reduction from the proposal are then applied to all Members. 3) We cannot model whether a Member would demonstratedly need to develop capacity to fish in their own EEZ, and therefore which Members would be entitled to a "uplift". </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW (May 13, 2021) - pretty sure we can not model the S&amp;DT "uplift" criteria here. Made this clear in the text. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Original Brazil formula proposal. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev.1 of the Brazil formula proposal. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Applying the Ecuador et al. exemptions to old Chair's text. </t>
+  </si>
+  <si>
+    <t>Added (May 25, 2021)</t>
+  </si>
+  <si>
+    <t>NEW Chair's text</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;Final determinations are made by existing RFMO/A vessel lists, and by flag and coastal Member states.&lt;/li&gt;&lt;li&gt;No publically available data exist for most flag or coastal Members. The possible effects of modeling this proposal is therefore a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about the expected IUU-findings.&lt;/li&gt;&lt;li&gt;No proportionality or the duration of prohibition is considered.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subsidies granted by developing and LDC Members shall be allowed for small scale fishing within their own territorial waters. As written, this exception might only apply for a transition period of 2 years, but for the purposes of modeling we assume it to apply indefinitely. </t>
+  </si>
+  <si>
+    <t>IUU1, IUU2, IUU3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This communication aims to represent the progress made since the last consolidated text was released, and to provide some suggested compromises on remaining outstanding issues. As written, it still provides two possible options for S&amp;DT for Article 5 prohibitions. For the purposes of modeling here, we use ALT 1.  </t>
+  </si>
+  <si>
+    <t>For IUU: Subsidies granted by developing and LDC Members shall be allowed for small scale fishing within their own territorial waters. Such an exemption might only apply for a transition period of 2 years, but we model it as if such an exemption would continue indefinitely. For Overfished: Subsidies granted by developing and LDC Members shall be allowed for small scale fishing within their own territorial waters. Such an exemption might only apply for a transition period of 2 years, but we model it as if such an exemption would continue indefinitely. For OCOF: Subsidies granted by LDCs shall be allowed, and subsidies granted by developing countries shall be allowed for fishing in their territorial seas, or for fishing in their EEZs and high seas unless any of the following conditions are met for three consecutive years (2016-2018): a) GNI per capita is greater than US $5000 (constant 2010 US$), b) they engage in distant water fishing, or c) the contribution from Agriculture, Forestry and Fishing to their national GDP (World Bank) is greater than 10%. Transition periods are also considered as an alternative but are not modeled here. If transition periods are employed, LDCs would enjoy a transition period specifically for them.</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126/Rev.2</t>
+  </si>
+  <si>
+    <t>Chair's text - Consolidated text (Dec 2020)</t>
+  </si>
+  <si>
+    <t>Draft consolidated text (Dec 2020)</t>
+  </si>
+  <si>
+    <t>This communication was circulated at the request of the Chair of the Negotiating Group on Rules on December 18, 2020.</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126/Rev.2 | Objective Definition</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126/Rev.2 | Relevant Authorities</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126/Rev.2 | TN/RL/GEN/199 | Objective Definition</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126/Rev.2 | TN/RL/GEN/199 | Relevant Authorities</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126/Rev.2 | TN/RL/GEN/197/Rev.2 | Objective Definition</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126/Rev.2 | TN/RL/GEN/197/Rev.2 | Relevant Authorities</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126/Rev.2 | RD/TN/RL/81 | Objective Definition</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126/Rev.2 | RD/TN/RL/81 | Relevant Authorities</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126/Rev.2 | RD/TN/RL/124 | Objective Definition</t>
+  </si>
+  <si>
+    <t>RD/TN/RL/126/Rev.2 | RD/TN/RL/124 | Relevant Authorities</t>
+  </si>
+  <si>
+    <t>NEW Chair's text - sustainability criteria</t>
+  </si>
+  <si>
+    <t>Chair's text - Consolidated text (May 2021) - Sustainability scenario</t>
+  </si>
+  <si>
+    <t>Scenario based on Chair's text showing the hightes sustainability outcome</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;Final determinations are made by existing RFMO/A vessel lists, and by flag and coastal Member states.&lt;/li&gt;&lt;li&gt;No publically available data exist for most flag or coastal Members, so we assume 20% of fishing effort worldwide to be identified as IUU&lt;/li&gt;&lt;li&gt;No proportionality or the duration of prohibition is considered.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;There is uncertainty regarding the status of many fish stocks.&lt;/li&gt;&lt;li&gt;For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 0.8) in the RAM Legacy Stock Assessment Database are prohibited.&lt;/li&gt;&lt;li&gt;The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database.&lt;/li&gt;&lt;li&gt;The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text.&lt;/li&gt;&lt;li&gt;Additionally, as written, this text includes two alternative definitions used to identify an overfished stock - this is the less ambitious interpretation of the two (see Overfished - Negative effects (Option A)).&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;There is uncertainty regarding the status of many fish stocks.&lt;/li&gt;&lt;li&gt;For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 0.8) in the RAM Legacy Stock Assessment Database are prohibited.&lt;/li&gt;&lt;li&gt;The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database.&lt;/li&gt;&lt;li&gt;The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text.&lt;/li&gt;&lt;li&gt;The definition for an overfished stock subsidy prohibition considered here is the less ambitious interpretation considered in the previous version of the text (see Overfished - Negative effects (Option A)).&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction.&lt;/li&gt;&lt;li&gt;We note that this is a conservative interpretation of this proposal, as the text prohibits these types of subsidies for all fishing unless a Member can demonstrate that measures are implemented to maintain stocks at a biologically sustainable level. However, it is unclear how many Members would be able to satisfy this sustainability criteria, and thus we assume that such an exemption could be aquired by all Members.&lt;/li&gt;&lt;li&gt;By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited.&lt;/li&gt;&lt;li&gt;We note that this is an ambitious interpretation of this proposal, as the text provides an exemption if a Member can demonstrate that measures are implemented to maintain stocks at a biologically sustainable level. However, it is unclear how many Members would be able to satisfy this sustainability criteria.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, and by flag and coastal Member states. 2) No publically available data exist for most flag Members, nor for coastal Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 0.8) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) The definition for an overfished stock subsidy prohibition considered here is the less ambitious interpretation considered in the previous version of the text. For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: None.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For IUU: No flexibilities for developing countries. For Overfished: no flexibilities for developing countries. For OCOF: Transition period for subsidies granted by LDCs, and subsidies granted by developing countries shall be allowed a transition period of 2 years. No flexibility for fishing in their EEZs and RFMO/A.  An entension of the transition periods are possible for countries under 0.7% of FAO marine capture data and subsidies do not exceed USD25 million, subject to review and examination by the WTO Members. Extensions are granted every year and after the last extension is granted the Member will have 2 years to phase out the programs. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, and by flag and coastal states. 2) No publicly available data exist for most flag and coastal Members, therefore to model the potential impacts we assume 20% of the fishing effort worldwide to be identifiable as IUU. 3) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks id+S46entified as overfished (B/Bmsy &lt; 0.8) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) The definition for an overfished stock subsidy prohibition is the less ambitious interpretation considered in the previous version of the text. For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited. 2) We note that this is an ambitious interpretation of this proposal as no sustainability test is considered. </t>
+  </si>
+  <si>
+    <t>TN/RL/W/276 | Sustainability scenario</t>
   </si>
 </sst>
 </file>
@@ -2479,7 +2534,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2608,6 +2663,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2965,10 +3023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DC43"/>
+  <dimension ref="A1:DC44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
@@ -3012,7 +3070,7 @@
         <v>88</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>314</v>
@@ -3039,7 +3097,7 @@
         <v>125</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>479</v>
+        <v>467</v>
       </c>
       <c r="M1" s="9" t="s">
         <v>246</v>
@@ -3060,25 +3118,25 @@
         <v>245</v>
       </c>
       <c r="S1" s="33" t="s">
+        <v>427</v>
+      </c>
+      <c r="T1" s="33" t="s">
+        <v>437</v>
+      </c>
+      <c r="U1" s="33" t="s">
+        <v>428</v>
+      </c>
+      <c r="V1" s="33" t="s">
         <v>439</v>
       </c>
-      <c r="T1" s="33" t="s">
-        <v>449</v>
-      </c>
-      <c r="U1" s="33" t="s">
-        <v>440</v>
-      </c>
-      <c r="V1" s="33" t="s">
-        <v>451</v>
-      </c>
       <c r="W1" s="33" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="X1" s="33" t="s">
-        <v>453</v>
+        <v>441</v>
       </c>
       <c r="Y1" s="33" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="Z1" s="8" t="s">
         <v>7</v>
@@ -3282,13 +3340,13 @@
         <v>45</v>
       </c>
       <c r="CO1" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="CP1" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="CP1" s="8" t="s">
+      <c r="CQ1" s="8" t="s">
         <v>363</v>
-      </c>
-      <c r="CQ1" s="8" t="s">
-        <v>364</v>
       </c>
       <c r="CR1" s="8" t="s">
         <v>46</v>
@@ -3300,13 +3358,13 @@
         <v>49</v>
       </c>
       <c r="CU1" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="CV1" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="CV1" s="8" t="s">
+      <c r="CW1" s="8" t="s">
         <v>366</v>
-      </c>
-      <c r="CW1" s="8" t="s">
-        <v>367</v>
       </c>
       <c r="CX1" s="8" t="s">
         <v>50</v>
@@ -3318,13 +3376,13 @@
         <v>53</v>
       </c>
       <c r="DA1" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="DB1" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="DB1" s="8" t="s">
+      <c r="DC1" s="8" t="s">
         <v>369</v>
-      </c>
-      <c r="DC1" s="8" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="2" spans="1:107" s="8" customFormat="1" ht="282" customHeight="1">
@@ -3335,16 +3393,16 @@
         <v>98</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>601</v>
+        <v>579</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>58</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>99</v>
@@ -3365,10 +3423,10 @@
         <v>320</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>480</v>
+        <v>468</v>
       </c>
       <c r="N2" s="39" t="s">
-        <v>533</v>
+        <v>517</v>
       </c>
       <c r="O2" s="15" t="s">
         <v>142</v>
@@ -3380,28 +3438,28 @@
         <v>317</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="S2" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="T2" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="U2" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="V2" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="W2" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="X2" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="Y2" s="34" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
       <c r="Z2" s="15"/>
       <c r="AA2" s="15"/>
@@ -3471,18 +3529,18 @@
         <v>295</v>
       </c>
       <c r="CG2" s="15" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="CH2" s="15" t="s">
         <v>289</v>
       </c>
       <c r="CI2" s="15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="CJ2" s="15"/>
       <c r="CK2" s="15"/>
       <c r="CL2" s="29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="CM2" s="15"/>
       <c r="CN2" s="27">
@@ -3492,7 +3550,7 @@
       <c r="CP2" s="27"/>
       <c r="CQ2" s="27"/>
       <c r="CR2" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="CT2" s="15">
         <v>20</v>
@@ -3501,7 +3559,7 @@
       <c r="CV2" s="27"/>
       <c r="CW2" s="27"/>
       <c r="CX2" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="CY2" s="15"/>
       <c r="CZ2" s="15">
@@ -3519,10 +3577,10 @@
         <v>98</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>530</v>
+        <v>514</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>58</v>
@@ -3549,10 +3607,10 @@
         <v>301</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>481</v>
+        <v>469</v>
       </c>
       <c r="N3" s="39" t="s">
-        <v>532</v>
+        <v>516</v>
       </c>
       <c r="O3" s="15" t="s">
         <v>110</v>
@@ -3564,25 +3622,25 @@
         <v>317</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>534</v>
+        <v>518</v>
       </c>
       <c r="S3" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="T3" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="U3" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="V3" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="W3" s="34" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
       <c r="X3" s="34" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="Y3" s="34" t="s">
         <v>55</v>
@@ -3614,10 +3672,10 @@
         <v>98</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>600</v>
+        <v>578</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>536</v>
+        <v>520</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>58</v>
@@ -3639,7 +3697,7 @@
         <v>299</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>482</v>
+        <v>470</v>
       </c>
       <c r="N4" s="15" t="s">
         <v>78</v>
@@ -3651,31 +3709,31 @@
         <v>318</v>
       </c>
       <c r="Q4" s="40" t="s">
-        <v>535</v>
+        <v>519</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="S4" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="T4" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="U4" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="V4" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="W4" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="X4" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="Y4" s="34" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
       <c r="AF4" s="15" t="s">
         <v>288</v>
@@ -3690,13 +3748,13 @@
         <v>295</v>
       </c>
       <c r="CG4" s="15" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="CH4" s="15" t="s">
         <v>305</v>
       </c>
       <c r="CL4" s="15" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="CO4" s="27">
         <v>55</v>
@@ -3716,7 +3774,7 @@
         <v>121</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>529</v>
+        <v>513</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>58</v>
@@ -3725,7 +3783,7 @@
         <v>128</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>531</v>
+        <v>515</v>
       </c>
       <c r="I5" s="15" t="s">
         <v>55</v>
@@ -3740,10 +3798,10 @@
         <v>233</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>541</v>
+        <v>525</v>
       </c>
       <c r="N5" s="15" t="s">
-        <v>540</v>
+        <v>524</v>
       </c>
       <c r="O5" s="15" t="s">
         <v>130</v>
@@ -3755,25 +3813,25 @@
         <v>317</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
       <c r="S5" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="T5" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="U5" s="34" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="V5" s="34" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="W5" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="X5" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="Y5" s="34" t="s">
         <v>55</v>
@@ -3805,7 +3863,7 @@
         <v>90</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>528</v>
+        <v>512</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>58</v>
@@ -3826,7 +3884,7 @@
         <v>229</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>542</v>
+        <v>526</v>
       </c>
       <c r="N6" s="15" t="s">
         <v>139</v>
@@ -3841,25 +3899,25 @@
         <v>317</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
       <c r="S6" s="34" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
       <c r="T6" s="34" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="U6" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="V6" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="W6" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="X6" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="Y6" s="34" t="s">
         <v>55</v>
@@ -3894,7 +3952,7 @@
         <v>98</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>527</v>
+        <v>511</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>58</v>
@@ -3915,7 +3973,7 @@
         <v>230</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>483</v>
+        <v>471</v>
       </c>
       <c r="N7" s="15" t="s">
         <v>103</v>
@@ -3930,25 +3988,25 @@
         <v>317</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="S7" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="T7" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="U7" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="V7" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="W7" s="34" t="s">
-        <v>448</v>
+        <v>436</v>
       </c>
       <c r="X7" s="34" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="Y7" s="34" t="s">
         <v>55</v>
@@ -3960,7 +4018,7 @@
         <v>288</v>
       </c>
       <c r="BK7" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="BL7" s="15" t="s">
         <v>347</v>
@@ -3987,13 +4045,13 @@
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="37" t="s">
-        <v>567</v>
+        <v>549</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>58</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="H8" s="15" t="s">
         <v>341</v>
@@ -4011,7 +4069,7 @@
         <v>302</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>484</v>
+        <v>472</v>
       </c>
       <c r="N8" s="15" t="s">
         <v>113</v>
@@ -4020,31 +4078,31 @@
         <v>114</v>
       </c>
       <c r="P8" s="15" t="s">
-        <v>537</v>
+        <v>521</v>
       </c>
       <c r="Q8" s="41" t="s">
-        <v>526</v>
+        <v>510</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
       <c r="S8" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="T8" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="U8" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="V8" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="W8" s="34" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
       <c r="X8" s="34" t="s">
-        <v>526</v>
+        <v>510</v>
       </c>
       <c r="Y8" s="34" t="s">
         <v>55</v>
@@ -4091,7 +4149,7 @@
         <v>121</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>602</v>
+        <v>580</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>58</v>
@@ -4115,7 +4173,7 @@
         <v>232</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>485</v>
+        <v>473</v>
       </c>
       <c r="N9" s="15" t="s">
         <v>127</v>
@@ -4127,28 +4185,28 @@
         <v>328</v>
       </c>
       <c r="Q9" s="40" t="s">
-        <v>539</v>
+        <v>523</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="S9" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="T9" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="U9" s="34" t="s">
-        <v>455</v>
+        <v>443</v>
       </c>
       <c r="V9" s="34" t="s">
-        <v>565</v>
+        <v>547</v>
       </c>
       <c r="W9" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="X9" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="Y9" s="34" t="s">
         <v>55</v>
@@ -4183,7 +4241,7 @@
         <v>98</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>603</v>
+        <v>581</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>58</v>
@@ -4192,7 +4250,7 @@
         <v>68</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>538</v>
+        <v>522</v>
       </c>
       <c r="I10" s="14" t="s">
         <v>58</v>
@@ -4207,7 +4265,7 @@
         <v>319</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>486</v>
+        <v>474</v>
       </c>
       <c r="N10" s="15" t="s">
         <v>70</v>
@@ -4216,34 +4274,34 @@
         <v>124</v>
       </c>
       <c r="P10" s="15" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="Q10" s="20" t="s">
         <v>317</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
       <c r="S10" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="T10" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="U10" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="V10" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="W10" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="X10" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="Y10" s="34" t="s">
-        <v>456</v>
+        <v>444</v>
       </c>
       <c r="AF10" s="15" t="s">
         <v>288</v>
@@ -4258,7 +4316,7 @@
         <v>295</v>
       </c>
       <c r="CG10" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="CH10" s="15" t="s">
         <v>289</v>
@@ -4293,7 +4351,7 @@
         <v>98</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>604</v>
+        <v>582</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>58</v>
@@ -4317,7 +4375,7 @@
         <v>300</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>487</v>
+        <v>475</v>
       </c>
       <c r="N11" s="15" t="s">
         <v>111</v>
@@ -4332,25 +4390,25 @@
         <v>317</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="S11" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="T11" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="U11" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="V11" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="W11" s="34" t="s">
-        <v>457</v>
+        <v>445</v>
       </c>
       <c r="X11" s="34" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="Y11" s="34" t="s">
         <v>55</v>
@@ -4362,7 +4420,7 @@
         <v>288</v>
       </c>
       <c r="BK11" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="BL11" s="15" t="s">
         <v>347</v>
@@ -4394,7 +4452,7 @@
         <v>90</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>528</v>
+        <v>512</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>58</v>
@@ -4415,7 +4473,7 @@
         <v>297</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>543</v>
+        <v>527</v>
       </c>
       <c r="N12" s="15" t="s">
         <v>94</v>
@@ -4430,25 +4488,25 @@
         <v>317</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="S12" s="34" t="s">
-        <v>458</v>
+        <v>446</v>
       </c>
       <c r="T12" s="34" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="U12" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="V12" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="W12" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="X12" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="Y12" s="34" t="s">
         <v>55</v>
@@ -4489,7 +4547,7 @@
         <v>85</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>551</v>
+        <v>533</v>
       </c>
       <c r="I13" s="14" t="s">
         <v>58</v>
@@ -4504,7 +4562,7 @@
         <v>338</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>488</v>
+        <v>476</v>
       </c>
       <c r="N13" s="15" t="s">
         <v>86</v>
@@ -4519,25 +4577,25 @@
         <v>317</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="S13" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="T13" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="U13" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="V13" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="W13" s="34" t="s">
-        <v>478</v>
+        <v>466</v>
       </c>
       <c r="X13" s="34" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="Y13" s="34" t="s">
         <v>55</v>
@@ -4549,7 +4607,7 @@
         <v>288</v>
       </c>
       <c r="BK13" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="BL13" s="15" t="s">
         <v>347</v>
@@ -4572,10 +4630,10 @@
         <v>98</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>548</v>
+        <v>530</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>559</v>
+        <v>541</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>58</v>
@@ -4596,43 +4654,43 @@
         <v>43775</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="M14" s="17" t="s">
-        <v>489</v>
+        <v>477</v>
       </c>
       <c r="N14" s="15" t="s">
         <v>116</v>
       </c>
       <c r="O14" s="15" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="P14" s="15" t="s">
         <v>330</v>
       </c>
       <c r="Q14" s="41" t="s">
-        <v>563</v>
+        <v>545</v>
       </c>
       <c r="R14" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="S14" s="34" t="s">
+        <v>459</v>
+      </c>
+      <c r="T14" s="34" t="s">
+        <v>438</v>
+      </c>
+      <c r="U14" s="34" t="s">
+        <v>459</v>
+      </c>
+      <c r="V14" s="34" t="s">
+        <v>438</v>
+      </c>
+      <c r="W14" s="34" t="s">
+        <v>447</v>
+      </c>
+      <c r="X14" s="34" t="s">
         <v>550</v>
-      </c>
-      <c r="S14" s="34" t="s">
-        <v>471</v>
-      </c>
-      <c r="T14" s="34" t="s">
-        <v>450</v>
-      </c>
-      <c r="U14" s="34" t="s">
-        <v>471</v>
-      </c>
-      <c r="V14" s="34" t="s">
-        <v>450</v>
-      </c>
-      <c r="W14" s="34" t="s">
-        <v>459</v>
-      </c>
-      <c r="X14" s="34" t="s">
-        <v>568</v>
       </c>
       <c r="Y14" s="34" t="s">
         <v>55</v>
@@ -4688,10 +4746,10 @@
         <v>90</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>549</v>
+        <v>531</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>605</v>
+        <v>583</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>58</v>
@@ -4700,7 +4758,7 @@
         <v>91</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>552</v>
+        <v>534</v>
       </c>
       <c r="I15" s="15" t="s">
         <v>55</v>
@@ -4712,10 +4770,10 @@
         <v>43801</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="M15" s="17" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="N15" s="15" t="s">
         <v>315</v>
@@ -4724,31 +4782,31 @@
         <v>92</v>
       </c>
       <c r="P15" s="15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="Q15" s="40" t="s">
-        <v>564</v>
+        <v>546</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="S15" s="34" t="s">
-        <v>460</v>
+        <v>448</v>
       </c>
       <c r="T15" s="34" t="s">
-        <v>569</v>
+        <v>551</v>
       </c>
       <c r="U15" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="V15" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="W15" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="X15" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="Y15" s="34" t="s">
         <v>55</v>
@@ -4808,7 +4866,7 @@
         <v>343</v>
       </c>
       <c r="M16" s="17" t="s">
-        <v>490</v>
+        <v>478</v>
       </c>
       <c r="N16" s="15" t="s">
         <v>143</v>
@@ -4817,20 +4875,20 @@
         <v>144</v>
       </c>
       <c r="P16" s="15" t="s">
-        <v>467</v>
+        <v>455</v>
       </c>
       <c r="Q16" s="18"/>
       <c r="R16" s="4" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="S16" s="34" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="U16" s="34" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="W16" s="34" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
     </row>
     <row r="17" spans="1:107" ht="112">
@@ -4864,7 +4922,7 @@
         <v>344</v>
       </c>
       <c r="M17" s="17" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="N17" s="15" t="s">
         <v>119</v>
@@ -4873,20 +4931,20 @@
         <v>120</v>
       </c>
       <c r="P17" s="15" t="s">
-        <v>468</v>
+        <v>456</v>
       </c>
       <c r="Q17" s="18"/>
       <c r="R17" s="4" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="S17" s="34" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="U17" s="34" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="W17" s="34" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
     </row>
     <row r="18" spans="1:107" ht="84">
@@ -4928,20 +4986,20 @@
         <v>133</v>
       </c>
       <c r="P18" s="15" t="s">
-        <v>469</v>
+        <v>457</v>
       </c>
       <c r="Q18" s="18"/>
       <c r="R18" s="4" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="S18" s="34" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="U18" s="34" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="W18" s="34" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
     </row>
     <row r="19" spans="1:107" ht="224">
@@ -4952,16 +5010,16 @@
         <v>121</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>597</v>
+        <v>575</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>58</v>
       </c>
       <c r="G19" s="39" t="s">
-        <v>553</v>
+        <v>535</v>
       </c>
       <c r="I19" s="15" t="s">
         <v>55</v>
@@ -4985,26 +5043,26 @@
         <v>123</v>
       </c>
       <c r="P19" s="15" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="Q19" s="18"/>
       <c r="R19" s="4"/>
     </row>
     <row r="20" spans="1:107" ht="224">
       <c r="A20" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>121</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>58</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>598</v>
+        <v>576</v>
       </c>
       <c r="I20" s="15" t="s">
         <v>55</v>
@@ -5028,31 +5086,31 @@
         <v>123</v>
       </c>
       <c r="P20" s="15" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="Q20" s="20" t="s">
         <v>317</v>
       </c>
       <c r="R20" s="4" t="s">
-        <v>596</v>
+        <v>574</v>
       </c>
       <c r="S20" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="T20" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="U20" s="34" t="s">
-        <v>554</v>
+        <v>536</v>
       </c>
       <c r="V20" s="34" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="W20" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="X20" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="Y20" s="34" t="s">
         <v>55</v>
@@ -5078,19 +5136,19 @@
     </row>
     <row r="21" spans="1:107" ht="224">
       <c r="A21" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>121</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>58</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>599</v>
+        <v>577</v>
       </c>
       <c r="I21" s="15" t="s">
         <v>55</v>
@@ -5114,31 +5172,31 @@
         <v>123</v>
       </c>
       <c r="P21" s="15" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="Q21" s="20" t="s">
         <v>317</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>579</v>
+        <v>559</v>
       </c>
       <c r="S21" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="T21" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="U21" s="34" t="s">
-        <v>580</v>
+        <v>560</v>
       </c>
       <c r="V21" s="34" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="W21" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="X21" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="Y21" s="34" t="s">
         <v>55</v>
@@ -5170,7 +5228,7 @@
         <v>98</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>58</v>
@@ -5194,7 +5252,7 @@
         <v>235</v>
       </c>
       <c r="M22" s="17" t="s">
-        <v>492</v>
+        <v>480</v>
       </c>
       <c r="N22" s="15" t="s">
         <v>236</v>
@@ -5209,25 +5267,25 @@
         <v>317</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="S22" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="T22" s="34" t="s">
+        <v>438</v>
+      </c>
+      <c r="U22" s="34" t="s">
+        <v>449</v>
+      </c>
+      <c r="V22" s="34" t="s">
+        <v>440</v>
+      </c>
+      <c r="W22" s="34" t="s">
         <v>450</v>
       </c>
-      <c r="U22" s="34" t="s">
-        <v>461</v>
-      </c>
-      <c r="V22" s="34" t="s">
-        <v>452</v>
-      </c>
-      <c r="W22" s="34" t="s">
-        <v>462</v>
-      </c>
       <c r="X22" s="34" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="Y22" s="34" t="s">
         <v>55</v>
@@ -5245,7 +5303,7 @@
         <v>288</v>
       </c>
       <c r="BK22" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="BL22" s="15" t="s">
         <v>347</v>
@@ -5271,10 +5329,10 @@
         <v>90</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>595</v>
+        <v>573</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>58</v>
@@ -5283,10 +5341,10 @@
         <v>309</v>
       </c>
       <c r="G23" s="15" t="s">
+        <v>357</v>
+      </c>
+      <c r="H23" s="15" t="s">
         <v>358</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>359</v>
       </c>
       <c r="I23" s="15" t="s">
         <v>55</v>
@@ -5301,7 +5359,7 @@
         <v>228</v>
       </c>
       <c r="M23" s="17" t="s">
-        <v>544</v>
+        <v>528</v>
       </c>
       <c r="N23" s="15" t="s">
         <v>137</v>
@@ -5310,31 +5368,31 @@
         <v>332</v>
       </c>
       <c r="P23" s="39" t="s">
-        <v>560</v>
+        <v>542</v>
       </c>
       <c r="Q23" s="18" t="s">
-        <v>562</v>
+        <v>544</v>
       </c>
       <c r="R23" s="4" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="S23" s="34" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
       <c r="T23" s="34" t="s">
-        <v>568</v>
+        <v>550</v>
       </c>
       <c r="U23" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="V23" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="W23" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="X23" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="Y23" s="34" t="s">
         <v>55</v>
@@ -5396,10 +5454,10 @@
         <v>98</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>593</v>
+        <v>571</v>
       </c>
       <c r="D24" s="37" t="s">
-        <v>594</v>
+        <v>572</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>58</v>
@@ -5408,7 +5466,7 @@
         <v>231</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="I24" s="15" t="s">
         <v>55</v>
@@ -5423,7 +5481,7 @@
         <v>303</v>
       </c>
       <c r="M24" s="17" t="s">
-        <v>493</v>
+        <v>481</v>
       </c>
       <c r="N24" s="15" t="s">
         <v>113</v>
@@ -5435,28 +5493,28 @@
         <v>333</v>
       </c>
       <c r="Q24" s="18" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="R24" s="4" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="S24" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="T24" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="U24" s="34" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="V24" s="34" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="W24" s="34" t="s">
-        <v>464</v>
+        <v>452</v>
       </c>
       <c r="X24" s="34" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="Y24" s="34" t="s">
         <v>55</v>
@@ -5500,7 +5558,7 @@
         <v>89</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>591</v>
+        <v>569</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22" t="s">
@@ -5526,10 +5584,10 @@
         <v>298</v>
       </c>
       <c r="M25" s="9" t="s">
-        <v>494</v>
+        <v>482</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>545</v>
+        <v>529</v>
       </c>
       <c r="O25" s="8" t="s">
         <v>334</v>
@@ -5538,28 +5596,28 @@
         <v>336</v>
       </c>
       <c r="Q25" s="24" t="s">
-        <v>566</v>
+        <v>548</v>
       </c>
       <c r="R25" s="25" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
       <c r="S25" s="35" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
       <c r="T25" s="35" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="U25" s="35" t="s">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="V25" s="35" t="s">
-        <v>570</v>
+        <v>552</v>
       </c>
       <c r="W25" s="35" t="s">
-        <v>465</v>
+        <v>453</v>
       </c>
       <c r="X25" s="35" t="s">
-        <v>571</v>
+        <v>553</v>
       </c>
       <c r="Y25" s="35" t="s">
         <v>55</v>
@@ -5632,13 +5690,13 @@
       <c r="BI25" s="8"/>
       <c r="BJ25" s="8"/>
       <c r="BK25" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="BL25" s="8" t="s">
         <v>347</v>
       </c>
       <c r="BM25" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="BN25" s="8"/>
       <c r="BO25" s="8"/>
@@ -5711,10 +5769,10 @@
         <v>89</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>592</v>
+        <v>570</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>590</v>
+        <v>568</v>
       </c>
       <c r="E26" s="14" t="s">
         <v>58</v>
@@ -5736,7 +5794,7 @@
         <v>244</v>
       </c>
       <c r="M26" s="17" t="s">
-        <v>495</v>
+        <v>483</v>
       </c>
       <c r="N26" s="15" t="s">
         <v>135</v>
@@ -5745,31 +5803,31 @@
         <v>335</v>
       </c>
       <c r="P26" s="15" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="Q26" s="3" t="s">
-        <v>572</v>
+        <v>554</v>
       </c>
       <c r="R26" s="4" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="S26" s="34" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
       <c r="T26" s="34" t="s">
-        <v>568</v>
+        <v>550</v>
       </c>
       <c r="U26" s="35" t="s">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="V26" s="34" t="s">
-        <v>568</v>
+        <v>550</v>
       </c>
       <c r="W26" s="35" t="s">
-        <v>465</v>
+        <v>453</v>
       </c>
       <c r="X26" s="34" t="s">
-        <v>466</v>
+        <v>454</v>
       </c>
       <c r="Y26" s="34" t="s">
         <v>55</v>
@@ -5820,25 +5878,25 @@
         <v>295</v>
       </c>
       <c r="AZ26" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BC26" s="15" t="s">
         <v>295</v>
       </c>
       <c r="BD26" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BG26" s="15" t="s">
         <v>288</v>
       </c>
       <c r="BK26" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="BL26" s="8" t="s">
         <v>347</v>
       </c>
       <c r="BM26" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="BP26" s="8">
         <v>24</v>
@@ -5859,7 +5917,7 @@
         <v>295</v>
       </c>
       <c r="BY26" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="CB26" s="15" t="s">
         <v>288</v>
@@ -5876,20 +5934,20 @@
         <v>89</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>606</v>
+        <v>584</v>
       </c>
       <c r="D27" s="42" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="E27" s="14" t="s">
         <v>58</v>
       </c>
       <c r="F27" s="19"/>
       <c r="G27" s="14" t="s">
-        <v>415</v>
+        <v>603</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I27" s="14" t="s">
         <v>55</v>
@@ -5898,22 +5956,22 @@
         <v>351</v>
       </c>
       <c r="K27" s="16">
-        <v>44007</v>
+        <v>44183</v>
       </c>
       <c r="L27" s="17" t="s">
         <v>352</v>
       </c>
       <c r="M27" s="17" t="s">
-        <v>546</v>
+        <v>604</v>
       </c>
       <c r="N27" s="15" t="s">
-        <v>547</v>
+        <v>605</v>
       </c>
       <c r="O27" s="15" t="s">
-        <v>353</v>
+        <v>606</v>
       </c>
       <c r="P27" s="15" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="Q27" s="3"/>
       <c r="R27" s="4"/>
@@ -5930,26 +5988,26 @@
     </row>
     <row r="28" spans="1:107" ht="407" customHeight="1">
       <c r="A28" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="D28" s="42" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>58</v>
       </c>
       <c r="F28" s="19"/>
       <c r="G28" s="14" t="s">
-        <v>413</v>
+        <v>607</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I28" s="14" t="s">
         <v>55</v>
@@ -5958,52 +6016,52 @@
         <v>351</v>
       </c>
       <c r="K28" s="16">
-        <v>44007</v>
+        <v>44183</v>
       </c>
       <c r="L28" s="17" t="s">
         <v>352</v>
       </c>
       <c r="M28" s="17" t="s">
-        <v>546</v>
+        <v>604</v>
       </c>
       <c r="N28" s="15" t="s">
-        <v>547</v>
+        <v>605</v>
       </c>
       <c r="O28" s="15" t="s">
+        <v>606</v>
+      </c>
+      <c r="P28" s="15" t="s">
+        <v>566</v>
+      </c>
+      <c r="Q28" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="R28" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="S28" s="34" t="s">
+        <v>460</v>
+      </c>
+      <c r="T28" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="U28" s="34" t="s">
+        <v>536</v>
+      </c>
+      <c r="V28" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="W28" s="34" t="s">
+        <v>464</v>
+      </c>
+      <c r="X28" s="34" t="s">
+        <v>465</v>
+      </c>
+      <c r="Y28" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z28" s="15" t="s">
         <v>353</v>
-      </c>
-      <c r="P28" s="15" t="s">
-        <v>587</v>
-      </c>
-      <c r="Q28" s="18" t="s">
-        <v>588</v>
-      </c>
-      <c r="R28" s="4" t="s">
-        <v>555</v>
-      </c>
-      <c r="S28" s="34" t="s">
-        <v>472</v>
-      </c>
-      <c r="T28" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="U28" s="34" t="s">
-        <v>554</v>
-      </c>
-      <c r="V28" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="W28" s="34" t="s">
-        <v>476</v>
-      </c>
-      <c r="X28" s="34" t="s">
-        <v>477</v>
-      </c>
-      <c r="Y28" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z28" s="15" t="s">
-        <v>354</v>
       </c>
       <c r="AA28" s="15" t="s">
         <v>288</v>
@@ -6018,13 +6076,13 @@
         <v>295</v>
       </c>
       <c r="AH28" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AJ28" s="15" t="s">
         <v>295</v>
       </c>
       <c r="AK28" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AM28" s="15" t="s">
         <v>288</v>
@@ -6045,19 +6103,19 @@
         <v>295</v>
       </c>
       <c r="AZ28" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BC28" s="15" t="s">
         <v>295</v>
       </c>
       <c r="BD28" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BG28" s="15" t="s">
         <v>288</v>
       </c>
       <c r="BK28" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="BL28" s="15" t="s">
         <v>347</v>
@@ -6081,7 +6139,7 @@
         <v>295</v>
       </c>
       <c r="BY28" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="CB28" s="15" t="s">
         <v>288</v>
@@ -6092,26 +6150,26 @@
     </row>
     <row r="29" spans="1:107" ht="407" customHeight="1">
       <c r="A29" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="D29" s="42" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>58</v>
       </c>
       <c r="F29" s="19"/>
       <c r="G29" s="14" t="s">
-        <v>414</v>
+        <v>608</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I29" s="14" t="s">
         <v>55</v>
@@ -6120,52 +6178,52 @@
         <v>351</v>
       </c>
       <c r="K29" s="16">
-        <v>44007</v>
+        <v>44183</v>
       </c>
       <c r="L29" s="17" t="s">
         <v>352</v>
       </c>
       <c r="M29" s="17" t="s">
-        <v>546</v>
+        <v>604</v>
       </c>
       <c r="N29" s="15" t="s">
-        <v>547</v>
+        <v>605</v>
       </c>
       <c r="O29" s="15" t="s">
+        <v>606</v>
+      </c>
+      <c r="P29" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q29" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="R29" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="S29" s="34" t="s">
+        <v>460</v>
+      </c>
+      <c r="T29" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="U29" s="34" t="s">
+        <v>621</v>
+      </c>
+      <c r="V29" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="W29" s="34" t="s">
+        <v>464</v>
+      </c>
+      <c r="X29" s="34" t="s">
+        <v>465</v>
+      </c>
+      <c r="Y29" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z29" s="15" t="s">
         <v>353</v>
-      </c>
-      <c r="P29" s="15" t="s">
-        <v>435</v>
-      </c>
-      <c r="Q29" s="18" t="s">
-        <v>588</v>
-      </c>
-      <c r="R29" s="4" t="s">
-        <v>581</v>
-      </c>
-      <c r="S29" s="34" t="s">
-        <v>472</v>
-      </c>
-      <c r="T29" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="U29" s="34" t="s">
-        <v>582</v>
-      </c>
-      <c r="V29" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="W29" s="34" t="s">
-        <v>476</v>
-      </c>
-      <c r="X29" s="34" t="s">
-        <v>477</v>
-      </c>
-      <c r="Y29" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z29" s="15" t="s">
-        <v>354</v>
       </c>
       <c r="AA29" s="15" t="s">
         <v>288</v>
@@ -6180,13 +6238,13 @@
         <v>295</v>
       </c>
       <c r="AH29" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AJ29" s="15" t="s">
         <v>295</v>
       </c>
       <c r="AK29" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AM29" s="15" t="s">
         <v>288</v>
@@ -6207,19 +6265,19 @@
         <v>295</v>
       </c>
       <c r="AZ29" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BC29" s="15" t="s">
         <v>295</v>
       </c>
       <c r="BD29" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BG29" s="15" t="s">
         <v>288</v>
       </c>
       <c r="BK29" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="BL29" s="15" t="s">
         <v>347</v>
@@ -6243,7 +6301,7 @@
         <v>295</v>
       </c>
       <c r="BY29" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="CB29" s="15" t="s">
         <v>288</v>
@@ -6254,23 +6312,23 @@
     </row>
     <row r="30" spans="1:107" ht="407" customHeight="1">
       <c r="A30" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B30" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="D30" s="43" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="F30" s="19"/>
       <c r="G30" s="14" t="s">
-        <v>407</v>
+        <v>609</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I30" s="14" t="s">
         <v>55</v>
@@ -6279,52 +6337,52 @@
         <v>351</v>
       </c>
       <c r="K30" s="16">
-        <v>44007</v>
+        <v>44183</v>
       </c>
       <c r="L30" s="17" t="s">
         <v>352</v>
       </c>
       <c r="M30" s="17" t="s">
-        <v>546</v>
+        <v>604</v>
       </c>
       <c r="N30" s="15" t="s">
-        <v>547</v>
+        <v>605</v>
       </c>
       <c r="O30" s="15" t="s">
+        <v>606</v>
+      </c>
+      <c r="P30" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q30" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="R30" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="S30" s="34" t="s">
+        <v>460</v>
+      </c>
+      <c r="T30" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="U30" s="34" t="s">
+        <v>536</v>
+      </c>
+      <c r="V30" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="W30" s="34" t="s">
+        <v>464</v>
+      </c>
+      <c r="X30" s="34" t="s">
+        <v>465</v>
+      </c>
+      <c r="Y30" s="34" t="s">
+        <v>434</v>
+      </c>
+      <c r="Z30" s="15" t="s">
         <v>353</v>
-      </c>
-      <c r="P30" s="15" t="s">
-        <v>435</v>
-      </c>
-      <c r="Q30" s="18" t="s">
-        <v>588</v>
-      </c>
-      <c r="R30" s="4" t="s">
-        <v>583</v>
-      </c>
-      <c r="S30" s="34" t="s">
-        <v>472</v>
-      </c>
-      <c r="T30" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="U30" s="34" t="s">
-        <v>554</v>
-      </c>
-      <c r="V30" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="W30" s="34" t="s">
-        <v>476</v>
-      </c>
-      <c r="X30" s="34" t="s">
-        <v>477</v>
-      </c>
-      <c r="Y30" s="34" t="s">
-        <v>446</v>
-      </c>
-      <c r="Z30" s="15" t="s">
-        <v>354</v>
       </c>
       <c r="AA30" s="15" t="s">
         <v>288</v>
@@ -6339,13 +6397,13 @@
         <v>295</v>
       </c>
       <c r="AH30" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AJ30" s="15" t="s">
         <v>295</v>
       </c>
       <c r="AK30" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AM30" s="15" t="s">
         <v>288</v>
@@ -6366,19 +6424,19 @@
         <v>295</v>
       </c>
       <c r="AZ30" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BC30" s="15" t="s">
         <v>295</v>
       </c>
       <c r="BD30" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BG30" s="15" t="s">
         <v>288</v>
       </c>
       <c r="BK30" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="BL30" s="15" t="s">
         <v>347</v>
@@ -6402,7 +6460,7 @@
         <v>295</v>
       </c>
       <c r="BY30" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="CB30" s="15" t="s">
         <v>288</v>
@@ -6411,13 +6469,13 @@
         <v>295</v>
       </c>
       <c r="CG30" s="15" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="CH30" s="15" t="s">
         <v>305</v>
       </c>
       <c r="CL30" s="15" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="CO30" s="27">
         <v>55</v>
@@ -6431,23 +6489,23 @@
     </row>
     <row r="31" spans="1:107" ht="407" customHeight="1">
       <c r="A31" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B31" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="D31" s="43" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="F31" s="19"/>
       <c r="G31" s="14" t="s">
-        <v>408</v>
+        <v>610</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I31" s="14" t="s">
         <v>55</v>
@@ -6456,52 +6514,52 @@
         <v>351</v>
       </c>
       <c r="K31" s="16">
-        <v>44007</v>
+        <v>44183</v>
       </c>
       <c r="L31" s="17" t="s">
         <v>352</v>
       </c>
       <c r="M31" s="17" t="s">
-        <v>546</v>
+        <v>604</v>
       </c>
       <c r="N31" s="15" t="s">
-        <v>547</v>
+        <v>605</v>
       </c>
       <c r="O31" s="15" t="s">
+        <v>606</v>
+      </c>
+      <c r="P31" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q31" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="R31" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="S31" s="34" t="s">
+        <v>460</v>
+      </c>
+      <c r="T31" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="U31" s="34" t="s">
+        <v>621</v>
+      </c>
+      <c r="V31" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="W31" s="34" t="s">
+        <v>464</v>
+      </c>
+      <c r="X31" s="34" t="s">
+        <v>465</v>
+      </c>
+      <c r="Y31" s="34" t="s">
+        <v>434</v>
+      </c>
+      <c r="Z31" s="15" t="s">
         <v>353</v>
-      </c>
-      <c r="P31" s="15" t="s">
-        <v>435</v>
-      </c>
-      <c r="Q31" s="18" t="s">
-        <v>588</v>
-      </c>
-      <c r="R31" s="4" t="s">
-        <v>583</v>
-      </c>
-      <c r="S31" s="34" t="s">
-        <v>472</v>
-      </c>
-      <c r="T31" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="U31" s="34" t="s">
-        <v>582</v>
-      </c>
-      <c r="V31" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="W31" s="34" t="s">
-        <v>476</v>
-      </c>
-      <c r="X31" s="34" t="s">
-        <v>477</v>
-      </c>
-      <c r="Y31" s="34" t="s">
-        <v>446</v>
-      </c>
-      <c r="Z31" s="15" t="s">
-        <v>354</v>
       </c>
       <c r="AA31" s="15" t="s">
         <v>288</v>
@@ -6516,13 +6574,13 @@
         <v>295</v>
       </c>
       <c r="AH31" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AJ31" s="15" t="s">
         <v>295</v>
       </c>
       <c r="AK31" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AM31" s="15" t="s">
         <v>288</v>
@@ -6543,19 +6601,19 @@
         <v>295</v>
       </c>
       <c r="AZ31" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BC31" s="15" t="s">
         <v>295</v>
       </c>
       <c r="BD31" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BG31" s="15" t="s">
         <v>288</v>
       </c>
       <c r="BK31" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="BL31" s="15" t="s">
         <v>347</v>
@@ -6579,7 +6637,7 @@
         <v>295</v>
       </c>
       <c r="BY31" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="CB31" s="15" t="s">
         <v>288</v>
@@ -6588,13 +6646,13 @@
         <v>295</v>
       </c>
       <c r="CG31" s="15" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="CH31" s="15" t="s">
         <v>305</v>
       </c>
       <c r="CL31" s="15" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="CO31" s="27">
         <v>55</v>
@@ -6608,23 +6666,23 @@
     </row>
     <row r="32" spans="1:107" ht="407" customHeight="1">
       <c r="A32" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B32" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D32" s="43" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="F32" s="19"/>
       <c r="G32" s="14" t="s">
-        <v>403</v>
+        <v>611</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I32" s="14" t="s">
         <v>55</v>
@@ -6633,52 +6691,52 @@
         <v>351</v>
       </c>
       <c r="K32" s="16">
-        <v>44007</v>
+        <v>44183</v>
       </c>
       <c r="L32" s="17" t="s">
         <v>352</v>
       </c>
       <c r="M32" s="17" t="s">
-        <v>546</v>
+        <v>604</v>
       </c>
       <c r="N32" s="15" t="s">
-        <v>547</v>
+        <v>605</v>
       </c>
       <c r="O32" s="15" t="s">
+        <v>606</v>
+      </c>
+      <c r="P32" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q32" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="R32" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="S32" s="34" t="s">
+        <v>460</v>
+      </c>
+      <c r="T32" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="U32" s="34" t="s">
+        <v>536</v>
+      </c>
+      <c r="V32" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="W32" s="34" t="s">
+        <v>464</v>
+      </c>
+      <c r="X32" s="34" t="s">
+        <v>465</v>
+      </c>
+      <c r="Y32" s="34" t="s">
+        <v>444</v>
+      </c>
+      <c r="Z32" s="15" t="s">
         <v>353</v>
-      </c>
-      <c r="P32" s="15" t="s">
-        <v>435</v>
-      </c>
-      <c r="Q32" s="18" t="s">
-        <v>588</v>
-      </c>
-      <c r="R32" s="4" t="s">
-        <v>556</v>
-      </c>
-      <c r="S32" s="34" t="s">
-        <v>472</v>
-      </c>
-      <c r="T32" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="U32" s="34" t="s">
-        <v>554</v>
-      </c>
-      <c r="V32" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="W32" s="34" t="s">
-        <v>476</v>
-      </c>
-      <c r="X32" s="34" t="s">
-        <v>477</v>
-      </c>
-      <c r="Y32" s="34" t="s">
-        <v>456</v>
-      </c>
-      <c r="Z32" s="15" t="s">
-        <v>354</v>
       </c>
       <c r="AA32" s="15" t="s">
         <v>288</v>
@@ -6705,19 +6763,19 @@
         <v>295</v>
       </c>
       <c r="AZ32" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BC32" s="15" t="s">
         <v>295</v>
       </c>
       <c r="BD32" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BG32" s="15" t="s">
         <v>288</v>
       </c>
       <c r="BK32" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="BL32" s="15" t="s">
         <v>347</v>
@@ -6735,7 +6793,7 @@
         <v>295</v>
       </c>
       <c r="CG32" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="CH32" s="15" t="s">
         <v>289</v>
@@ -6764,23 +6822,23 @@
     </row>
     <row r="33" spans="1:107" ht="407" customHeight="1">
       <c r="A33" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B33" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D33" s="43" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="F33" s="19"/>
       <c r="G33" s="14" t="s">
-        <v>404</v>
+        <v>612</v>
       </c>
       <c r="H33" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I33" s="14" t="s">
         <v>55</v>
@@ -6789,52 +6847,52 @@
         <v>351</v>
       </c>
       <c r="K33" s="16">
-        <v>44007</v>
+        <v>44183</v>
       </c>
       <c r="L33" s="17" t="s">
         <v>352</v>
       </c>
       <c r="M33" s="17" t="s">
-        <v>546</v>
+        <v>604</v>
       </c>
       <c r="N33" s="15" t="s">
-        <v>547</v>
+        <v>605</v>
       </c>
       <c r="O33" s="15" t="s">
+        <v>606</v>
+      </c>
+      <c r="P33" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q33" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="R33" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="S33" s="34" t="s">
+        <v>460</v>
+      </c>
+      <c r="T33" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="U33" s="34" t="s">
+        <v>621</v>
+      </c>
+      <c r="V33" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="W33" s="34" t="s">
+        <v>464</v>
+      </c>
+      <c r="X33" s="34" t="s">
+        <v>465</v>
+      </c>
+      <c r="Y33" s="34" t="s">
+        <v>444</v>
+      </c>
+      <c r="Z33" s="15" t="s">
         <v>353</v>
-      </c>
-      <c r="P33" s="15" t="s">
-        <v>435</v>
-      </c>
-      <c r="Q33" s="18" t="s">
-        <v>588</v>
-      </c>
-      <c r="R33" s="4" t="s">
-        <v>584</v>
-      </c>
-      <c r="S33" s="34" t="s">
-        <v>472</v>
-      </c>
-      <c r="T33" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="U33" s="34" t="s">
-        <v>582</v>
-      </c>
-      <c r="V33" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="W33" s="34" t="s">
-        <v>476</v>
-      </c>
-      <c r="X33" s="34" t="s">
-        <v>477</v>
-      </c>
-      <c r="Y33" s="34" t="s">
-        <v>456</v>
-      </c>
-      <c r="Z33" s="15" t="s">
-        <v>354</v>
       </c>
       <c r="AA33" s="15" t="s">
         <v>288</v>
@@ -6861,19 +6919,19 @@
         <v>295</v>
       </c>
       <c r="AZ33" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BC33" s="15" t="s">
         <v>295</v>
       </c>
       <c r="BD33" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BG33" s="15" t="s">
         <v>288</v>
       </c>
       <c r="BK33" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="BL33" s="15" t="s">
         <v>347</v>
@@ -6891,7 +6949,7 @@
         <v>295</v>
       </c>
       <c r="CG33" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="CH33" s="15" t="s">
         <v>289</v>
@@ -6920,23 +6978,23 @@
     </row>
     <row r="34" spans="1:107" ht="407" customHeight="1">
       <c r="A34" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D34" s="43" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="F34" s="19"/>
       <c r="G34" s="14" t="s">
-        <v>399</v>
+        <v>613</v>
       </c>
       <c r="H34" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I34" s="14" t="s">
         <v>55</v>
@@ -6945,52 +7003,52 @@
         <v>351</v>
       </c>
       <c r="K34" s="16">
-        <v>44007</v>
+        <v>44183</v>
       </c>
       <c r="L34" s="17" t="s">
         <v>352</v>
       </c>
       <c r="M34" s="17" t="s">
-        <v>546</v>
+        <v>604</v>
       </c>
       <c r="N34" s="15" t="s">
-        <v>547</v>
+        <v>605</v>
       </c>
       <c r="O34" s="15" t="s">
+        <v>606</v>
+      </c>
+      <c r="P34" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q34" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="R34" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="S34" s="34" t="s">
+        <v>460</v>
+      </c>
+      <c r="T34" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="U34" s="34" t="s">
+        <v>536</v>
+      </c>
+      <c r="V34" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="W34" s="34" t="s">
+        <v>464</v>
+      </c>
+      <c r="X34" s="34" t="s">
+        <v>465</v>
+      </c>
+      <c r="Y34" s="34" t="s">
+        <v>432</v>
+      </c>
+      <c r="Z34" s="15" t="s">
         <v>353</v>
-      </c>
-      <c r="P34" s="15" t="s">
-        <v>435</v>
-      </c>
-      <c r="Q34" s="18" t="s">
-        <v>588</v>
-      </c>
-      <c r="R34" s="4" t="s">
-        <v>557</v>
-      </c>
-      <c r="S34" s="34" t="s">
-        <v>472</v>
-      </c>
-      <c r="T34" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="U34" s="34" t="s">
-        <v>554</v>
-      </c>
-      <c r="V34" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="W34" s="34" t="s">
-        <v>476</v>
-      </c>
-      <c r="X34" s="34" t="s">
-        <v>477</v>
-      </c>
-      <c r="Y34" s="34" t="s">
-        <v>444</v>
-      </c>
-      <c r="Z34" s="15" t="s">
-        <v>354</v>
       </c>
       <c r="AA34" s="15" t="s">
         <v>288</v>
@@ -7017,19 +7075,19 @@
         <v>295</v>
       </c>
       <c r="AZ34" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BC34" s="15" t="s">
         <v>295</v>
       </c>
       <c r="BD34" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BG34" s="15" t="s">
         <v>288</v>
       </c>
       <c r="BK34" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="BL34" s="15" t="s">
         <v>347</v>
@@ -7047,29 +7105,29 @@
         <v>295</v>
       </c>
       <c r="CG34" s="15" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="CH34" s="15" t="s">
         <v>289</v>
       </c>
       <c r="CI34" s="15" t="s">
+        <v>375</v>
+      </c>
+      <c r="CL34" s="29" t="s">
         <v>376</v>
-      </c>
-      <c r="CL34" s="29" t="s">
-        <v>377</v>
       </c>
       <c r="CN34" s="27">
         <v>10</v>
       </c>
       <c r="CR34" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="CS34" s="8"/>
       <c r="CT34" s="15">
         <v>20</v>
       </c>
       <c r="CX34" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="CZ34" s="15">
         <v>30</v>
@@ -7077,23 +7135,23 @@
     </row>
     <row r="35" spans="1:107" ht="407" customHeight="1">
       <c r="A35" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B35" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D35" s="43" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="F35" s="19"/>
       <c r="G35" s="14" t="s">
-        <v>400</v>
+        <v>614</v>
       </c>
       <c r="H35" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I35" s="14" t="s">
         <v>55</v>
@@ -7102,52 +7160,52 @@
         <v>351</v>
       </c>
       <c r="K35" s="16">
-        <v>44007</v>
+        <v>44183</v>
       </c>
       <c r="L35" s="17" t="s">
         <v>352</v>
       </c>
       <c r="M35" s="17" t="s">
-        <v>546</v>
+        <v>604</v>
       </c>
       <c r="N35" s="15" t="s">
-        <v>547</v>
+        <v>605</v>
       </c>
       <c r="O35" s="15" t="s">
+        <v>606</v>
+      </c>
+      <c r="P35" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q35" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="R35" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="S35" s="34" t="s">
+        <v>460</v>
+      </c>
+      <c r="T35" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="U35" s="34" t="s">
+        <v>621</v>
+      </c>
+      <c r="V35" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="W35" s="34" t="s">
+        <v>464</v>
+      </c>
+      <c r="X35" s="34" t="s">
+        <v>465</v>
+      </c>
+      <c r="Y35" s="34" t="s">
+        <v>432</v>
+      </c>
+      <c r="Z35" s="15" t="s">
         <v>353</v>
-      </c>
-      <c r="P35" s="15" t="s">
-        <v>435</v>
-      </c>
-      <c r="Q35" s="18" t="s">
-        <v>588</v>
-      </c>
-      <c r="R35" s="4" t="s">
-        <v>585</v>
-      </c>
-      <c r="S35" s="34" t="s">
-        <v>472</v>
-      </c>
-      <c r="T35" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="U35" s="34" t="s">
-        <v>582</v>
-      </c>
-      <c r="V35" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="W35" s="34" t="s">
-        <v>476</v>
-      </c>
-      <c r="X35" s="34" t="s">
-        <v>477</v>
-      </c>
-      <c r="Y35" s="34" t="s">
-        <v>444</v>
-      </c>
-      <c r="Z35" s="15" t="s">
-        <v>354</v>
       </c>
       <c r="AA35" s="15" t="s">
         <v>288</v>
@@ -7174,19 +7232,19 @@
         <v>295</v>
       </c>
       <c r="AZ35" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BC35" s="15" t="s">
         <v>295</v>
       </c>
       <c r="BD35" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BG35" s="15" t="s">
         <v>288</v>
       </c>
       <c r="BK35" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="BL35" s="15" t="s">
         <v>347</v>
@@ -7204,29 +7262,29 @@
         <v>295</v>
       </c>
       <c r="CG35" s="15" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="CH35" s="15" t="s">
         <v>289</v>
       </c>
       <c r="CI35" s="15" t="s">
+        <v>375</v>
+      </c>
+      <c r="CL35" s="29" t="s">
         <v>376</v>
-      </c>
-      <c r="CL35" s="29" t="s">
-        <v>377</v>
       </c>
       <c r="CN35" s="27">
         <v>10</v>
       </c>
       <c r="CR35" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="CS35" s="8"/>
       <c r="CT35" s="15">
         <v>20</v>
       </c>
       <c r="CX35" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="CZ35" s="15">
         <v>30</v>
@@ -7234,23 +7292,23 @@
     </row>
     <row r="36" spans="1:107" ht="407" customHeight="1">
       <c r="A36" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B36" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D36" s="43" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="F36" s="19"/>
       <c r="G36" s="14" t="s">
-        <v>416</v>
+        <v>615</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I36" s="14" t="s">
         <v>55</v>
@@ -7259,52 +7317,52 @@
         <v>351</v>
       </c>
       <c r="K36" s="16">
-        <v>44007</v>
+        <v>44183</v>
       </c>
       <c r="L36" s="17" t="s">
         <v>352</v>
       </c>
       <c r="M36" s="17" t="s">
-        <v>546</v>
+        <v>604</v>
       </c>
       <c r="N36" s="15" t="s">
-        <v>547</v>
+        <v>605</v>
       </c>
       <c r="O36" s="15" t="s">
+        <v>606</v>
+      </c>
+      <c r="P36" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q36" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="R36" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="S36" s="34" t="s">
+        <v>460</v>
+      </c>
+      <c r="T36" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="U36" s="34" t="s">
+        <v>536</v>
+      </c>
+      <c r="V36" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="W36" s="34" t="s">
+        <v>464</v>
+      </c>
+      <c r="X36" s="34" t="s">
+        <v>465</v>
+      </c>
+      <c r="Y36" s="35" t="s">
+        <v>462</v>
+      </c>
+      <c r="Z36" s="15" t="s">
         <v>353</v>
-      </c>
-      <c r="P36" s="15" t="s">
-        <v>435</v>
-      </c>
-      <c r="Q36" s="18" t="s">
-        <v>588</v>
-      </c>
-      <c r="R36" s="4" t="s">
-        <v>558</v>
-      </c>
-      <c r="S36" s="34" t="s">
-        <v>472</v>
-      </c>
-      <c r="T36" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="U36" s="34" t="s">
-        <v>554</v>
-      </c>
-      <c r="V36" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="W36" s="34" t="s">
-        <v>476</v>
-      </c>
-      <c r="X36" s="34" t="s">
-        <v>477</v>
-      </c>
-      <c r="Y36" s="35" t="s">
-        <v>474</v>
-      </c>
-      <c r="Z36" s="15" t="s">
-        <v>354</v>
       </c>
       <c r="AA36" s="15" t="s">
         <v>288</v>
@@ -7331,19 +7389,19 @@
         <v>295</v>
       </c>
       <c r="AZ36" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BC36" s="15" t="s">
         <v>295</v>
       </c>
       <c r="BD36" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BG36" s="15" t="s">
         <v>288</v>
       </c>
       <c r="BK36" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="BL36" s="15" t="s">
         <v>347</v>
@@ -7361,34 +7419,34 @@
         <v>295</v>
       </c>
       <c r="CG36" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="CH36" s="15" t="s">
         <v>305</v>
       </c>
       <c r="CL36" s="15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="37" spans="1:107" ht="407" customHeight="1">
       <c r="A37" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B37" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D37" s="43" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="F37" s="19"/>
       <c r="G37" s="14" t="s">
-        <v>396</v>
+        <v>616</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I37" s="14" t="s">
         <v>55</v>
@@ -7397,52 +7455,52 @@
         <v>351</v>
       </c>
       <c r="K37" s="16">
-        <v>44007</v>
+        <v>44183</v>
       </c>
       <c r="L37" s="17" t="s">
         <v>352</v>
       </c>
       <c r="M37" s="17" t="s">
-        <v>546</v>
+        <v>604</v>
       </c>
       <c r="N37" s="15" t="s">
-        <v>547</v>
+        <v>605</v>
       </c>
       <c r="O37" s="15" t="s">
+        <v>606</v>
+      </c>
+      <c r="P37" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q37" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="R37" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="S37" s="34" t="s">
+        <v>460</v>
+      </c>
+      <c r="T37" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="U37" s="34" t="s">
+        <v>621</v>
+      </c>
+      <c r="V37" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="W37" s="34" t="s">
+        <v>464</v>
+      </c>
+      <c r="X37" s="34" t="s">
+        <v>465</v>
+      </c>
+      <c r="Y37" s="35" t="s">
+        <v>462</v>
+      </c>
+      <c r="Z37" s="15" t="s">
         <v>353</v>
-      </c>
-      <c r="P37" s="15" t="s">
-        <v>435</v>
-      </c>
-      <c r="Q37" s="18" t="s">
-        <v>588</v>
-      </c>
-      <c r="R37" s="4" t="s">
-        <v>586</v>
-      </c>
-      <c r="S37" s="34" t="s">
-        <v>472</v>
-      </c>
-      <c r="T37" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="U37" s="34" t="s">
-        <v>582</v>
-      </c>
-      <c r="V37" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="W37" s="34" t="s">
-        <v>476</v>
-      </c>
-      <c r="X37" s="34" t="s">
-        <v>477</v>
-      </c>
-      <c r="Y37" s="35" t="s">
-        <v>474</v>
-      </c>
-      <c r="Z37" s="15" t="s">
-        <v>354</v>
       </c>
       <c r="AA37" s="15" t="s">
         <v>288</v>
@@ -7469,19 +7527,19 @@
         <v>295</v>
       </c>
       <c r="AZ37" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BC37" s="15" t="s">
         <v>295</v>
       </c>
       <c r="BD37" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BG37" s="15" t="s">
         <v>288</v>
       </c>
       <c r="BK37" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="BL37" s="15" t="s">
         <v>347</v>
@@ -7499,13 +7557,13 @@
         <v>295</v>
       </c>
       <c r="CG37" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="CH37" s="15" t="s">
         <v>305</v>
       </c>
       <c r="CL37" s="15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="38" spans="1:107" ht="407" customHeight="1">
@@ -7515,63 +7573,66 @@
       <c r="B38" s="13" t="s">
         <v>98</v>
       </c>
+      <c r="C38" s="31" t="s">
+        <v>593</v>
+      </c>
       <c r="F38" s="19"/>
       <c r="G38" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="J38" s="8" t="s">
         <v>382</v>
-      </c>
-      <c r="H38" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="I38" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="J38" s="8" t="s">
-        <v>383</v>
       </c>
       <c r="K38" s="23">
         <v>43890</v>
       </c>
       <c r="L38" s="9" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="M38" s="9" t="s">
-        <v>496</v>
+        <v>484</v>
       </c>
       <c r="N38" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="O38" s="5" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="P38" s="15" t="s">
-        <v>438</v>
+        <v>426</v>
       </c>
       <c r="Q38" s="10" t="s">
         <v>317</v>
       </c>
       <c r="R38" s="25" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="S38" s="35" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="T38" s="35" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="U38" s="35" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="V38" s="35" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="W38" s="35" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="X38" s="35" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="Y38" s="35" t="s">
-        <v>474</v>
+        <v>462</v>
       </c>
       <c r="AF38" s="15" t="s">
         <v>288</v>
@@ -7586,13 +7647,13 @@
         <v>295</v>
       </c>
       <c r="CG38" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="CH38" s="15" t="s">
         <v>305</v>
       </c>
       <c r="CL38" s="15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="39" spans="1:107" ht="297" customHeight="1">
@@ -7602,69 +7663,72 @@
       <c r="B39" s="13" t="s">
         <v>98</v>
       </c>
+      <c r="C39" s="31" t="s">
+        <v>594</v>
+      </c>
       <c r="D39" s="42" t="s">
-        <v>575</v>
+        <v>592</v>
       </c>
       <c r="E39" s="14" t="s">
         <v>55</v>
       </c>
       <c r="F39" s="19"/>
       <c r="G39" s="8" t="s">
-        <v>497</v>
+        <v>485</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>497</v>
+        <v>485</v>
       </c>
       <c r="I39" s="8" t="s">
         <v>55</v>
       </c>
       <c r="J39" s="8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="K39" s="23">
         <v>44110</v>
       </c>
       <c r="L39" s="9" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="M39" s="9" t="s">
-        <v>498</v>
+        <v>486</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>499</v>
+        <v>487</v>
       </c>
       <c r="O39" s="5" t="s">
-        <v>500</v>
+        <v>488</v>
       </c>
       <c r="P39" s="15" t="s">
-        <v>501</v>
+        <v>489</v>
       </c>
       <c r="Q39" s="24" t="s">
-        <v>573</v>
+        <v>555</v>
       </c>
       <c r="R39" s="25" t="s">
-        <v>502</v>
+        <v>591</v>
       </c>
       <c r="S39" s="35" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="T39" s="35" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="U39" s="35" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="V39" s="35" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="W39" s="35" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="X39" s="35" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="Y39" s="35" t="s">
-        <v>574</v>
+        <v>556</v>
       </c>
       <c r="AF39" s="15" t="s">
         <v>288</v>
@@ -7685,7 +7749,7 @@
         <v>305</v>
       </c>
       <c r="CL39" s="15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="40" spans="1:107" ht="297" customHeight="1">
@@ -7695,55 +7759,58 @@
       <c r="B40" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D40" s="37" t="s">
-        <v>577</v>
+      <c r="C40" s="31" t="s">
+        <v>590</v>
+      </c>
+      <c r="D40" s="42" t="s">
+        <v>558</v>
       </c>
       <c r="E40" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F40" s="36" t="s">
-        <v>503</v>
+      <c r="F40" s="7" t="s">
+        <v>490</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>504</v>
+        <v>491</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>504</v>
+        <v>491</v>
       </c>
       <c r="I40" s="8" t="s">
         <v>55</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>505</v>
+        <v>492</v>
       </c>
       <c r="K40" s="23">
         <v>44246</v>
       </c>
       <c r="L40" s="9" t="s">
-        <v>506</v>
+        <v>493</v>
       </c>
       <c r="M40" s="9" t="s">
-        <v>507</v>
+        <v>494</v>
       </c>
       <c r="N40" s="8" t="s">
-        <v>508</v>
+        <v>495</v>
       </c>
       <c r="O40" s="5"/>
       <c r="P40" s="5" t="s">
-        <v>509</v>
+        <v>496</v>
       </c>
       <c r="Q40" s="10"/>
       <c r="R40" s="4" t="s">
-        <v>576</v>
+        <v>557</v>
       </c>
       <c r="S40" s="34" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="U40" s="34" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="W40" s="34" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
     </row>
     <row r="41" spans="1:107" ht="297" customHeight="1">
@@ -7753,48 +7820,153 @@
       <c r="B41" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D41" s="37" t="s">
+      <c r="C41" s="31" t="s">
+        <v>595</v>
+      </c>
+      <c r="D41" s="42" t="s">
         <v>589</v>
       </c>
       <c r="E41" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F41" s="36" t="s">
-        <v>511</v>
+      <c r="F41" s="7" t="s">
+        <v>497</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>512</v>
+        <v>498</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>512</v>
+        <v>498</v>
       </c>
       <c r="I41" s="8" t="s">
         <v>55</v>
       </c>
       <c r="J41" s="8" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="K41" s="23">
         <v>44249</v>
       </c>
       <c r="L41" s="9" t="s">
-        <v>516</v>
+        <v>502</v>
       </c>
       <c r="M41" s="9" t="s">
-        <v>514</v>
+        <v>500</v>
       </c>
       <c r="N41" s="8" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
       <c r="O41" s="5"/>
       <c r="P41" s="5" t="s">
-        <v>517</v>
+        <v>503</v>
       </c>
       <c r="Q41" s="10" t="s">
-        <v>510</v>
+        <v>588</v>
       </c>
       <c r="R41" s="11" t="s">
-        <v>578</v>
+        <v>585</v>
+      </c>
+      <c r="S41" s="34" t="s">
+        <v>460</v>
+      </c>
+      <c r="T41" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="U41" s="34" t="s">
+        <v>536</v>
+      </c>
+      <c r="V41" s="34" t="s">
+        <v>586</v>
+      </c>
+      <c r="W41" s="34" t="s">
+        <v>464</v>
+      </c>
+      <c r="X41" s="34" t="s">
+        <v>587</v>
+      </c>
+      <c r="Y41" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z41" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="AA41" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="AC41" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="AF41" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="AG41" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="AH41" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="AJ41" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="AK41" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="AM41" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="AP41" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="AQ41" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="AR41" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="AX41" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="AY41" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="BC41" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="BG41" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="BK41" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="BL41" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="BM41" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="BO41" s="15">
+        <v>5</v>
+      </c>
+      <c r="BS41" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="BT41" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="BU41" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="BX41" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="BY41" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="CB41" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="CF41" s="15" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="42" spans="1:107" ht="297" customHeight="1">
@@ -7805,17 +7977,20 @@
         <v>89</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>518</v>
+        <v>597</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>596</v>
       </c>
       <c r="E42" s="14" t="s">
         <v>55</v>
       </c>
       <c r="F42" s="36"/>
       <c r="G42" s="8" t="s">
-        <v>524</v>
+        <v>508</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>519</v>
+        <v>504</v>
       </c>
       <c r="I42" s="14" t="s">
         <v>58</v>
@@ -7830,39 +8005,205 @@
         <v>352</v>
       </c>
       <c r="M42" s="17" t="s">
-        <v>520</v>
+        <v>505</v>
       </c>
       <c r="N42" s="15" t="s">
-        <v>521</v>
+        <v>506</v>
       </c>
       <c r="O42" s="15" t="s">
-        <v>522</v>
+        <v>507</v>
       </c>
       <c r="P42" s="15" t="s">
-        <v>523</v>
-      </c>
-      <c r="Q42" s="10"/>
-      <c r="R42" s="11"/>
+        <v>601</v>
+      </c>
+      <c r="Q42" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="R42" s="11" t="s">
+        <v>625</v>
+      </c>
+      <c r="S42" s="34" t="s">
+        <v>598</v>
+      </c>
+      <c r="T42" s="34" t="s">
+        <v>599</v>
+      </c>
+      <c r="U42" s="34" t="s">
+        <v>622</v>
+      </c>
+      <c r="V42" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="W42" s="34" t="s">
+        <v>623</v>
+      </c>
+      <c r="X42" s="34" t="s">
+        <v>465</v>
+      </c>
+      <c r="Y42" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z42" s="15" t="s">
+        <v>600</v>
+      </c>
+      <c r="AA42" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="AC42" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="AF42" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="AG42" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="AH42" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="AJ42" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="AK42" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="AM42" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="AP42" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="AQ42" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="AR42" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="AX42" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="AY42" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="AZ42" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="BC42" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="BD42" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="BG42" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="BK42" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="BL42" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="BM42" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="BO42" s="15">
+        <v>5</v>
+      </c>
+      <c r="BS42" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="BT42" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="BU42" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="BX42" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="BY42" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="CB42" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="CF42" s="15" t="s">
+        <v>288</v>
+      </c>
     </row>
-    <row r="43" spans="1:107" ht="42">
+    <row r="43" spans="1:107" ht="297" customHeight="1">
       <c r="A43" s="12" t="s">
         <v>58</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="G43" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="I43" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>617</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>596</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F43" s="36"/>
+      <c r="G43" s="8" t="s">
+        <v>628</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="I43" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="L43" s="26"/>
-      <c r="M43" s="26"/>
-      <c r="Q43" s="18"/>
-      <c r="R43" s="4"/>
+      <c r="J43" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="K43" s="16">
+        <v>44327</v>
+      </c>
+      <c r="L43" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="M43" s="17" t="s">
+        <v>618</v>
+      </c>
+      <c r="N43" s="15" t="s">
+        <v>619</v>
+      </c>
+      <c r="Q43" s="44" t="s">
+        <v>626</v>
+      </c>
+      <c r="R43" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="S43" s="34" t="s">
+        <v>620</v>
+      </c>
+      <c r="T43" s="34" t="s">
+        <v>440</v>
+      </c>
+      <c r="U43" s="34" t="s">
+        <v>622</v>
+      </c>
+      <c r="V43" s="34" t="s">
+        <v>440</v>
+      </c>
+      <c r="W43" s="34" t="s">
+        <v>624</v>
+      </c>
+      <c r="X43" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="Y43" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z43" s="15" t="s">
+        <v>600</v>
+      </c>
       <c r="AA43" s="15" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="AB43" s="15">
         <v>20</v>
@@ -7876,187 +8217,277 @@
       <c r="AG43" s="15" t="s">
         <v>288</v>
       </c>
-      <c r="AI43" s="15">
-        <v>5</v>
-      </c>
       <c r="AJ43" s="15" t="s">
         <v>288</v>
       </c>
-      <c r="AL43" s="15">
-        <v>5</v>
-      </c>
       <c r="AM43" s="15" t="s">
         <v>288</v>
       </c>
-      <c r="AO43" s="15">
-        <v>5</v>
+      <c r="AP43" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="AQ43" s="15" t="s">
+        <v>347</v>
       </c>
       <c r="AR43" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="AT43" s="15">
+      <c r="AX43" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="AY43" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="BC43" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="BG43" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="BK43" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="BL43" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="BM43" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="BS43" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="BT43" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="BU43" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="BX43" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="BY43" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="CB43" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="CF43" s="15" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="44" spans="1:107" ht="42">
+      <c r="A44" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G44" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I44" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="L44" s="26"/>
+      <c r="M44" s="26"/>
+      <c r="Q44" s="18"/>
+      <c r="R44" s="4"/>
+      <c r="AA44" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="AB44" s="15">
+        <v>20</v>
+      </c>
+      <c r="AC44" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="AF44" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="AG44" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="AI44" s="15">
         <v>5</v>
       </c>
-      <c r="AU43" s="15">
+      <c r="AJ44" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="AL44" s="15">
+        <v>5</v>
+      </c>
+      <c r="AM44" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="AO44" s="15">
+        <v>5</v>
+      </c>
+      <c r="AR44" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="AT44" s="15">
+        <v>5</v>
+      </c>
+      <c r="AU44" s="15">
         <v>24</v>
       </c>
-      <c r="AV43" s="15">
+      <c r="AV44" s="15">
         <v>100</v>
       </c>
-      <c r="AW43" s="15">
+      <c r="AW44" s="15">
         <v>400</v>
       </c>
-      <c r="AX43" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="AY43" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="BA43" s="15">
+      <c r="AX44" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="AY44" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="BA44" s="15">
         <v>5</v>
       </c>
-      <c r="BB43" s="15">
+      <c r="BB44" s="15">
         <v>5</v>
       </c>
-      <c r="BC43" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="BE43" s="15">
+      <c r="BC44" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="BE44" s="15">
         <v>5</v>
       </c>
-      <c r="BF43" s="15">
+      <c r="BF44" s="15">
         <v>5</v>
       </c>
-      <c r="BG43" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="BI43" s="15">
+      <c r="BG44" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="BI44" s="15">
         <v>5</v>
       </c>
-      <c r="BJ43" s="15">
+      <c r="BJ44" s="15">
         <v>5</v>
       </c>
-      <c r="BL43" s="15" t="s">
+      <c r="BL44" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="BO43" s="15">
+      <c r="BO44" s="15">
         <v>5</v>
       </c>
-      <c r="BP43" s="15">
+      <c r="BP44" s="15">
         <v>24</v>
       </c>
-      <c r="BQ43" s="15">
+      <c r="BQ44" s="15">
         <v>100</v>
       </c>
-      <c r="BR43" s="15">
+      <c r="BR44" s="15">
         <v>400</v>
       </c>
-      <c r="BS43" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="BT43" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="BV43" s="15">
+      <c r="BS44" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="BT44" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="BV44" s="15">
         <v>5</v>
       </c>
-      <c r="BW43" s="15">
+      <c r="BW44" s="15">
         <v>5</v>
       </c>
-      <c r="BX43" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="BZ43" s="15">
+      <c r="BX44" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="BZ44" s="15">
         <v>5</v>
       </c>
-      <c r="CA43" s="15">
+      <c r="CA44" s="15">
         <v>5</v>
       </c>
-      <c r="CB43" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="CD43" s="15">
+      <c r="CB44" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="CD44" s="15">
         <v>5</v>
       </c>
-      <c r="CE43" s="15">
+      <c r="CE44" s="15">
         <v>5</v>
       </c>
-      <c r="CF43" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="CG43" s="15" t="s">
+      <c r="CF44" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="CG44" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="CH43" s="15" t="s">
+      <c r="CH44" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="CI43" s="15" t="s">
+      <c r="CI44" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="CJ43" s="15">
+      <c r="CJ44" s="15">
         <v>0.7</v>
       </c>
-      <c r="CK43" s="15" t="s">
+      <c r="CK44" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="CL43" s="15" t="s">
+      <c r="CL44" s="15" t="s">
         <v>291</v>
       </c>
-      <c r="CM43" s="15">
+      <c r="CM44" s="15">
         <v>50</v>
       </c>
-      <c r="CN43" s="27">
+      <c r="CN44" s="27">
         <v>5</v>
       </c>
-      <c r="CO43" s="27">
+      <c r="CO44" s="27">
         <v>5</v>
       </c>
-      <c r="CP43" s="27">
+      <c r="CP44" s="27">
         <v>5</v>
       </c>
-      <c r="CQ43" s="27">
+      <c r="CQ44" s="27">
         <v>5</v>
       </c>
-      <c r="CR43" s="15" t="s">
+      <c r="CR44" s="15" t="s">
         <v>292</v>
       </c>
-      <c r="CS43" s="15">
+      <c r="CS44" s="15">
         <v>5</v>
       </c>
-      <c r="CT43" s="15">
+      <c r="CT44" s="15">
         <v>5</v>
       </c>
-      <c r="CU43" s="27">
+      <c r="CU44" s="27">
         <v>5</v>
       </c>
-      <c r="CV43" s="27">
+      <c r="CV44" s="27">
         <v>5</v>
       </c>
-      <c r="CW43" s="27">
+      <c r="CW44" s="27">
         <v>5</v>
       </c>
-      <c r="CX43" s="15" t="s">
+      <c r="CX44" s="15" t="s">
         <v>293</v>
       </c>
-      <c r="CY43" s="15">
+      <c r="CY44" s="15">
         <v>5</v>
       </c>
-      <c r="CZ43" s="15">
+      <c r="CZ44" s="15">
         <v>5</v>
       </c>
-      <c r="DA43" s="27">
+      <c r="DA44" s="27">
         <v>5</v>
       </c>
-      <c r="DB43" s="27">
+      <c r="DB44" s="27">
         <v>5</v>
       </c>
-      <c r="DC43" s="27">
+      <c r="DC44" s="27">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:CZ43">
-    <sortCondition ref="K2:K43"/>
+  <sortState ref="A2:CZ44">
+    <sortCondition ref="K2:K44"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
last proposal assumptions update
</commit_message>
<xml_diff>
--- a/app/data/wto_proposal_settings_master.xlsx
+++ b/app/data/wto_proposal_settings_master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kat/GitHub/SubsidyExplorer/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0482749-5CA5-0D43-96FD-BCD8904DCE2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC53ADA1-BBD9-434F-9AD2-736296497AF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1813,9 +1813,6 @@
     <t>Subsidies granted by all Members shall be allowed for fishing within their own territorial waters.</t>
   </si>
   <si>
-    <t>Subsidies granted by LDCs shall be allowed, and subsidies granted by all other Members shall be allowed for fishing in their territorial seas.</t>
-  </si>
-  <si>
     <t xml:space="preserve">For IUU: Subsidies granted by developing and LDC Members shall be allowed for small scale fishing: a) for unreported and unregulated fishing: b) within their own territorial waters. Transition periods are also considered as an alternative but are not modeled here. For Overfished: Subsidies granted by all Members for fishing within their own territorial sea shall be allowed. Transition periods are also considered as an alternative but are not modeled here. For OCOF: Subsidies granted by LDCs shall be allowed, and subsidies granted by all other Members shall be allowed for fishing in their territorial seas. Transition periods are also considered as an alternative but are not modeled here. If transition periods were employed, we assume that LDCs would enjoy a transition period specifically for them. </t>
   </si>
   <si>
@@ -1912,9 +1909,6 @@
     <t>&lt;ol&gt;&lt;li&gt;There is uncertainty regarding the status of many fish stocks.&lt;/li&gt;&lt;li&gt;For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 0.8) in the RAM Legacy Stock Assessment Database are prohibited.&lt;/li&gt;&lt;li&gt;The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database.&lt;/li&gt;&lt;li&gt;The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text.&lt;/li&gt;&lt;li&gt;The definition for an overfished stock subsidy prohibition considered here is the less ambitious interpretation considered in the previous version of the text (see Overfished - Negative effects (Option A)).&lt;/li&gt;&lt;/ol&gt;</t>
   </si>
   <si>
-    <t>&lt;ol&gt;&lt;li&gt;We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction.&lt;/li&gt;&lt;li&gt;We note that this is a conservative interpretation of this proposal, as the text prohibits these types of subsidies for all fishing unless a Member can demonstrate that measures are implemented to maintain stocks at a biologically sustainable level. However, it is unclear how many Members would be able to satisfy this sustainability criteria, and thus we assume that such an exemption could be aquired by all Members.&lt;/li&gt;&lt;li&gt;By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited.&lt;/li&gt;&lt;/ol&gt;</t>
-  </si>
-  <si>
     <t>For IUU: 1) Final determinations are made by existing RFMO/A vessel lists, and by flag and coastal Member states. 2) No publically available data exist for most flag Members, nor for coastal Members. 3) The possible effects is a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about expected IUU-findings. 4) No proportionality or the duration of prohibition is considered. For Overfished: 1) There is uncertainty  regarding the status of many fish stocks. 2) For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 0.8) in the RAM Legacy Stock Assessment Database are prohibited. 3) The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database. 4) The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text. 5) The definition for an overfished stock subsidy prohibition considered here is the less ambitious interpretation considered in the previous version of the text. For OFOC: 1) We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. 2) We note that this is an ambitious interpretation of this proposal, as the text makes it clear that the fact that a subsidy is granted is not reason enough for that subsidy to be prohibited. However, data does not exist at present to make this determination for subsidy programs globally. 3) By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited. For Cap: None.</t>
   </si>
   <si>
@@ -1930,9 +1924,6 @@
     <t>&lt;ol&gt;&lt;li&gt;There is uncertainty regarding the status of many fish stocks.&lt;/li&gt;&lt;li&gt;For the purposes of modeling this proposal, we assume that subsidies to fishing on stocks identified as overfished (B/Bmsy &lt; 0.8) in the RAM Legacy Stock Assessment Database are prohibited.&lt;/li&gt;&lt;li&gt;The proportion of stocks identified as overfished in the RAM Legacy Stock Assessment Database likely underestimates the actual proportion of stocks that are overfished globally, but it is unclear whether enough evidence would exist to trigger this prohibition for stocks not included in this database.&lt;/li&gt;&lt;li&gt;The proposal is ambiguous about which reference points might be used to make an overfished determination, and we therefore note that this is only one very narrow possible interpretation of this text.&lt;/li&gt;&lt;li&gt;The definition for an overfished stock subsidy prohibition considered here is the more ambitious interpretation considered in the previous version of the text (see OFOC - Negative effects (Option A)).&lt;/li&gt;&lt;/ol&gt;</t>
   </si>
   <si>
-    <t>&lt;ol&gt;&lt;li&gt;We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited.&lt;/li&gt;&lt;li&gt;We note that this is an ambitious interpretation of this proposal, no exemption is provided to demonstrate that measures are implemented to maintain stocks at a biologically sustainable level.&lt;/li&gt;&lt;/ol&gt;</t>
-  </si>
-  <si>
     <t>Subsidies granted by developing and LDC Members shall be allowed for fishing within their own territorial waters. As written, this exception might only apply with a transition period, but for the purposes of modeling we assume it to apply indefinitely.</t>
   </si>
   <si>
@@ -2005,10 +1996,36 @@
     <t>Need to identify developing countries meeting non-industrial criteria. The three options associated with defining it could be calculated on the back-end.</t>
   </si>
   <si>
-    <t xml:space="preserve">Added (May 25, 2021) - As compared to the old Chair's text, this does do something different for Overfished, but not for OFOC. NEW (May 13, 2021). I think we just pick an Overfished definition and our broadest definition of OFOC and simulate the 12nm exception Need guidance on which Chair's text to apply it to. </t>
-  </si>
-  <si>
     <t>Updated text (6/8/21). NEW + Added (May 25, 2021).</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;As written, this text would prohibit all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 unless a Member can demonstrate that measures are implemented to maintain stocks at a biologically sustainable level. It is unclear how many Members would be able to satisfy this sustainability criteria, and thus we assume that such an exemption could be aquired by all Members. We note that this is therefore a conservative interpretation of this text.&lt;/li&gt;&lt;li&gt;We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. 2019 are prohibited for all fishing (within Members' own EEZs, on the high seas, and in the EEZs of other coastal states). We note that this is an ambitious interpretation of this proposal as no exemption is provided to demonstrate that measures are implemented to maintain stocks at a biologically sustainable level.&lt;/li&gt;&lt;li&gt;The specific provisions related to high seas fishing and/or fishing in the EEZs of other coastal states are covered in the first assumption.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>Subsidies granted by LDCs shall be allowed, and subsidies granted by all other Members shall be allowed for fishing in their territorial seas. Subsidies granted by developing country Members for fishing in their EEZs and high seas will be allowed unless any of the following conditions are met for three consecutive years (2016-2018): a) GNI per capita is greater than US $5000 (constant 2010 US$), b) they engage in distant water fishing, or c) the contribution from Agriculture, Forestry and Fishing to their national GDP (World Bank) is greater than 10%.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Need to add conditional developing country S&amp;DT.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Added (May 25, 2021) - As compared to the old Chair's text, this does do something different for Overfished, but not for OFOC. NEW (May 13, 2021). I think we just pick an Overfished definition and our broadest definition of OFOC and simulate the 12nm exception Need guidance on which Chair's text to apply it to. </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3056,8 +3073,8 @@
   <dimension ref="A1:DB44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P14" sqref="P14"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
@@ -3422,7 +3439,7 @@
         <v>565</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>355</v>
@@ -3603,7 +3620,7 @@
         <v>509</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="E3" s="15" t="s">
         <v>330</v>
@@ -3695,7 +3712,7 @@
         <v>564</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>77</v>
@@ -3747,7 +3764,7 @@
         <v>454</v>
       </c>
       <c r="W4" s="34" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="X4" s="34" t="s">
         <v>433</v>
@@ -3768,10 +3785,10 @@
         <v>369</v>
       </c>
       <c r="CG4" s="15" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="CH4" s="15" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="CK4" s="15" t="s">
         <v>359</v>
@@ -4059,7 +4076,7 @@
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="42" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="F8" s="39" t="s">
         <v>504</v>
@@ -4110,10 +4127,10 @@
         <v>437</v>
       </c>
       <c r="V8" s="34" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="W8" s="34" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="X8" s="34" t="s">
         <v>55</v>
@@ -4131,7 +4148,7 @@
         <v>346</v>
       </c>
       <c r="BL8" s="15" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="BN8" s="15">
         <v>5</v>
@@ -4629,10 +4646,10 @@
         <v>98</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="D14" s="42" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="F14" s="15" t="s">
         <v>240</v>
@@ -4683,10 +4700,10 @@
         <v>437</v>
       </c>
       <c r="V14" s="34" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="W14" s="34" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="X14" s="34" t="s">
         <v>55</v>
@@ -4766,7 +4783,7 @@
         <v>389</v>
       </c>
       <c r="P15" s="40" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="Q15" s="4" t="s">
         <v>414</v>
@@ -4775,7 +4792,7 @@
         <v>445</v>
       </c>
       <c r="S15" s="34" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="T15" s="34" t="s">
         <v>454</v>
@@ -4985,7 +5002,7 @@
         <v>561</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="F19" s="39" t="s">
         <v>528</v>
@@ -5242,7 +5259,7 @@
         <v>437</v>
       </c>
       <c r="V22" s="34" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="W22" s="34" t="s">
         <v>439</v>
@@ -5411,10 +5428,10 @@
         <v>98</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="D24" s="42" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="E24" s="15" t="s">
         <v>231</v>
@@ -5465,7 +5482,7 @@
         <v>437</v>
       </c>
       <c r="V24" s="34" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="W24" s="34" t="s">
         <v>372</v>
@@ -5483,7 +5500,7 @@
         <v>64</v>
       </c>
       <c r="BK24" s="15" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="BR24" s="15" t="s">
         <v>295</v>
@@ -5723,7 +5740,7 @@
         <v>558</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="F26" s="14" t="s">
         <v>322</v>
@@ -5889,7 +5906,7 @@
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="14" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="G27" s="14" t="s">
         <v>354</v>
@@ -5907,13 +5924,13 @@
         <v>351</v>
       </c>
       <c r="L27" s="17" t="s">
+        <v>586</v>
+      </c>
+      <c r="M27" s="15" t="s">
         <v>587</v>
       </c>
-      <c r="M27" s="15" t="s">
+      <c r="N27" s="15" t="s">
         <v>588</v>
-      </c>
-      <c r="N27" s="15" t="s">
-        <v>589</v>
       </c>
       <c r="O27" s="15" t="s">
         <v>422</v>
@@ -5946,7 +5963,7 @@
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="14" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G28" s="14" t="s">
         <v>354</v>
@@ -5964,13 +5981,13 @@
         <v>351</v>
       </c>
       <c r="L28" s="17" t="s">
+        <v>586</v>
+      </c>
+      <c r="M28" s="15" t="s">
         <v>587</v>
       </c>
-      <c r="M28" s="15" t="s">
+      <c r="N28" s="15" t="s">
         <v>588</v>
-      </c>
-      <c r="N28" s="15" t="s">
-        <v>589</v>
       </c>
       <c r="O28" s="15" t="s">
         <v>555</v>
@@ -6105,7 +6122,7 @@
       </c>
       <c r="E29" s="19"/>
       <c r="F29" s="14" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G29" s="14" t="s">
         <v>354</v>
@@ -6123,13 +6140,13 @@
         <v>351</v>
       </c>
       <c r="L29" s="17" t="s">
+        <v>586</v>
+      </c>
+      <c r="M29" s="15" t="s">
         <v>587</v>
       </c>
-      <c r="M29" s="15" t="s">
+      <c r="N29" s="15" t="s">
         <v>588</v>
-      </c>
-      <c r="N29" s="15" t="s">
-        <v>589</v>
       </c>
       <c r="O29" s="15" t="s">
         <v>422</v>
@@ -6147,7 +6164,7 @@
         <v>456</v>
       </c>
       <c r="T29" s="34" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="U29" s="34" t="s">
         <v>458</v>
@@ -6264,7 +6281,7 @@
       </c>
       <c r="E30" s="19"/>
       <c r="F30" s="14" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="G30" s="14" t="s">
         <v>354</v>
@@ -6282,13 +6299,13 @@
         <v>351</v>
       </c>
       <c r="L30" s="17" t="s">
+        <v>586</v>
+      </c>
+      <c r="M30" s="15" t="s">
         <v>587</v>
       </c>
-      <c r="M30" s="15" t="s">
+      <c r="N30" s="15" t="s">
         <v>588</v>
-      </c>
-      <c r="N30" s="15" t="s">
-        <v>589</v>
       </c>
       <c r="O30" s="15" t="s">
         <v>422</v>
@@ -6441,7 +6458,7 @@
       </c>
       <c r="E31" s="19"/>
       <c r="F31" s="14" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G31" s="14" t="s">
         <v>354</v>
@@ -6459,13 +6476,13 @@
         <v>351</v>
       </c>
       <c r="L31" s="17" t="s">
+        <v>586</v>
+      </c>
+      <c r="M31" s="15" t="s">
         <v>587</v>
       </c>
-      <c r="M31" s="15" t="s">
+      <c r="N31" s="15" t="s">
         <v>588</v>
-      </c>
-      <c r="N31" s="15" t="s">
-        <v>589</v>
       </c>
       <c r="O31" s="15" t="s">
         <v>422</v>
@@ -6483,7 +6500,7 @@
         <v>456</v>
       </c>
       <c r="T31" s="34" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="U31" s="34" t="s">
         <v>458</v>
@@ -6618,7 +6635,7 @@
       </c>
       <c r="E32" s="19"/>
       <c r="F32" s="14" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="G32" s="14" t="s">
         <v>354</v>
@@ -6636,13 +6653,13 @@
         <v>351</v>
       </c>
       <c r="L32" s="17" t="s">
+        <v>586</v>
+      </c>
+      <c r="M32" s="15" t="s">
         <v>587</v>
       </c>
-      <c r="M32" s="15" t="s">
+      <c r="N32" s="15" t="s">
         <v>588</v>
-      </c>
-      <c r="N32" s="15" t="s">
-        <v>589</v>
       </c>
       <c r="O32" s="15" t="s">
         <v>422</v>
@@ -6774,7 +6791,7 @@
       </c>
       <c r="E33" s="19"/>
       <c r="F33" s="14" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="G33" s="14" t="s">
         <v>354</v>
@@ -6792,13 +6809,13 @@
         <v>351</v>
       </c>
       <c r="L33" s="17" t="s">
+        <v>586</v>
+      </c>
+      <c r="M33" s="15" t="s">
         <v>587</v>
       </c>
-      <c r="M33" s="15" t="s">
+      <c r="N33" s="15" t="s">
         <v>588</v>
-      </c>
-      <c r="N33" s="15" t="s">
-        <v>589</v>
       </c>
       <c r="O33" s="15" t="s">
         <v>422</v>
@@ -6816,7 +6833,7 @@
         <v>456</v>
       </c>
       <c r="T33" s="34" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="U33" s="34" t="s">
         <v>458</v>
@@ -6930,7 +6947,7 @@
       </c>
       <c r="E34" s="19"/>
       <c r="F34" s="14" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="G34" s="14" t="s">
         <v>354</v>
@@ -6948,13 +6965,13 @@
         <v>351</v>
       </c>
       <c r="L34" s="17" t="s">
+        <v>586</v>
+      </c>
+      <c r="M34" s="15" t="s">
         <v>587</v>
       </c>
-      <c r="M34" s="15" t="s">
+      <c r="N34" s="15" t="s">
         <v>588</v>
-      </c>
-      <c r="N34" s="15" t="s">
-        <v>589</v>
       </c>
       <c r="O34" s="15" t="s">
         <v>422</v>
@@ -7087,7 +7104,7 @@
       </c>
       <c r="E35" s="19"/>
       <c r="F35" s="14" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G35" s="14" t="s">
         <v>354</v>
@@ -7105,13 +7122,13 @@
         <v>351</v>
       </c>
       <c r="L35" s="17" t="s">
+        <v>586</v>
+      </c>
+      <c r="M35" s="15" t="s">
         <v>587</v>
       </c>
-      <c r="M35" s="15" t="s">
+      <c r="N35" s="15" t="s">
         <v>588</v>
-      </c>
-      <c r="N35" s="15" t="s">
-        <v>589</v>
       </c>
       <c r="O35" s="15" t="s">
         <v>422</v>
@@ -7129,7 +7146,7 @@
         <v>456</v>
       </c>
       <c r="T35" s="34" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="U35" s="34" t="s">
         <v>458</v>
@@ -7244,7 +7261,7 @@
       </c>
       <c r="E36" s="19"/>
       <c r="F36" s="14" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G36" s="14" t="s">
         <v>354</v>
@@ -7262,13 +7279,13 @@
         <v>351</v>
       </c>
       <c r="L36" s="17" t="s">
+        <v>586</v>
+      </c>
+      <c r="M36" s="15" t="s">
         <v>587</v>
       </c>
-      <c r="M36" s="15" t="s">
+      <c r="N36" s="15" t="s">
         <v>588</v>
-      </c>
-      <c r="N36" s="15" t="s">
-        <v>589</v>
       </c>
       <c r="O36" s="15" t="s">
         <v>422</v>
@@ -7382,7 +7399,7 @@
       </c>
       <c r="E37" s="19"/>
       <c r="F37" s="14" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G37" s="14" t="s">
         <v>354</v>
@@ -7400,13 +7417,13 @@
         <v>351</v>
       </c>
       <c r="L37" s="17" t="s">
+        <v>586</v>
+      </c>
+      <c r="M37" s="15" t="s">
         <v>587</v>
       </c>
-      <c r="M37" s="15" t="s">
+      <c r="N37" s="15" t="s">
         <v>588</v>
-      </c>
-      <c r="N37" s="15" t="s">
-        <v>589</v>
       </c>
       <c r="O37" s="15" t="s">
         <v>422</v>
@@ -7424,7 +7441,7 @@
         <v>456</v>
       </c>
       <c r="T37" s="34" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="U37" s="34" t="s">
         <v>458</v>
@@ -7513,7 +7530,7 @@
         <v>98</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E38" s="19"/>
       <c r="F38" s="8" t="s">
@@ -7603,10 +7620,10 @@
         <v>98</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D39" s="42" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E39" s="19"/>
       <c r="F39" s="8" t="s">
@@ -7643,7 +7660,7 @@
         <v>544</v>
       </c>
       <c r="Q39" s="25" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="R39" s="35" t="s">
         <v>454</v>
@@ -7696,7 +7713,7 @@
         <v>89</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D40" s="42" t="s">
         <v>547</v>
@@ -7754,10 +7771,10 @@
         <v>89</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D41" s="42" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>492</v>
@@ -7791,7 +7808,7 @@
         <v>498</v>
       </c>
       <c r="P41" s="10" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="Q41" s="11" t="s">
         <v>571</v>
@@ -7803,7 +7820,7 @@
         <v>456</v>
       </c>
       <c r="T41" s="34" t="s">
-        <v>529</v>
+        <v>549</v>
       </c>
       <c r="U41" s="34" t="s">
         <v>572</v>
@@ -7812,7 +7829,7 @@
         <v>459</v>
       </c>
       <c r="W41" s="34" t="s">
-        <v>573</v>
+        <v>637</v>
       </c>
       <c r="X41" s="34" t="s">
         <v>55</v>
@@ -7845,7 +7862,7 @@
         <v>288</v>
       </c>
       <c r="AO41" s="15" t="s">
-        <v>304</v>
+        <v>325</v>
       </c>
       <c r="AP41" s="8" t="s">
         <v>346</v>
@@ -7907,10 +7924,10 @@
         <v>89</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D42" s="42" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="E42" s="36"/>
       <c r="F42" s="8" t="s">
@@ -7941,37 +7958,37 @@
         <v>502</v>
       </c>
       <c r="O42" s="15" t="s">
+        <v>583</v>
+      </c>
+      <c r="P42" s="10" t="s">
         <v>584</v>
       </c>
-      <c r="P42" s="10" t="s">
-        <v>585</v>
-      </c>
       <c r="Q42" s="11" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="R42" s="34" t="s">
+        <v>581</v>
+      </c>
+      <c r="S42" s="34" t="s">
+        <v>612</v>
+      </c>
+      <c r="T42" s="34" t="s">
+        <v>604</v>
+      </c>
+      <c r="U42" s="34" t="s">
+        <v>610</v>
+      </c>
+      <c r="V42" s="34" t="s">
+        <v>635</v>
+      </c>
+      <c r="W42" s="34" t="s">
+        <v>611</v>
+      </c>
+      <c r="X42" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y42" s="15" t="s">
         <v>582</v>
-      </c>
-      <c r="S42" s="34" t="s">
-        <v>615</v>
-      </c>
-      <c r="T42" s="34" t="s">
-        <v>605</v>
-      </c>
-      <c r="U42" s="34" t="s">
-        <v>613</v>
-      </c>
-      <c r="V42" s="34" t="s">
-        <v>606</v>
-      </c>
-      <c r="W42" s="34" t="s">
-        <v>614</v>
-      </c>
-      <c r="X42" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y42" s="15" t="s">
-        <v>583</v>
       </c>
       <c r="Z42" s="15" t="s">
         <v>288</v>
@@ -8066,14 +8083,14 @@
         <v>89</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D43" s="42" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="E43" s="36"/>
       <c r="F43" s="8" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="G43" s="8" t="s">
         <v>499</v>
@@ -8091,40 +8108,40 @@
         <v>351</v>
       </c>
       <c r="L43" s="17" t="s">
+        <v>600</v>
+      </c>
+      <c r="M43" s="15" t="s">
         <v>601</v>
       </c>
-      <c r="M43" s="15" t="s">
+      <c r="P43" s="44" t="s">
+        <v>606</v>
+      </c>
+      <c r="Q43" s="4" t="s">
+        <v>607</v>
+      </c>
+      <c r="R43" s="34" t="s">
         <v>602</v>
-      </c>
-      <c r="P43" s="44" t="s">
-        <v>608</v>
-      </c>
-      <c r="Q43" s="4" t="s">
-        <v>609</v>
-      </c>
-      <c r="R43" s="34" t="s">
-        <v>603</v>
       </c>
       <c r="S43" s="34" t="s">
         <v>439</v>
       </c>
       <c r="T43" s="34" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="U43" s="34" t="s">
         <v>439</v>
       </c>
       <c r="V43" s="34" t="s">
-        <v>612</v>
+        <v>636</v>
       </c>
       <c r="W43" s="34" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="X43" s="34" t="s">
         <v>55</v>
       </c>
       <c r="Y43" s="15" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="Z43" s="15" t="s">
         <v>295</v>

</xml_diff>